<commit_message>
Made many files to debug comms between BW16 and Atmega.  Have serial communication now working with between the two.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="76">
   <si>
     <t>App use only</t>
   </si>
@@ -314,29 +314,6 @@
   </si>
   <si>
     <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>tbd</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>§</t>
     </r>
     <r>
@@ -400,12 +377,59 @@
   <si>
     <t>11:#,12:#,13:#.</t>
   </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>“GET/##.#.”</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,6 +632,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2577,8 +2608,8 @@
   </sheetPr>
   <dimension ref="A3:A34"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,17 +2631,17 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2661,7 +2692,7 @@
   </sheetPr>
   <dimension ref="A2:BC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
@@ -2825,7 +2856,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="79" t="s">
         <v>0</v>
@@ -2949,7 +2980,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="79" t="s">
         <v>0</v>
@@ -3073,7 +3104,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="79" t="s">
         <v>0</v>
@@ -3197,7 +3228,7 @@
         <v>33</v>
       </c>
       <c r="D6" s="78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="79" t="s">
         <v>0</v>
@@ -3321,7 +3352,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="78" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="79" t="s">
         <v>4</v>
@@ -3445,7 +3476,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="79" t="s">
         <v>7</v>
@@ -3569,7 +3600,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="79" t="s">
         <v>7</v>
@@ -3693,7 +3724,7 @@
         <v>33</v>
       </c>
       <c r="D10" s="78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="79" t="s">
         <v>7</v>
@@ -3817,7 +3848,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="79" t="s">
         <v>4</v>
@@ -3941,7 +3972,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" s="79" t="s">
         <v>4</v>
@@ -4065,7 +4096,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="79"/>
       <c r="F13" s="80" t="str">
@@ -4187,7 +4218,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="79" t="s">
         <v>4</v>
@@ -4311,7 +4342,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="79" t="s">
         <v>7</v>
@@ -7629,7 +7660,7 @@
     </row>
     <row r="54" spans="6:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>AC44</f>

</xml_diff>

<commit_message>
temporarily assigned inky to test play Mr. Pacman.  Made other changes I want saved.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="82">
   <si>
     <t>App use only</t>
   </si>
@@ -311,6 +311,56 @@
   </si>
   <si>
     <t>If ESP8266 fails to connect to local network, it will establish its own network…</t>
+  </si>
+  <si>
+    <t>Motion Enable</t>
+  </si>
+  <si>
+    <t>Sound Enable</t>
+  </si>
+  <si>
+    <t>Performance number</t>
+  </si>
+  <si>
+    <t>Light Enable</t>
+  </si>
+  <si>
+    <t>Clock Enable</t>
+  </si>
+  <si>
+    <t>Light Pinky</t>
+  </si>
+  <si>
+    <t>Light Clyde</t>
+  </si>
+  <si>
+    <t>Light Cherry</t>
+  </si>
+  <si>
+    <t>Light PacMan</t>
+  </si>
+  <si>
+    <t>Light Blinky</t>
+  </si>
+  <si>
+    <t>Light Inky</t>
+  </si>
+  <si>
+    <t>11:#,12:#,13:#.</t>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>    ZPMZ</t>
+    </r>
   </si>
   <si>
     <r>
@@ -332,104 +382,42 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>“cmd:M” a</t>
+      <t>“ZPMZ21:0x,”</t>
     </r>
   </si>
   <si>
-    <t>Motion Enable</t>
-  </si>
-  <si>
-    <t>Everything Enable</t>
-  </si>
-  <si>
-    <t>Sound Enable</t>
-  </si>
-  <si>
-    <t>Performance number</t>
-  </si>
-  <si>
-    <t>Light Enable</t>
-  </si>
-  <si>
-    <t>Clock Enable</t>
-  </si>
-  <si>
-    <t>Room Light Sensor Trigger Value</t>
-  </si>
-  <si>
-    <t>Light Pinky</t>
-  </si>
-  <si>
-    <t>Light Clyde</t>
-  </si>
-  <si>
-    <t>Light Cherry</t>
-  </si>
-  <si>
-    <t>Light PacMan</t>
-  </si>
-  <si>
-    <t>Light Blinky</t>
-  </si>
-  <si>
-    <t>Light Inky</t>
-  </si>
-  <si>
-    <t>11:#,12:#,13:#.</t>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>GET</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>§</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>“GET/##.#.”</t>
-    </r>
+    <t>Night Light Enable</t>
+  </si>
+  <si>
+    <t>Location (SF=1, Brkgs=2) (ip address)</t>
+  </si>
+  <si>
+    <t>######</t>
+  </si>
+  <si>
+    <t>Alarm Time</t>
+  </si>
+  <si>
+    <t>Alarm Date</t>
+  </si>
+  <si>
+    <t>Master Enable</t>
+  </si>
+  <si>
+    <t>Light Sensor Enable</t>
+  </si>
+  <si>
+    <t>Light Sensor trigger value</t>
+  </si>
+  <si>
+    <t>Alarm Enable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,13 +621,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -803,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -936,9 +917,6 @@
     <xf numFmtId="0" fontId="24" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2608,7 +2586,7 @@
   </sheetPr>
   <dimension ref="A3:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -2631,18 +2609,16 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2692,8 +2668,8 @@
   </sheetPr>
   <dimension ref="A2:BC63"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2845,53 +2821,53 @@
       <c r="BB2" s="51"/>
       <c r="BC2" s="51"/>
     </row>
-    <row r="3" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76">
+    <row r="3" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75">
         <v>1</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="75">
         <v>11</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="79" t="s">
+      <c r="D3" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="80" t="str">
+      <c r="F3" s="79" t="str">
         <f t="shared" ref="F3:F6" si="12">CONCATENATE($B3,":",$C3,",")</f>
         <v>11:#,</v>
       </c>
-      <c r="G3" s="81" t="str">
+      <c r="G3" s="80" t="str">
         <f t="shared" ref="G3:G6" si="13">CONCATENATE($F3,$D3,",")</f>
-        <v>11:#,Everything Enable,</v>
-      </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82" t="s">
+        <v>11:#,Master Enable,</v>
+      </c>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="82" t="str">
+      <c r="K3" s="81" t="str">
         <f t="shared" ref="K3:K6" si="14">CONCATENATE($B3,":",$C3,",")</f>
         <v>11:#,</v>
       </c>
-      <c r="L3" s="82" t="str">
+      <c r="L3" s="81" t="str">
         <f t="shared" ref="L3:L6" si="15">CONCATENATE($K3,$D3,",")</f>
-        <v>11:#,Everything Enable,</v>
-      </c>
-      <c r="M3" s="83"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="83" t="s">
+        <v>11:#,Master Enable,</v>
+      </c>
+      <c r="M3" s="82"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="86"/>
-      <c r="T3" s="85" t="s">
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X3" s="59" t="str">
@@ -2900,7 +2876,7 @@
       </c>
       <c r="Y3" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,</v>
+        <v>11:#,Master Enable,</v>
       </c>
       <c r="Z3" s="60" t="str">
         <f t="shared" si="2"/>
@@ -2919,7 +2895,7 @@
       </c>
       <c r="AD3" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,</v>
+        <v>11:#,Master Enable,</v>
       </c>
       <c r="AE3" s="61" t="str">
         <f t="shared" si="6"/>
@@ -2969,53 +2945,53 @@
       <c r="BB3" s="51"/>
       <c r="BC3" s="51"/>
     </row>
-    <row r="4" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76">
+    <row r="4" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75">
         <v>2</v>
       </c>
-      <c r="B4" s="76">
+      <c r="B4" s="75">
         <v>12</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="79" t="s">
+      <c r="E4" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="80" t="str">
+      <c r="F4" s="79" t="str">
         <f t="shared" si="12"/>
         <v>12:#,</v>
       </c>
-      <c r="G4" s="81" t="str">
+      <c r="G4" s="80" t="str">
         <f t="shared" si="13"/>
-        <v>12:#,Sound Enable,</v>
-      </c>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82" t="s">
+        <v>12:#,Light Enable,</v>
+      </c>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="82" t="str">
+      <c r="K4" s="81" t="str">
         <f t="shared" si="14"/>
         <v>12:#,</v>
       </c>
-      <c r="L4" s="82" t="str">
+      <c r="L4" s="81" t="str">
         <f t="shared" si="15"/>
-        <v>12:#,Sound Enable,</v>
-      </c>
-      <c r="M4" s="83"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="83" t="s">
+        <v>12:#,Light Enable,</v>
+      </c>
+      <c r="M4" s="82"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="85" t="s">
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X4" s="59" t="str">
@@ -3024,7 +3000,7 @@
       </c>
       <c r="Y4" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,</v>
       </c>
       <c r="Z4" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3043,7 +3019,7 @@
       </c>
       <c r="AD4" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,</v>
       </c>
       <c r="AE4" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3093,53 +3069,53 @@
       <c r="BB4" s="51"/>
       <c r="BC4" s="51"/>
     </row>
-    <row r="5" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76">
+    <row r="5" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="75">
         <v>3</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="75">
         <v>13</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="79" t="s">
+      <c r="D5" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="80" t="str">
+      <c r="F5" s="79" t="str">
         <f t="shared" si="12"/>
         <v>13:#,</v>
       </c>
-      <c r="G5" s="81" t="str">
+      <c r="G5" s="80" t="str">
         <f t="shared" si="13"/>
-        <v>13:#,Light Enable,</v>
-      </c>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82" t="s">
+        <v>13:#,Sound Enable,</v>
+      </c>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="82" t="str">
+      <c r="K5" s="81" t="str">
         <f t="shared" si="14"/>
         <v>13:#,</v>
       </c>
-      <c r="L5" s="82" t="str">
+      <c r="L5" s="81" t="str">
         <f t="shared" si="15"/>
-        <v>13:#,Light Enable,</v>
-      </c>
-      <c r="M5" s="83"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="83" t="s">
+        <v>13:#,Sound Enable,</v>
+      </c>
+      <c r="M5" s="82"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="85" t="s">
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X5" s="59" t="str">
@@ -3148,7 +3124,7 @@
       </c>
       <c r="Y5" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,</v>
       </c>
       <c r="Z5" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3167,7 +3143,7 @@
       </c>
       <c r="AD5" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,</v>
       </c>
       <c r="AE5" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3217,53 +3193,53 @@
       <c r="BB5" s="51"/>
       <c r="BC5" s="51"/>
     </row>
-    <row r="6" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76">
+    <row r="6" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
         <v>4</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="75">
         <v>14</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="79" t="s">
+      <c r="D6" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="80" t="str">
+      <c r="F6" s="79" t="str">
         <f t="shared" si="12"/>
         <v>14:#,</v>
       </c>
-      <c r="G6" s="81" t="str">
+      <c r="G6" s="80" t="str">
         <f t="shared" si="13"/>
         <v>14:#,Motion Enable,</v>
       </c>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82" t="s">
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="82" t="str">
+      <c r="K6" s="81" t="str">
         <f t="shared" si="14"/>
         <v>14:#,</v>
       </c>
-      <c r="L6" s="82" t="str">
+      <c r="L6" s="81" t="str">
         <f t="shared" si="15"/>
         <v>14:#,Motion Enable,</v>
       </c>
-      <c r="M6" s="83"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="83" t="s">
+      <c r="M6" s="82"/>
+      <c r="N6" s="83"/>
+      <c r="O6" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="85"/>
-      <c r="S6" s="86"/>
-      <c r="T6" s="85" t="s">
+      <c r="P6" s="83"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="84"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X6" s="59" t="str">
@@ -3272,7 +3248,7 @@
       </c>
       <c r="Y6" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,</v>
       </c>
       <c r="Z6" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3291,7 +3267,7 @@
       </c>
       <c r="AD6" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,</v>
       </c>
       <c r="AE6" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3341,53 +3317,53 @@
       <c r="BB6" s="51"/>
       <c r="BC6" s="51"/>
     </row>
-    <row r="7" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="76">
+    <row r="7" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="75">
         <v>5</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="75">
         <v>15</v>
       </c>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="79" t="s">
+      <c r="D7" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="80" t="str">
+      <c r="F7" s="79" t="str">
         <f t="shared" ref="F7" si="16">CONCATENATE($B7,":",$C7,",")</f>
         <v>15:#,</v>
       </c>
-      <c r="G7" s="81" t="str">
+      <c r="G7" s="80" t="str">
         <f>CONCATENATE($F7,$D7,",")</f>
         <v>15:#,Clock Enable,</v>
       </c>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82" t="s">
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="82" t="str">
+      <c r="K7" s="81" t="str">
         <f t="shared" ref="K7:K11" si="17">CONCATENATE($B7,":",$C7,",")</f>
         <v>15:#,</v>
       </c>
-      <c r="L7" s="82" t="str">
+      <c r="L7" s="81" t="str">
         <f>CONCATENATE($K7,$D7,",")</f>
         <v>15:#,Clock Enable,</v>
       </c>
-      <c r="M7" s="83"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="83" t="s">
+      <c r="M7" s="82"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="85"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="85" t="s">
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="84"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X7" s="59" t="str">
@@ -3396,7 +3372,7 @@
       </c>
       <c r="Y7" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,</v>
       </c>
       <c r="Z7" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3415,7 +3391,7 @@
       </c>
       <c r="AD7" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,</v>
       </c>
       <c r="AE7" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3465,62 +3441,62 @@
       <c r="BB7" s="51"/>
       <c r="BC7" s="51"/>
     </row>
-    <row r="8" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76">
+    <row r="8" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="75">
         <v>6</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="75">
         <v>16</v>
       </c>
-      <c r="C8" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="79" t="s">
+      <c r="C8" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="80" t="str">
+      <c r="F8" s="79" t="str">
         <f>CONCATENATE($B8,":",$C8,",")</f>
-        <v>16:####,</v>
-      </c>
-      <c r="G8" s="81" t="str">
-        <f>CONCATENATE($F8,$D8,",")</f>
-        <v>16:####,Room Light Sensor Trigger Value,</v>
-      </c>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82" t="s">
+        <v>16:#,</v>
+      </c>
+      <c r="G8" s="80" t="str">
+        <f>CONCATENATE($F8,$D20,",")</f>
+        <v>16:#,Alarm Time,</v>
+      </c>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="82" t="str">
+      <c r="K8" s="81" t="str">
         <f t="shared" si="17"/>
-        <v>16:####,</v>
-      </c>
-      <c r="L8" s="82" t="str">
-        <f t="shared" ref="L8:L11" si="18">CONCATENATE($K8,$D8,",")</f>
-        <v>16:####,Room Light Sensor Trigger Value,</v>
-      </c>
-      <c r="M8" s="83"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="83" t="s">
+        <v>16:#,</v>
+      </c>
+      <c r="L8" s="81" t="str">
+        <f>CONCATENATE($K8,$D20,",")</f>
+        <v>16:#,Alarm Time,</v>
+      </c>
+      <c r="M8" s="82"/>
+      <c r="N8" s="83"/>
+      <c r="O8" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="84"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="86"/>
-      <c r="T8" s="85" t="s">
+      <c r="P8" s="83"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="84"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X8" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,</v>
       </c>
       <c r="Y8" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,</v>
       </c>
       <c r="Z8" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3535,11 +3511,11 @@
       </c>
       <c r="AC8" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,</v>
       </c>
       <c r="AD8" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,</v>
       </c>
       <c r="AE8" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3589,62 +3565,62 @@
       <c r="BB8" s="51"/>
       <c r="BC8" s="51"/>
     </row>
-    <row r="9" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76">
+    <row r="9" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="75">
         <v>7</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="75">
         <v>17</v>
       </c>
-      <c r="C9" s="77" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="79" t="s">
+      <c r="C9" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="80" t="str">
+      <c r="F9" s="79" t="str">
         <f>CONCATENATE($B9,":",$C9,",")</f>
-        <v>17:##,</v>
-      </c>
-      <c r="G9" s="81" t="str">
-        <f>CONCATENATE($F9,$D9,",")</f>
-        <v>17:##,Performance number,</v>
-      </c>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82" t="s">
+        <v>17:#,</v>
+      </c>
+      <c r="G9" s="80" t="str">
+        <f>CONCATENATE($F9,$D21,",")</f>
+        <v>17:#,Performance number,</v>
+      </c>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="82" t="str">
+      <c r="K9" s="81" t="str">
         <f t="shared" si="17"/>
-        <v>17:##,</v>
-      </c>
-      <c r="L9" s="82" t="str">
-        <f t="shared" si="18"/>
-        <v>17:##,Performance number,</v>
-      </c>
-      <c r="M9" s="83"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="83" t="s">
+        <v>17:#,</v>
+      </c>
+      <c r="L9" s="81" t="str">
+        <f>CONCATENATE($K9,$D21,",")</f>
+        <v>17:#,Performance number,</v>
+      </c>
+      <c r="M9" s="82"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="84"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="85" t="s">
+      <c r="P9" s="83"/>
+      <c r="Q9" s="83"/>
+      <c r="R9" s="84"/>
+      <c r="S9" s="85"/>
+      <c r="T9" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X9" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,</v>
       </c>
       <c r="Y9" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,</v>
       </c>
       <c r="Z9" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3659,11 +3635,11 @@
       </c>
       <c r="AC9" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,</v>
       </c>
       <c r="AD9" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,</v>
       </c>
       <c r="AE9" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3713,62 +3689,62 @@
       <c r="BB9" s="51"/>
       <c r="BC9" s="51"/>
     </row>
-    <row r="10" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="76">
+    <row r="10" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="75">
         <v>8</v>
       </c>
-      <c r="B10" s="76">
+      <c r="B10" s="75">
         <v>18</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="79" t="s">
+      <c r="D10" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="80" t="str">
+      <c r="F10" s="79" t="str">
         <f>CONCATENATE($B10,":",$C10,",")</f>
         <v>18:#,</v>
       </c>
-      <c r="G10" s="81" t="str">
+      <c r="G10" s="80" t="str">
         <f>CONCATENATE($F10,$D10,",")</f>
-        <v>18:#,Light Pinky,</v>
-      </c>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82" t="s">
+        <v>18:#,Light Cherry,</v>
+      </c>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="82" t="str">
+      <c r="K10" s="81" t="str">
         <f t="shared" si="17"/>
         <v>18:#,</v>
       </c>
-      <c r="L10" s="82" t="str">
-        <f t="shared" si="18"/>
-        <v>18:#,Light Pinky,</v>
-      </c>
-      <c r="M10" s="83"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="83" t="s">
+      <c r="L10" s="81" t="str">
+        <f t="shared" ref="L10:L11" si="18">CONCATENATE($K10,$D10,",")</f>
+        <v>18:#,Light Cherry,</v>
+      </c>
+      <c r="M10" s="82"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="84"/>
-      <c r="R10" s="85"/>
-      <c r="S10" s="86"/>
-      <c r="T10" s="85" t="s">
+      <c r="P10" s="83"/>
+      <c r="Q10" s="83"/>
+      <c r="R10" s="84"/>
+      <c r="S10" s="85"/>
+      <c r="T10" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X10" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,</v>
       </c>
       <c r="Y10" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,</v>
       </c>
       <c r="Z10" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3783,11 +3759,11 @@
       </c>
       <c r="AC10" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,</v>
       </c>
       <c r="AD10" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,</v>
       </c>
       <c r="AE10" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3837,62 +3813,62 @@
       <c r="BB10" s="51"/>
       <c r="BC10" s="51"/>
     </row>
-    <row r="11" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="76">
+    <row r="11" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="75">
         <v>9</v>
       </c>
-      <c r="B11" s="76">
+      <c r="B11" s="75">
         <v>19</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="79" t="s">
+      <c r="D11" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="80" t="str">
-        <f t="shared" ref="F11:F20" si="19">CONCATENATE($B11,":",$C11,",")</f>
+      <c r="F11" s="79" t="str">
+        <f t="shared" ref="F11:F21" si="19">CONCATENATE($B11,":",$C11,",")</f>
         <v>19:#,</v>
       </c>
-      <c r="G11" s="81" t="str">
+      <c r="G11" s="80" t="str">
         <f t="shared" ref="G11:G24" si="20">CONCATENATE($F11,$D11,",")</f>
-        <v>19:#,Light Clyde,</v>
-      </c>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82" t="s">
+        <v>19:#,Light PacMan,</v>
+      </c>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="82" t="str">
+      <c r="K11" s="81" t="str">
         <f t="shared" si="17"/>
         <v>19:#,</v>
       </c>
-      <c r="L11" s="82" t="str">
+      <c r="L11" s="81" t="str">
         <f t="shared" si="18"/>
-        <v>19:#,Light Clyde,</v>
-      </c>
-      <c r="M11" s="83"/>
-      <c r="N11" s="84"/>
-      <c r="O11" s="83" t="s">
+        <v>19:#,Light PacMan,</v>
+      </c>
+      <c r="M11" s="82"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P11" s="84"/>
-      <c r="Q11" s="84"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="85" t="s">
+      <c r="P11" s="83"/>
+      <c r="Q11" s="83"/>
+      <c r="R11" s="84"/>
+      <c r="S11" s="85"/>
+      <c r="T11" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X11" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,</v>
       </c>
       <c r="Y11" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,</v>
       </c>
       <c r="Z11" s="60" t="str">
         <f t="shared" si="2"/>
@@ -3907,11 +3883,11 @@
       </c>
       <c r="AC11" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,</v>
       </c>
       <c r="AD11" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,</v>
       </c>
       <c r="AE11" s="61" t="str">
         <f t="shared" si="6"/>
@@ -3961,62 +3937,62 @@
       <c r="BB11" s="51"/>
       <c r="BC11" s="51"/>
     </row>
-    <row r="12" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="76">
+    <row r="12" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="75">
         <v>10</v>
       </c>
-      <c r="B12" s="76">
+      <c r="B12" s="75">
         <v>20</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="79" t="s">
+      <c r="D12" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="80" t="str">
+      <c r="F12" s="79" t="str">
         <f t="shared" si="19"/>
         <v>20:#,</v>
       </c>
-      <c r="G12" s="81" t="str">
+      <c r="G12" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>20:#,Light Cherry,</v>
-      </c>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82" t="s">
+        <v>20:#,Light Blinky,</v>
+      </c>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="82" t="str">
-        <f t="shared" ref="K12:K18" si="21">CONCATENATE($B12,":",$C12,",")</f>
+      <c r="K12" s="81" t="str">
+        <f t="shared" ref="K12:K21" si="21">CONCATENATE($B12,":",$C12,",")</f>
         <v>20:#,</v>
       </c>
-      <c r="L12" s="82" t="str">
-        <f t="shared" ref="L12:L18" si="22">CONCATENATE($K12,$D12,",")</f>
-        <v>20:#,Light Cherry,</v>
-      </c>
-      <c r="M12" s="83"/>
-      <c r="N12" s="84"/>
-      <c r="O12" s="83" t="s">
+      <c r="L12" s="81" t="str">
+        <f t="shared" ref="L12:L21" si="22">CONCATENATE($K12,$D12,",")</f>
+        <v>20:#,Light Blinky,</v>
+      </c>
+      <c r="M12" s="82"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P12" s="84"/>
-      <c r="Q12" s="84"/>
-      <c r="R12" s="85"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="85" t="s">
+      <c r="P12" s="83"/>
+      <c r="Q12" s="83"/>
+      <c r="R12" s="84"/>
+      <c r="S12" s="85"/>
+      <c r="T12" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X12" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,</v>
       </c>
       <c r="Y12" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,</v>
       </c>
       <c r="Z12" s="60" t="str">
         <f t="shared" si="2"/>
@@ -4031,11 +4007,11 @@
       </c>
       <c r="AC12" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,</v>
       </c>
       <c r="AD12" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,</v>
       </c>
       <c r="AE12" s="61" t="str">
         <f t="shared" si="6"/>
@@ -4085,60 +4061,60 @@
       <c r="BB12" s="51"/>
       <c r="BC12" s="51"/>
     </row>
-    <row r="13" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="76">
+    <row r="13" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="75">
         <v>11</v>
       </c>
-      <c r="B13" s="76">
+      <c r="B13" s="75">
         <v>21</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="79"/>
-      <c r="F13" s="80" t="str">
+      <c r="D13" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79" t="str">
         <f t="shared" si="19"/>
         <v>21:#,</v>
       </c>
-      <c r="G13" s="81" t="str">
+      <c r="G13" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>21:#,Light PacMan,</v>
-      </c>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82" t="s">
+        <v>21:#,Light Inky,</v>
+      </c>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="82" t="str">
+      <c r="K13" s="81" t="str">
         <f t="shared" si="21"/>
         <v>21:#,</v>
       </c>
-      <c r="L13" s="82" t="str">
+      <c r="L13" s="81" t="str">
         <f t="shared" si="22"/>
-        <v>21:#,Light PacMan,</v>
-      </c>
-      <c r="M13" s="83"/>
-      <c r="N13" s="84"/>
-      <c r="O13" s="83" t="s">
+        <v>21:#,Light Inky,</v>
+      </c>
+      <c r="M13" s="82"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P13" s="84"/>
-      <c r="Q13" s="84"/>
-      <c r="R13" s="85"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="85" t="s">
+      <c r="P13" s="83"/>
+      <c r="Q13" s="83"/>
+      <c r="R13" s="84"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X13" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,</v>
       </c>
       <c r="Y13" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,</v>
       </c>
       <c r="Z13" s="60" t="str">
         <f t="shared" si="2"/>
@@ -4153,11 +4129,11 @@
       </c>
       <c r="AC13" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,</v>
       </c>
       <c r="AD13" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,</v>
       </c>
       <c r="AE13" s="61" t="str">
         <f t="shared" si="6"/>
@@ -4207,62 +4183,62 @@
       <c r="BB13" s="51"/>
       <c r="BC13" s="51"/>
     </row>
-    <row r="14" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="76">
+    <row r="14" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="75">
         <v>12</v>
       </c>
-      <c r="B14" s="76">
+      <c r="B14" s="75">
         <v>22</v>
       </c>
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="79" t="s">
+      <c r="D14" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="80" t="str">
+      <c r="F14" s="79" t="str">
         <f t="shared" si="19"/>
         <v>22:#,</v>
       </c>
-      <c r="G14" s="81" t="str">
+      <c r="G14" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>22:#,Light Blinky,</v>
-      </c>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82" t="s">
+        <v>22:#,Light Sensor Enable,</v>
+      </c>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="82" t="str">
+      <c r="K14" s="81" t="str">
         <f t="shared" si="21"/>
         <v>22:#,</v>
       </c>
-      <c r="L14" s="82" t="str">
+      <c r="L14" s="81" t="str">
         <f t="shared" si="22"/>
-        <v>22:#,Light Blinky,</v>
-      </c>
-      <c r="M14" s="83"/>
-      <c r="N14" s="84"/>
-      <c r="O14" s="83" t="s">
+        <v>22:#,Light Sensor Enable,</v>
+      </c>
+      <c r="M14" s="82"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="84"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="86"/>
-      <c r="T14" s="85" t="s">
+      <c r="P14" s="83"/>
+      <c r="Q14" s="83"/>
+      <c r="R14" s="84"/>
+      <c r="S14" s="85"/>
+      <c r="T14" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X14" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,</v>
       </c>
       <c r="Y14" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,</v>
       </c>
       <c r="Z14" s="60" t="str">
         <f t="shared" si="2"/>
@@ -4277,11 +4253,11 @@
       </c>
       <c r="AC14" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,</v>
       </c>
       <c r="AD14" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,</v>
       </c>
       <c r="AE14" s="61" t="str">
         <f t="shared" si="6"/>
@@ -4331,68 +4307,68 @@
       <c r="BB14" s="51"/>
       <c r="BC14" s="51"/>
     </row>
-    <row r="15" spans="1:55" s="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="76">
+    <row r="15" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="75">
         <v>13</v>
       </c>
-      <c r="B15" s="76">
+      <c r="B15" s="75">
         <v>23</v>
       </c>
-      <c r="C15" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="79" t="s">
+      <c r="C15" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="80" t="str">
+      <c r="F15" s="79" t="str">
         <f t="shared" si="19"/>
-        <v>23:#,</v>
-      </c>
-      <c r="G15" s="81" t="str">
+        <v>23:####,</v>
+      </c>
+      <c r="G15" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>23:#,Light Inky,</v>
-      </c>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82" t="s">
+        <v>23:####,Light Sensor trigger value,</v>
+      </c>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="82" t="str">
+      <c r="K15" s="81" t="str">
         <f t="shared" si="21"/>
-        <v>23:#,</v>
-      </c>
-      <c r="L15" s="82" t="str">
+        <v>23:####,</v>
+      </c>
+      <c r="L15" s="81" t="str">
         <f t="shared" si="22"/>
-        <v>23:#,Light Inky,</v>
-      </c>
-      <c r="M15" s="83"/>
-      <c r="N15" s="84"/>
-      <c r="O15" s="83" t="s">
+        <v>23:####,Light Sensor trigger value,</v>
+      </c>
+      <c r="M15" s="82"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="P15" s="84" t="str">
+      <c r="P15" s="83" t="str">
         <f>CONCATENATE(B15,":",C15,",")</f>
-        <v>23:#,</v>
-      </c>
-      <c r="Q15" s="84" t="str">
+        <v>23:####,</v>
+      </c>
+      <c r="Q15" s="83" t="str">
         <f>CONCATENATE($P15,$D15,",")</f>
-        <v>23:#,Light Inky,</v>
-      </c>
-      <c r="R15" s="85"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="85" t="s">
+        <v>23:####,Light Sensor trigger value,</v>
+      </c>
+      <c r="R15" s="84"/>
+      <c r="S15" s="85"/>
+      <c r="T15" s="84" t="s">
         <v>2</v>
       </c>
       <c r="X15" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,</v>
       </c>
       <c r="Y15" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,</v>
       </c>
       <c r="Z15" s="60" t="str">
         <f t="shared" si="2"/>
@@ -4407,11 +4383,11 @@
       </c>
       <c r="AC15" s="60" t="str">
         <f t="shared" si="4"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,</v>
       </c>
       <c r="AD15" s="60" t="str">
         <f t="shared" si="5"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,</v>
       </c>
       <c r="AE15" s="61" t="str">
         <f t="shared" si="6"/>
@@ -4426,11 +4402,11 @@
       </c>
       <c r="AH15" s="61" t="str">
         <f t="shared" si="8"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,</v>
       </c>
       <c r="AI15" s="61" t="str">
         <f t="shared" si="9"/>
-        <v>23:#,Light Inky,</v>
+        <v>23:####,Light Sensor trigger value,</v>
       </c>
       <c r="AJ15" s="51" t="str">
         <f t="shared" si="10"/>
@@ -4461,64 +4437,68 @@
       <c r="BB15" s="51"/>
       <c r="BC15" s="51"/>
     </row>
-    <row r="16" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51">
+    <row r="16" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="75">
         <v>14</v>
       </c>
-      <c r="B16" s="51">
+      <c r="B16" s="75">
         <v>24</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="62" t="s">
+      <c r="C16" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="53" t="str">
+      <c r="F16" s="79" t="str">
         <f t="shared" si="19"/>
-        <v>24:,</v>
-      </c>
-      <c r="G16" s="63" t="str">
+        <v>24:#,</v>
+      </c>
+      <c r="G16" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>24:,,</v>
-      </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54" t="s">
+        <v>24:#,Night Light Enable,</v>
+      </c>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="54" t="str">
+      <c r="K16" s="81" t="str">
         <f t="shared" si="21"/>
-        <v>24:,</v>
-      </c>
-      <c r="L16" s="54" t="str">
+        <v>24:#,</v>
+      </c>
+      <c r="L16" s="81" t="str">
         <f t="shared" si="22"/>
-        <v>24:,,</v>
-      </c>
-      <c r="M16" s="55"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="55" t="s">
+        <v>24:#,Night Light Enable,</v>
+      </c>
+      <c r="M16" s="82"/>
+      <c r="N16" s="83"/>
+      <c r="O16" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="56" t="str">
-        <f t="shared" ref="P16:P18" si="23">CONCATENATE(B16,":",C16,",")</f>
-        <v>24:,</v>
-      </c>
-      <c r="Q16" s="56" t="str">
+      <c r="P16" s="83" t="str">
+        <f t="shared" ref="P16:P19" si="23">CONCATENATE(B16,":",C16,",")</f>
+        <v>24:#,</v>
+      </c>
+      <c r="Q16" s="83" t="str">
         <f>CONCATENATE($P16,$D16,",")</f>
-        <v>24:,,</v>
-      </c>
-      <c r="R16" s="57"/>
-      <c r="S16" s="58"/>
-      <c r="T16" s="57" t="s">
+        <v>24:#,Night Light Enable,</v>
+      </c>
+      <c r="R16" s="84"/>
+      <c r="S16" s="85"/>
+      <c r="T16" s="84" t="s">
         <v>2</v>
       </c>
       <c r="X16" s="59" t="str">
         <f t="shared" ref="X16:X18" si="24">CONCATENATE(X15,F16)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,</v>
       </c>
       <c r="Y16" s="59" t="str">
         <f t="shared" ref="Y16:Y25" si="25">CONCATENATE(Y15,G16)</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,</v>
       </c>
       <c r="Z16" s="60" t="str">
         <f t="shared" ref="Z16:Z44" si="26">CONCATENATE(Z15,H16)</f>
@@ -4533,11 +4513,11 @@
       </c>
       <c r="AC16" s="60" t="str">
         <f t="shared" ref="AC16:AC44" si="28">CONCATENATE(AC15,K16)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,</v>
       </c>
       <c r="AD16" s="60" t="str">
         <f t="shared" ref="AD16:AD44" si="29">CONCATENATE(AD15,L16)</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,</v>
       </c>
       <c r="AE16" s="61" t="str">
         <f t="shared" ref="AE16:AE44" si="30">CONCATENATE(AE15,M16)</f>
@@ -4552,11 +4532,11 @@
       </c>
       <c r="AH16" s="61" t="str">
         <f t="shared" ref="AH16:AH44" si="32">CONCATENATE(AH15,P16)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,</v>
       </c>
       <c r="AI16" s="61" t="str">
         <f t="shared" ref="AI16:AI44" si="33">CONCATENATE(AI15,Q16)</f>
-        <v>23:#,Light Inky,24:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,</v>
       </c>
       <c r="AJ16" s="51" t="str">
         <f t="shared" ref="AJ16:AJ44" si="34">CONCATENATE(AJ15,R16)</f>
@@ -4569,65 +4549,86 @@
       <c r="AL16" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM16" s="51"/>
+      <c r="AN16" s="51"/>
+      <c r="AO16" s="51"/>
+      <c r="AP16" s="51"/>
+      <c r="AQ16" s="51"/>
+      <c r="AR16" s="51"/>
+      <c r="AS16" s="51"/>
+      <c r="AT16" s="51"/>
+      <c r="AU16" s="51"/>
+      <c r="AV16" s="51"/>
+      <c r="AW16" s="51"/>
+      <c r="AX16" s="51"/>
+      <c r="AY16" s="51"/>
+      <c r="AZ16" s="51"/>
+      <c r="BA16" s="51"/>
+      <c r="BB16" s="51"/>
+      <c r="BC16" s="51"/>
     </row>
-    <row r="17" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51">
+    <row r="17" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="75">
         <v>15</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="75">
         <v>25</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="62" t="s">
+      <c r="C17" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="53" t="str">
+      <c r="F17" s="79" t="str">
         <f t="shared" si="19"/>
-        <v>25:,</v>
-      </c>
-      <c r="G17" s="63" t="str">
+        <v>25:#,</v>
+      </c>
+      <c r="G17" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>25:,,</v>
-      </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54" t="s">
+        <v>25:#,Location (SF=1, Brkgs=2) (ip address),</v>
+      </c>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="54" t="str">
+      <c r="K17" s="81" t="str">
         <f t="shared" si="21"/>
-        <v>25:,</v>
-      </c>
-      <c r="L17" s="64" t="str">
+        <v>25:#,</v>
+      </c>
+      <c r="L17" s="81" t="str">
         <f t="shared" si="22"/>
-        <v>25:,,</v>
-      </c>
-      <c r="M17" s="55"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="55" t="s">
+        <v>25:#,Location (SF=1, Brkgs=2) (ip address),</v>
+      </c>
+      <c r="M17" s="82"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="P17" s="56" t="str">
+      <c r="P17" s="83" t="str">
         <f t="shared" si="23"/>
-        <v>25:,</v>
-      </c>
-      <c r="Q17" s="56" t="str">
+        <v>25:#,</v>
+      </c>
+      <c r="Q17" s="83" t="str">
         <f>CONCATENATE($P17,$D17,",")</f>
-        <v>25:,,</v>
-      </c>
-      <c r="R17" s="57"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="57" t="s">
+        <v>25:#,Location (SF=1, Brkgs=2) (ip address),</v>
+      </c>
+      <c r="R17" s="84"/>
+      <c r="S17" s="85"/>
+      <c r="T17" s="84" t="s">
         <v>2</v>
       </c>
       <c r="X17" s="59" t="str">
         <f t="shared" si="24"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,</v>
       </c>
       <c r="Y17" s="59" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),</v>
       </c>
       <c r="Z17" s="60" t="str">
         <f t="shared" si="26"/>
@@ -4642,11 +4643,11 @@
       </c>
       <c r="AC17" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,</v>
       </c>
       <c r="AD17" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),</v>
       </c>
       <c r="AE17" s="61" t="str">
         <f t="shared" si="30"/>
@@ -4661,11 +4662,11 @@
       </c>
       <c r="AH17" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,</v>
       </c>
       <c r="AI17" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),</v>
       </c>
       <c r="AJ17" s="51" t="str">
         <f t="shared" si="34"/>
@@ -4678,65 +4679,86 @@
       <c r="AL17" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM17" s="51"/>
+      <c r="AN17" s="51"/>
+      <c r="AO17" s="51"/>
+      <c r="AP17" s="51"/>
+      <c r="AQ17" s="51"/>
+      <c r="AR17" s="51"/>
+      <c r="AS17" s="51"/>
+      <c r="AT17" s="51"/>
+      <c r="AU17" s="51"/>
+      <c r="AV17" s="51"/>
+      <c r="AW17" s="51"/>
+      <c r="AX17" s="51"/>
+      <c r="AY17" s="51"/>
+      <c r="AZ17" s="51"/>
+      <c r="BA17" s="51"/>
+      <c r="BB17" s="51"/>
+      <c r="BC17" s="51"/>
     </row>
-    <row r="18" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51">
+    <row r="18" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="75">
         <v>16</v>
       </c>
-      <c r="B18" s="51">
+      <c r="B18" s="75">
         <v>26</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="62" t="s">
+      <c r="C18" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="53" t="str">
+      <c r="F18" s="79" t="str">
         <f t="shared" si="19"/>
-        <v>26:,</v>
-      </c>
-      <c r="G18" s="63" t="str">
+        <v>26:#,</v>
+      </c>
+      <c r="G18" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>26:,,</v>
-      </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54" t="s">
+        <v>26:#,Alarm Enable,</v>
+      </c>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K18" s="54" t="str">
+      <c r="K18" s="81" t="str">
         <f t="shared" si="21"/>
-        <v>26:,</v>
-      </c>
-      <c r="L18" s="64" t="str">
+        <v>26:#,</v>
+      </c>
+      <c r="L18" s="81" t="str">
         <f t="shared" si="22"/>
-        <v>26:,,</v>
-      </c>
-      <c r="M18" s="55"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="55" t="s">
+        <v>26:#,Alarm Enable,</v>
+      </c>
+      <c r="M18" s="82"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="P18" s="56" t="str">
+      <c r="P18" s="83" t="str">
         <f t="shared" si="23"/>
-        <v>26:,</v>
-      </c>
-      <c r="Q18" s="56" t="str">
+        <v>26:#,</v>
+      </c>
+      <c r="Q18" s="83" t="str">
         <f>CONCATENATE($P18,$D18,",")</f>
-        <v>26:,,</v>
-      </c>
-      <c r="R18" s="57"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="57" t="s">
+        <v>26:#,Alarm Enable,</v>
+      </c>
+      <c r="R18" s="84"/>
+      <c r="S18" s="85"/>
+      <c r="T18" s="84" t="s">
         <v>2</v>
       </c>
       <c r="X18" s="59" t="str">
         <f t="shared" si="24"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,</v>
       </c>
       <c r="Y18" s="59" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,</v>
       </c>
       <c r="Z18" s="60" t="str">
         <f t="shared" si="26"/>
@@ -4751,11 +4773,11 @@
       </c>
       <c r="AC18" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,</v>
       </c>
       <c r="AD18" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,</v>
       </c>
       <c r="AE18" s="61" t="str">
         <f t="shared" si="30"/>
@@ -4770,11 +4792,11 @@
       </c>
       <c r="AH18" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,</v>
       </c>
       <c r="AI18" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,</v>
       </c>
       <c r="AJ18" s="51" t="str">
         <f t="shared" si="34"/>
@@ -4787,53 +4809,86 @@
       <c r="AL18" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM18" s="51"/>
+      <c r="AN18" s="51"/>
+      <c r="AO18" s="51"/>
+      <c r="AP18" s="51"/>
+      <c r="AQ18" s="51"/>
+      <c r="AR18" s="51"/>
+      <c r="AS18" s="51"/>
+      <c r="AT18" s="51"/>
+      <c r="AU18" s="51"/>
+      <c r="AV18" s="51"/>
+      <c r="AW18" s="51"/>
+      <c r="AX18" s="51"/>
+      <c r="AY18" s="51"/>
+      <c r="AZ18" s="51"/>
+      <c r="BA18" s="51"/>
+      <c r="BB18" s="51"/>
+      <c r="BC18" s="51"/>
     </row>
-    <row r="19" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51">
+    <row r="19" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="75">
         <v>17</v>
       </c>
-      <c r="B19" s="51">
+      <c r="B19" s="75">
         <v>27</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="62" t="s">
+      <c r="C19" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="53" t="str">
+      <c r="F19" s="79" t="str">
         <f t="shared" si="19"/>
-        <v>27:,</v>
-      </c>
-      <c r="G19" s="63" t="str">
+        <v>27:######,</v>
+      </c>
+      <c r="G19" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>27:,,</v>
-      </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54" t="s">
+        <v>27:######,Alarm Date,</v>
+      </c>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="55" t="s">
+      <c r="K19" s="81" t="str">
+        <f t="shared" si="21"/>
+        <v>27:######,</v>
+      </c>
+      <c r="L19" s="81" t="str">
+        <f t="shared" si="22"/>
+        <v>27:######,Alarm Date,</v>
+      </c>
+      <c r="M19" s="82"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="57"/>
-      <c r="S19" s="58"/>
-      <c r="T19" s="57" t="s">
+      <c r="P19" s="83" t="str">
+        <f t="shared" si="23"/>
+        <v>27:######,</v>
+      </c>
+      <c r="Q19" s="83" t="str">
+        <f>CONCATENATE($P19,$D19,",")</f>
+        <v>27:######,Alarm Date,</v>
+      </c>
+      <c r="R19" s="84"/>
+      <c r="S19" s="85"/>
+      <c r="T19" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X19" s="59" t="str">
         <f t="shared" ref="X19:X36" si="36">CONCATENATE(X18,F19)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,</v>
       </c>
       <c r="Y19" s="59" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,</v>
       </c>
       <c r="Z19" s="60" t="str">
         <f t="shared" si="26"/>
@@ -4848,11 +4903,11 @@
       </c>
       <c r="AC19" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,</v>
       </c>
       <c r="AD19" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,</v>
       </c>
       <c r="AE19" s="61" t="str">
         <f t="shared" si="30"/>
@@ -4867,11 +4922,11 @@
       </c>
       <c r="AH19" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,</v>
       </c>
       <c r="AI19" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,</v>
       </c>
       <c r="AJ19" s="51" t="str">
         <f t="shared" si="34"/>
@@ -4884,53 +4939,86 @@
       <c r="AL19" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM19" s="51"/>
+      <c r="AN19" s="51"/>
+      <c r="AO19" s="51"/>
+      <c r="AP19" s="51"/>
+      <c r="AQ19" s="51"/>
+      <c r="AR19" s="51"/>
+      <c r="AS19" s="51"/>
+      <c r="AT19" s="51"/>
+      <c r="AU19" s="51"/>
+      <c r="AV19" s="51"/>
+      <c r="AW19" s="51"/>
+      <c r="AX19" s="51"/>
+      <c r="AY19" s="51"/>
+      <c r="AZ19" s="51"/>
+      <c r="BA19" s="51"/>
+      <c r="BB19" s="51"/>
+      <c r="BC19" s="51"/>
     </row>
-    <row r="20" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51">
+    <row r="20" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="75">
         <v>18</v>
       </c>
-      <c r="B20" s="51">
+      <c r="B20" s="75">
         <v>28</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="62" t="s">
+      <c r="C20" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="53" t="str">
+      <c r="F20" s="79" t="str">
         <f t="shared" si="19"/>
-        <v>28:,</v>
-      </c>
-      <c r="G20" s="63" t="str">
+        <v>28:######,</v>
+      </c>
+      <c r="G20" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>28:,,</v>
-      </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54" t="s">
+        <v>28:######,Alarm Time,</v>
+      </c>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="55" t="s">
+      <c r="K20" s="81" t="str">
+        <f t="shared" si="21"/>
+        <v>28:######,</v>
+      </c>
+      <c r="L20" s="81" t="str">
+        <f t="shared" si="22"/>
+        <v>28:######,Alarm Time,</v>
+      </c>
+      <c r="M20" s="82"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="57" t="s">
+      <c r="P20" s="83" t="str">
+        <f t="shared" ref="P20:P21" si="37">CONCATENATE(B20,":",C20,",")</f>
+        <v>28:######,</v>
+      </c>
+      <c r="Q20" s="83" t="str">
+        <f>CONCATENATE($P20,$D20,",")</f>
+        <v>28:######,Alarm Time,</v>
+      </c>
+      <c r="R20" s="84"/>
+      <c r="S20" s="85"/>
+      <c r="T20" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X20" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,</v>
       </c>
       <c r="Y20" s="59" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,</v>
       </c>
       <c r="Z20" s="60" t="str">
         <f t="shared" si="26"/>
@@ -4945,11 +5033,11 @@
       </c>
       <c r="AC20" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,</v>
       </c>
       <c r="AD20" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,</v>
       </c>
       <c r="AE20" s="61" t="str">
         <f t="shared" si="30"/>
@@ -4964,11 +5052,11 @@
       </c>
       <c r="AH20" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,</v>
       </c>
       <c r="AI20" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,</v>
       </c>
       <c r="AJ20" s="51" t="str">
         <f t="shared" si="34"/>
@@ -4981,53 +5069,86 @@
       <c r="AL20" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM20" s="51"/>
+      <c r="AN20" s="51"/>
+      <c r="AO20" s="51"/>
+      <c r="AP20" s="51"/>
+      <c r="AQ20" s="51"/>
+      <c r="AR20" s="51"/>
+      <c r="AS20" s="51"/>
+      <c r="AT20" s="51"/>
+      <c r="AU20" s="51"/>
+      <c r="AV20" s="51"/>
+      <c r="AW20" s="51"/>
+      <c r="AX20" s="51"/>
+      <c r="AY20" s="51"/>
+      <c r="AZ20" s="51"/>
+      <c r="BA20" s="51"/>
+      <c r="BB20" s="51"/>
+      <c r="BC20" s="51"/>
     </row>
-    <row r="21" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51">
+    <row r="21" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="75">
         <v>19</v>
       </c>
-      <c r="B21" s="51">
+      <c r="B21" s="75">
         <v>29</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="62" t="s">
+      <c r="C21" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="53" t="str">
-        <f>CONCATENATE($B21,":",$C21,",")</f>
-        <v>29:,</v>
-      </c>
-      <c r="G21" s="63" t="str">
+      <c r="F21" s="79" t="str">
+        <f t="shared" si="19"/>
+        <v>29:##,</v>
+      </c>
+      <c r="G21" s="80" t="str">
         <f t="shared" si="20"/>
-        <v>29:,,</v>
-      </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54" t="s">
+        <v>29:##,Performance number,</v>
+      </c>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="55" t="s">
+      <c r="K21" s="81" t="str">
+        <f t="shared" si="21"/>
+        <v>29:##,</v>
+      </c>
+      <c r="L21" s="81" t="str">
+        <f t="shared" si="22"/>
+        <v>29:##,Performance number,</v>
+      </c>
+      <c r="M21" s="82"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="57"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="57" t="s">
+      <c r="P21" s="83" t="str">
+        <f t="shared" si="37"/>
+        <v>29:##,</v>
+      </c>
+      <c r="Q21" s="83" t="str">
+        <f>CONCATENATE($P21,$D21,",")</f>
+        <v>29:##,Performance number,</v>
+      </c>
+      <c r="R21" s="84"/>
+      <c r="S21" s="85"/>
+      <c r="T21" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X21" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,</v>
       </c>
       <c r="Y21" s="59" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,</v>
       </c>
       <c r="Z21" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5042,11 +5163,11 @@
       </c>
       <c r="AC21" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,</v>
       </c>
       <c r="AD21" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,</v>
       </c>
       <c r="AE21" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5061,11 +5182,11 @@
       </c>
       <c r="AH21" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,</v>
       </c>
       <c r="AI21" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,</v>
       </c>
       <c r="AJ21" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5078,53 +5199,70 @@
       <c r="AL21" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM21" s="51"/>
+      <c r="AN21" s="51"/>
+      <c r="AO21" s="51"/>
+      <c r="AP21" s="51"/>
+      <c r="AQ21" s="51"/>
+      <c r="AR21" s="51"/>
+      <c r="AS21" s="51"/>
+      <c r="AT21" s="51"/>
+      <c r="AU21" s="51"/>
+      <c r="AV21" s="51"/>
+      <c r="AW21" s="51"/>
+      <c r="AX21" s="51"/>
+      <c r="AY21" s="51"/>
+      <c r="AZ21" s="51"/>
+      <c r="BA21" s="51"/>
+      <c r="BB21" s="51"/>
+      <c r="BC21" s="51"/>
     </row>
-    <row r="22" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51">
+    <row r="22" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="75">
         <v>20</v>
       </c>
-      <c r="B22" s="51">
+      <c r="B22" s="75">
         <v>30</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="62" t="s">
+      <c r="C22" s="76"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="53" t="str">
+      <c r="F22" s="79" t="str">
         <f>CONCATENATE($B22,":",$C22,",")</f>
         <v>30:,</v>
       </c>
-      <c r="G22" s="63" t="str">
+      <c r="G22" s="80" t="str">
         <f t="shared" si="20"/>
         <v>30:,,</v>
       </c>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54" t="s">
+      <c r="H22" s="81"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="55" t="s">
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="57"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="57" t="s">
+      <c r="P22" s="83"/>
+      <c r="Q22" s="83"/>
+      <c r="R22" s="84"/>
+      <c r="S22" s="85"/>
+      <c r="T22" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X22" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,</v>
       </c>
       <c r="Y22" s="59" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,</v>
       </c>
       <c r="Z22" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5139,11 +5277,11 @@
       </c>
       <c r="AC22" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,</v>
       </c>
       <c r="AD22" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,</v>
       </c>
       <c r="AE22" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5158,11 +5296,11 @@
       </c>
       <c r="AH22" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,</v>
       </c>
       <c r="AI22" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,</v>
       </c>
       <c r="AJ22" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5175,59 +5313,76 @@
       <c r="AL22" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM22" s="51"/>
+      <c r="AN22" s="51"/>
+      <c r="AO22" s="51"/>
+      <c r="AP22" s="51"/>
+      <c r="AQ22" s="51"/>
+      <c r="AR22" s="51"/>
+      <c r="AS22" s="51"/>
+      <c r="AT22" s="51"/>
+      <c r="AU22" s="51"/>
+      <c r="AV22" s="51"/>
+      <c r="AW22" s="51"/>
+      <c r="AX22" s="51"/>
+      <c r="AY22" s="51"/>
+      <c r="AZ22" s="51"/>
+      <c r="BA22" s="51"/>
+      <c r="BB22" s="51"/>
+      <c r="BC22" s="51"/>
     </row>
-    <row r="23" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="51">
+    <row r="23" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="75">
         <v>21</v>
       </c>
-      <c r="B23" s="51">
+      <c r="B23" s="75">
         <v>31</v>
       </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="62" t="s">
+      <c r="C23" s="76"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="53" t="str">
+      <c r="F23" s="79" t="str">
         <f>CONCATENATE($B23,":",$C23,",")</f>
         <v>31:,</v>
       </c>
-      <c r="G23" s="63" t="str">
+      <c r="G23" s="80" t="str">
         <f t="shared" si="20"/>
         <v>31:,,</v>
       </c>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54" t="s">
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="K23" s="54" t="str">
+      <c r="K23" s="81" t="str">
         <f>CONCATENATE($B23,":",$C23,",")</f>
         <v>31:,</v>
       </c>
-      <c r="L23" s="64" t="str">
+      <c r="L23" s="81" t="str">
         <f>CONCATENATE($K23,$D23,",")</f>
         <v>31:,,</v>
       </c>
-      <c r="M23" s="55"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="55" t="s">
+      <c r="M23" s="82"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="57"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="57" t="s">
+      <c r="P23" s="83"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="84"/>
+      <c r="S23" s="85"/>
+      <c r="T23" s="84" t="s">
         <v>1</v>
       </c>
       <c r="X23" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,</v>
       </c>
       <c r="Y23" s="59" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,</v>
       </c>
       <c r="Z23" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5242,11 +5397,11 @@
       </c>
       <c r="AC23" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,</v>
       </c>
       <c r="AD23" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,</v>
       </c>
       <c r="AE23" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5261,11 +5416,11 @@
       </c>
       <c r="AH23" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,</v>
       </c>
       <c r="AI23" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,</v>
       </c>
       <c r="AJ23" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5278,8 +5433,25 @@
       <c r="AL23" s="61" t="s">
         <v>49</v>
       </c>
+      <c r="AM23" s="51"/>
+      <c r="AN23" s="51"/>
+      <c r="AO23" s="51"/>
+      <c r="AP23" s="51"/>
+      <c r="AQ23" s="51"/>
+      <c r="AR23" s="51"/>
+      <c r="AS23" s="51"/>
+      <c r="AT23" s="51"/>
+      <c r="AU23" s="51"/>
+      <c r="AV23" s="51"/>
+      <c r="AW23" s="51"/>
+      <c r="AX23" s="51"/>
+      <c r="AY23" s="51"/>
+      <c r="AZ23" s="51"/>
+      <c r="BA23" s="51"/>
+      <c r="BB23" s="51"/>
+      <c r="BC23" s="51"/>
     </row>
-    <row r="24" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="51">
         <v>22</v>
       </c>
@@ -5318,10 +5490,10 @@
         <v>6</v>
       </c>
       <c r="P24" s="56" t="str">
-        <f t="shared" ref="P24" si="37">CONCATENATE(B24,":",C24,",")</f>
+        <f t="shared" ref="P24" si="38">CONCATENATE(B24,":",C24,",")</f>
         <v>32:,</v>
       </c>
-      <c r="Q24" s="67" t="str">
+      <c r="Q24" s="66" t="str">
         <f>CONCATENATE($P24,$D24,",")</f>
         <v>32:,,</v>
       </c>
@@ -5332,11 +5504,11 @@
       </c>
       <c r="X24" s="59" t="str">
         <f>CONCATENATE(X23,F24)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y24" s="59" t="str">
         <f>CONCATENATE(Y23,G24)</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z24" s="60" t="str">
         <f>CONCATENATE(Z23,H24)</f>
@@ -5351,11 +5523,11 @@
       </c>
       <c r="AC24" s="60" t="str">
         <f>CONCATENATE(AC23,K24)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD24" s="60" t="str">
         <f>CONCATENATE(AD23,L24)</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE24" s="61" t="str">
         <f>CONCATENATE(AE23,M24)</f>
@@ -5370,11 +5542,11 @@
       </c>
       <c r="AH24" s="61" t="str">
         <f>CONCATENATE(AH23,P24)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI24" s="61" t="str">
         <f>CONCATENATE(AI23,Q24)</f>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ24" s="51" t="str">
         <f>CONCATENATE(AJ23,R24)</f>
@@ -5388,7 +5560,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5425,11 +5597,11 @@
       </c>
       <c r="X25" s="22" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y25" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z25" s="37" t="str">
         <f t="shared" si="26"/>
@@ -5444,11 +5616,11 @@
       </c>
       <c r="AC25" s="37" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD25" s="37" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE25" s="18" t="str">
         <f t="shared" si="30"/>
@@ -5463,11 +5635,11 @@
       </c>
       <c r="AH25" s="18" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI25" s="18" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ25" t="str">
         <f t="shared" si="34"/>
@@ -5481,14 +5653,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51">
         <v>24</v>
       </c>
       <c r="B26" s="51">
         <v>34</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D26" s="52" t="s">
@@ -5500,14 +5672,14 @@
       <c r="F26" s="53"/>
       <c r="G26" s="53"/>
       <c r="H26" s="54" t="str">
-        <f t="shared" ref="H26:H42" si="38">CONCATENATE($B26,":",$C26,",")</f>
+        <f t="shared" ref="H26:H42" si="39">CONCATENATE($B26,":",$C26,",")</f>
         <v>34:#,</v>
       </c>
       <c r="I26" s="64" t="str">
         <f>CONCATENATE($H26,$D26,",")</f>
         <v>34:#,Shop door status,</v>
       </c>
-      <c r="J26" s="69" t="s">
+      <c r="J26" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K26" s="54"/>
@@ -5526,11 +5698,11 @@
       </c>
       <c r="X26" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y26" s="59" t="str">
         <f>CONCATENATE(Y25,G26)</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z26" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5545,11 +5717,11 @@
       </c>
       <c r="AC26" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD26" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE26" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5564,11 +5736,11 @@
       </c>
       <c r="AH26" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI26" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ26" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5582,14 +5754,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="51">
         <v>25</v>
       </c>
       <c r="B27" s="51">
         <v>35</v>
       </c>
-      <c r="C27" s="68" t="s">
+      <c r="C27" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="52" t="s">
@@ -5601,14 +5773,14 @@
       <c r="F27" s="53"/>
       <c r="G27" s="53"/>
       <c r="H27" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>35:#,</v>
       </c>
       <c r="I27" s="64" t="str">
-        <f t="shared" ref="I27:I42" si="39">CONCATENATE($H27,$D27,",")</f>
+        <f t="shared" ref="I27:I42" si="40">CONCATENATE($H27,$D27,",")</f>
         <v>35:#,Shop deadbolt status,</v>
       </c>
-      <c r="J27" s="69" t="s">
+      <c r="J27" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K27" s="54"/>
@@ -5627,11 +5799,11 @@
       </c>
       <c r="X27" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y27" s="59" t="str">
-        <f t="shared" ref="Y27:Y44" si="40">CONCATENATE(Y26,G27)</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" ref="Y27:Y44" si="41">CONCATENATE(Y26,G27)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z27" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5646,11 +5818,11 @@
       </c>
       <c r="AC27" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD27" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE27" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5665,11 +5837,11 @@
       </c>
       <c r="AH27" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI27" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ27" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5683,14 +5855,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="51">
         <v>26</v>
       </c>
       <c r="B28" s="51">
         <v>36</v>
       </c>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D28" s="52" t="s">
@@ -5702,14 +5874,14 @@
       <c r="F28" s="53"/>
       <c r="G28" s="53"/>
       <c r="H28" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>36:#,</v>
       </c>
       <c r="I28" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>36:#,Alarm mode,</v>
       </c>
-      <c r="J28" s="69" t="s">
+      <c r="J28" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K28" s="54"/>
@@ -5728,11 +5900,11 @@
       </c>
       <c r="X28" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y28" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z28" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5747,11 +5919,11 @@
       </c>
       <c r="AC28" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD28" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE28" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5766,11 +5938,11 @@
       </c>
       <c r="AH28" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI28" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ28" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5784,14 +5956,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="51">
         <v>27</v>
       </c>
       <c r="B29" s="51">
         <v>37</v>
       </c>
-      <c r="C29" s="70" t="s">
+      <c r="C29" s="69" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="65" t="s">
@@ -5803,14 +5975,14 @@
       <c r="F29" s="53"/>
       <c r="G29" s="53"/>
       <c r="H29" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>37:#,</v>
       </c>
       <c r="I29" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>37:#,Security Level (soft, med, hard),</v>
       </c>
-      <c r="J29" s="69" t="s">
+      <c r="J29" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K29" s="54"/>
@@ -5829,11 +6001,11 @@
       </c>
       <c r="X29" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y29" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z29" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5848,11 +6020,11 @@
       </c>
       <c r="AC29" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD29" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE29" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5867,11 +6039,11 @@
       </c>
       <c r="AH29" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI29" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ29" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5885,14 +6057,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="51">
         <v>28</v>
       </c>
       <c r="B30" s="51">
         <v>38</v>
       </c>
-      <c r="C30" s="70" t="s">
+      <c r="C30" s="69" t="s">
         <v>33</v>
       </c>
       <c r="D30" s="65" t="s">
@@ -5904,14 +6076,14 @@
       <c r="F30" s="53"/>
       <c r="G30" s="53"/>
       <c r="H30" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>38:#,</v>
       </c>
       <c r="I30" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>38:#,Manual change in alarm mode,</v>
       </c>
-      <c r="J30" s="69" t="s">
+      <c r="J30" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K30" s="54"/>
@@ -5930,11 +6102,11 @@
       </c>
       <c r="X30" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y30" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z30" s="60" t="str">
         <f t="shared" si="26"/>
@@ -5949,11 +6121,11 @@
       </c>
       <c r="AC30" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD30" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE30" s="61" t="str">
         <f t="shared" si="30"/>
@@ -5968,11 +6140,11 @@
       </c>
       <c r="AH30" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI30" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ30" s="51" t="str">
         <f t="shared" si="34"/>
@@ -5986,14 +6158,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="51">
         <v>29</v>
       </c>
       <c r="B31" s="51">
         <v>39</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="69" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="65" t="s">
@@ -6005,27 +6177,27 @@
       <c r="F31" s="53"/>
       <c r="G31" s="53"/>
       <c r="H31" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>39:####,</v>
       </c>
       <c r="I31" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>39:####,Shop Brightness (0 to ####),</v>
       </c>
-      <c r="J31" s="69" t="s">
+      <c r="J31" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K31" s="54"/>
       <c r="L31" s="54"/>
       <c r="M31" s="55" t="str">
-        <f t="shared" ref="M31:M44" si="41">CONCATENATE($B31,":",$C31,",")</f>
+        <f t="shared" ref="M31:M44" si="42">CONCATENATE($B31,":",$C31,",")</f>
         <v>39:####,</v>
       </c>
-      <c r="N31" s="67" t="str">
-        <f t="shared" ref="N31:N44" si="42">CONCATENATE($B31,":",$D31,",")</f>
+      <c r="N31" s="66" t="str">
+        <f t="shared" ref="N31:N44" si="43">CONCATENATE($B31,":",$D31,",")</f>
         <v>39:Shop Brightness (0 to ####),</v>
       </c>
-      <c r="O31" s="71" t="s">
+      <c r="O31" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P31" s="56"/>
@@ -6038,7 +6210,7 @@
         <f>CONCATENATE($R31,$D31,",")</f>
         <v>39:####,Shop Brightness (0 to ####),</v>
       </c>
-      <c r="T31" s="72" t="s">
+      <c r="T31" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U31" s="51" t="s">
@@ -6046,11 +6218,11 @@
       </c>
       <c r="X31" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y31" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z31" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6065,11 +6237,11 @@
       </c>
       <c r="AC31" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD31" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE31" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6084,11 +6256,11 @@
       </c>
       <c r="AH31" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI31" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ31" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6102,14 +6274,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:38" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:55" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="51">
         <v>30</v>
       </c>
       <c r="B32" s="51">
         <v>40</v>
       </c>
-      <c r="C32" s="70" t="s">
+      <c r="C32" s="69" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="65" t="s">
@@ -6121,40 +6293,40 @@
       <c r="F32" s="53"/>
       <c r="G32" s="53"/>
       <c r="H32" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>40:###,</v>
       </c>
       <c r="I32" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>40:###,Shop Temp now (### F) *,</v>
       </c>
-      <c r="J32" s="69" t="s">
+      <c r="J32" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K32" s="54"/>
       <c r="L32" s="54"/>
       <c r="M32" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>40:###,</v>
       </c>
-      <c r="N32" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N32" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>40:Shop Temp now (### F) *,</v>
       </c>
-      <c r="O32" s="71" t="s">
+      <c r="O32" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P32" s="56"/>
       <c r="Q32" s="56"/>
       <c r="R32" s="58" t="str">
-        <f t="shared" ref="R32:R38" si="43">CONCATENATE(B32,":",C32,",")</f>
+        <f t="shared" ref="R32:R38" si="44">CONCATENATE(B32,":",C32,",")</f>
         <v>40:###,</v>
       </c>
       <c r="S32" s="58" t="str">
-        <f t="shared" ref="S32:S38" si="44">CONCATENATE($R32,$D32,",")</f>
+        <f t="shared" ref="S32:S38" si="45">CONCATENATE($R32,$D32,",")</f>
         <v>40:###,Shop Temp now (### F) *,</v>
       </c>
-      <c r="T32" s="72" t="s">
+      <c r="T32" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U32" s="51" t="s">
@@ -6162,11 +6334,11 @@
       </c>
       <c r="X32" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y32" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z32" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6181,11 +6353,11 @@
       </c>
       <c r="AC32" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD32" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE32" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6200,11 +6372,11 @@
       </c>
       <c r="AH32" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI32" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ32" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6225,7 +6397,7 @@
       <c r="B33" s="51">
         <v>41</v>
       </c>
-      <c r="C33" s="70" t="s">
+      <c r="C33" s="69" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="65" t="s">
@@ -6237,40 +6409,40 @@
       <c r="F33" s="53"/>
       <c r="G33" s="53"/>
       <c r="H33" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>41:###,</v>
       </c>
       <c r="I33" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>41:###,Shop Humidity (### %) *,</v>
       </c>
-      <c r="J33" s="69" t="s">
+      <c r="J33" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K33" s="54"/>
       <c r="L33" s="54"/>
       <c r="M33" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>41:###,</v>
       </c>
-      <c r="N33" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N33" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>41:Shop Humidity (### %) *,</v>
       </c>
-      <c r="O33" s="71" t="s">
+      <c r="O33" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P33" s="56"/>
       <c r="Q33" s="56"/>
       <c r="R33" s="58" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>41:###,</v>
       </c>
       <c r="S33" s="58" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>41:###,Shop Humidity (### %) *,</v>
       </c>
-      <c r="T33" s="72" t="s">
+      <c r="T33" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U33" s="51" t="s">
@@ -6278,11 +6450,11 @@
       </c>
       <c r="X33" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y33" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z33" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6297,11 +6469,11 @@
       </c>
       <c r="AC33" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD33" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE33" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6316,11 +6488,11 @@
       </c>
       <c r="AH33" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI33" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ33" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6341,7 +6513,7 @@
       <c r="B34" s="51">
         <v>42</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C34" s="69" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="65" t="s">
@@ -6353,40 +6525,40 @@
       <c r="F34" s="53"/>
       <c r="G34" s="53"/>
       <c r="H34" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>42:###,</v>
       </c>
       <c r="I34" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>42:###,Shop Heat Index (### F) *,</v>
       </c>
-      <c r="J34" s="69" t="s">
+      <c r="J34" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K34" s="54"/>
       <c r="L34" s="54"/>
       <c r="M34" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>42:###,</v>
       </c>
-      <c r="N34" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N34" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>42:Shop Heat Index (### F) *,</v>
       </c>
-      <c r="O34" s="71" t="s">
+      <c r="O34" s="70" t="s">
         <v>22</v>
       </c>
       <c r="P34" s="56"/>
       <c r="Q34" s="56"/>
       <c r="R34" s="58" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>42:###,</v>
       </c>
       <c r="S34" s="58" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>42:###,Shop Heat Index (### F) *,</v>
       </c>
-      <c r="T34" s="72" t="s">
+      <c r="T34" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U34" s="51" t="s">
@@ -6394,11 +6566,11 @@
       </c>
       <c r="X34" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y34" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z34" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6413,11 +6585,11 @@
       </c>
       <c r="AC34" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD34" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE34" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6432,11 +6604,11 @@
       </c>
       <c r="AH34" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI34" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ34" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6457,7 +6629,7 @@
       <c r="B35" s="51">
         <v>43</v>
       </c>
-      <c r="C35" s="70" t="s">
+      <c r="C35" s="69" t="s">
         <v>42</v>
       </c>
       <c r="D35" s="65" t="s">
@@ -6469,40 +6641,40 @@
       <c r="F35" s="53"/>
       <c r="G35" s="53"/>
       <c r="H35" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>43:####,</v>
       </c>
       <c r="I35" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>43:####,Motion@base of stairs,</v>
       </c>
-      <c r="J35" s="69" t="s">
+      <c r="J35" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K35" s="54"/>
       <c r="L35" s="54"/>
       <c r="M35" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>43:####,</v>
       </c>
-      <c r="N35" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N35" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>43:Motion@base of stairs,</v>
       </c>
-      <c r="O35" s="71" t="s">
+      <c r="O35" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P35" s="56"/>
       <c r="Q35" s="56"/>
       <c r="R35" s="58" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>43:####,</v>
       </c>
       <c r="S35" s="58" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>43:####,Motion@base of stairs,</v>
       </c>
-      <c r="T35" s="72" t="s">
+      <c r="T35" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U35" s="51" t="s">
@@ -6510,11 +6682,11 @@
       </c>
       <c r="X35" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y35" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z35" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6529,11 +6701,11 @@
       </c>
       <c r="AC35" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD35" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE35" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6548,11 +6720,11 @@
       </c>
       <c r="AH35" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI35" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ35" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6573,7 +6745,7 @@
       <c r="B36" s="51">
         <v>44</v>
       </c>
-      <c r="C36" s="70" t="s">
+      <c r="C36" s="69" t="s">
         <v>42</v>
       </c>
       <c r="D36" s="65" t="s">
@@ -6585,40 +6757,40 @@
       <c r="F36" s="53"/>
       <c r="G36" s="53"/>
       <c r="H36" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>44:####,</v>
       </c>
       <c r="I36" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>44:####,Motion@top of stairs,</v>
       </c>
-      <c r="J36" s="69" t="s">
+      <c r="J36" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K36" s="54"/>
       <c r="L36" s="54"/>
       <c r="M36" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>44:####,</v>
       </c>
-      <c r="N36" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N36" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>44:Motion@top of stairs,</v>
       </c>
-      <c r="O36" s="71" t="s">
+      <c r="O36" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P36" s="56"/>
       <c r="Q36" s="56"/>
       <c r="R36" s="58" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>44:####,</v>
       </c>
       <c r="S36" s="58" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>44:####,Motion@top of stairs,</v>
       </c>
-      <c r="T36" s="72" t="s">
+      <c r="T36" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U36" s="51" t="s">
@@ -6626,11 +6798,11 @@
       </c>
       <c r="X36" s="59" t="str">
         <f t="shared" si="36"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y36" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z36" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6645,11 +6817,11 @@
       </c>
       <c r="AC36" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD36" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE36" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6664,11 +6836,11 @@
       </c>
       <c r="AH36" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI36" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ36" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6689,7 +6861,7 @@
       <c r="B37" s="51">
         <v>45</v>
       </c>
-      <c r="C37" s="70" t="s">
+      <c r="C37" s="69" t="s">
         <v>42</v>
       </c>
       <c r="D37" s="65" t="s">
@@ -6701,52 +6873,52 @@
       <c r="F37" s="53"/>
       <c r="G37" s="53"/>
       <c r="H37" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>45:####,</v>
       </c>
       <c r="I37" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>45:####,Motion@garage door,</v>
       </c>
-      <c r="J37" s="69" t="s">
+      <c r="J37" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K37" s="54"/>
       <c r="L37" s="54"/>
       <c r="M37" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>45:####,</v>
       </c>
-      <c r="N37" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N37" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>45:Motion@garage door,</v>
       </c>
-      <c r="O37" s="71" t="s">
+      <c r="O37" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P37" s="56"/>
       <c r="Q37" s="56"/>
       <c r="R37" s="58" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>45:####,</v>
       </c>
       <c r="S37" s="58" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>45:####,Motion@garage door,</v>
       </c>
-      <c r="T37" s="72" t="s">
+      <c r="T37" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U37" s="51" t="s">
         <v>53</v>
       </c>
       <c r="X37" s="59" t="str">
-        <f t="shared" ref="X37:X44" si="45">CONCATENATE(X36,F37)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <f t="shared" ref="X37:X44" si="46">CONCATENATE(X36,F37)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y37" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z37" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6761,11 +6933,11 @@
       </c>
       <c r="AC37" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD37" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE37" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6780,11 +6952,11 @@
       </c>
       <c r="AH37" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI37" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ37" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6805,7 +6977,7 @@
       <c r="B38" s="51">
         <v>46</v>
       </c>
-      <c r="C38" s="70" t="s">
+      <c r="C38" s="69" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="65" t="s">
@@ -6817,52 +6989,52 @@
       <c r="F38" s="53"/>
       <c r="G38" s="53"/>
       <c r="H38" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>46:####,</v>
       </c>
       <c r="I38" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>46:####,Motion@windows,</v>
       </c>
-      <c r="J38" s="69" t="s">
+      <c r="J38" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K38" s="54"/>
       <c r="L38" s="54"/>
       <c r="M38" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>46:####,</v>
       </c>
-      <c r="N38" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N38" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>46:Motion@windows,</v>
       </c>
-      <c r="O38" s="71" t="s">
+      <c r="O38" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P38" s="56"/>
       <c r="Q38" s="56"/>
       <c r="R38" s="58" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>46:####,</v>
       </c>
       <c r="S38" s="58" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>46:####,Motion@windows,</v>
       </c>
-      <c r="T38" s="72" t="s">
+      <c r="T38" s="71" t="s">
         <v>43</v>
       </c>
       <c r="U38" s="51" t="s">
         <v>54</v>
       </c>
       <c r="X38" s="59" t="str">
-        <f t="shared" si="45"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <f t="shared" si="46"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y38" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z38" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6877,11 +7049,11 @@
       </c>
       <c r="AC38" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD38" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE38" s="61" t="str">
         <f t="shared" si="30"/>
@@ -6896,11 +7068,11 @@
       </c>
       <c r="AH38" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI38" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ38" s="51" t="str">
         <f t="shared" si="34"/>
@@ -6921,7 +7093,7 @@
       <c r="B39" s="51">
         <v>47</v>
       </c>
-      <c r="C39" s="70" t="s">
+      <c r="C39" s="69" t="s">
         <v>41</v>
       </c>
       <c r="D39" s="65" t="s">
@@ -6933,27 +7105,27 @@
       <c r="F39" s="53"/>
       <c r="G39" s="53"/>
       <c r="H39" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>47:###,</v>
       </c>
       <c r="I39" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>47:###,ShopTempDayHigh (### F),</v>
       </c>
-      <c r="J39" s="69" t="s">
+      <c r="J39" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K39" s="54"/>
       <c r="L39" s="54"/>
       <c r="M39" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>47:###,</v>
       </c>
-      <c r="N39" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N39" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>47:ShopTempDayHigh (### F),</v>
       </c>
-      <c r="O39" s="71" t="s">
+      <c r="O39" s="70" t="s">
         <v>22</v>
       </c>
       <c r="P39" s="56"/>
@@ -6964,12 +7136,12 @@
         <v>1</v>
       </c>
       <c r="X39" s="59" t="str">
-        <f t="shared" si="45"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <f t="shared" si="46"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y39" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z39" s="60" t="str">
         <f t="shared" si="26"/>
@@ -6984,11 +7156,11 @@
       </c>
       <c r="AC39" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD39" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE39" s="61" t="str">
         <f t="shared" si="30"/>
@@ -7003,11 +7175,11 @@
       </c>
       <c r="AH39" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI39" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ39" s="51" t="str">
         <f t="shared" si="34"/>
@@ -7028,7 +7200,7 @@
       <c r="B40" s="51">
         <v>48</v>
       </c>
-      <c r="C40" s="70" t="s">
+      <c r="C40" s="69" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="65" t="s">
@@ -7040,27 +7212,27 @@
       <c r="F40" s="53"/>
       <c r="G40" s="53"/>
       <c r="H40" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>48:###,</v>
       </c>
       <c r="I40" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>48:###,ShopTempDayLow (### F),</v>
       </c>
-      <c r="J40" s="69" t="s">
+      <c r="J40" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K40" s="54"/>
       <c r="L40" s="54"/>
       <c r="M40" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>48:###,</v>
       </c>
-      <c r="N40" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N40" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>48:ShopTempDayLow (### F),</v>
       </c>
-      <c r="O40" s="71" t="s">
+      <c r="O40" s="70" t="s">
         <v>22</v>
       </c>
       <c r="P40" s="56"/>
@@ -7071,12 +7243,12 @@
         <v>1</v>
       </c>
       <c r="X40" s="59" t="str">
-        <f t="shared" si="45"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <f t="shared" si="46"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y40" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z40" s="60" t="str">
         <f t="shared" si="26"/>
@@ -7091,11 +7263,11 @@
       </c>
       <c r="AC40" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD40" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE40" s="61" t="str">
         <f t="shared" si="30"/>
@@ -7110,11 +7282,11 @@
       </c>
       <c r="AH40" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI40" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ40" s="51" t="str">
         <f t="shared" si="34"/>
@@ -7135,7 +7307,7 @@
       <c r="B41" s="51">
         <v>49</v>
       </c>
-      <c r="C41" s="70" t="s">
+      <c r="C41" s="69" t="s">
         <v>42</v>
       </c>
       <c r="D41" s="65" t="s">
@@ -7147,27 +7319,27 @@
       <c r="F41" s="53"/>
       <c r="G41" s="53"/>
       <c r="H41" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>49:####,</v>
       </c>
       <c r="I41" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>49:####,SM_Outlet#0-3States,</v>
       </c>
-      <c r="J41" s="69" t="s">
+      <c r="J41" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K41" s="54"/>
       <c r="L41" s="54"/>
       <c r="M41" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>49:####,</v>
       </c>
-      <c r="N41" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N41" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>49:SM_Outlet#0-3States,</v>
       </c>
-      <c r="O41" s="71" t="s">
+      <c r="O41" s="70" t="s">
         <v>22</v>
       </c>
       <c r="P41" s="56"/>
@@ -7177,19 +7349,19 @@
         <v>49:####,</v>
       </c>
       <c r="S41" s="58" t="str">
-        <f t="shared" ref="S41:S42" si="46">CONCATENATE($R41,$D41,",")</f>
+        <f t="shared" ref="S41:S42" si="47">CONCATENATE($R41,$D41,",")</f>
         <v>49:####,SM_Outlet#0-3States,</v>
       </c>
       <c r="T41" s="57" t="s">
         <v>1</v>
       </c>
       <c r="X41" s="59" t="str">
-        <f t="shared" si="45"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <f t="shared" si="46"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y41" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z41" s="60" t="str">
         <f t="shared" si="26"/>
@@ -7204,11 +7376,11 @@
       </c>
       <c r="AC41" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD41" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE41" s="61" t="str">
         <f t="shared" si="30"/>
@@ -7223,11 +7395,11 @@
       </c>
       <c r="AH41" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI41" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ41" s="51" t="str">
         <f t="shared" si="34"/>
@@ -7248,7 +7420,7 @@
       <c r="B42" s="51">
         <v>50</v>
       </c>
-      <c r="C42" s="70" t="s">
+      <c r="C42" s="69" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="65" t="s">
@@ -7260,27 +7432,27 @@
       <c r="F42" s="53"/>
       <c r="G42" s="53"/>
       <c r="H42" s="54" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>50:##,</v>
       </c>
       <c r="I42" s="64" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>50:##,MotionButton1-2 states (disarm,arm),</v>
       </c>
-      <c r="J42" s="69" t="s">
+      <c r="J42" s="68" t="s">
         <v>11</v>
       </c>
       <c r="K42" s="54"/>
       <c r="L42" s="54"/>
       <c r="M42" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>50:##,</v>
       </c>
-      <c r="N42" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N42" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>50:MotionButton1-2 states (disarm,arm),</v>
       </c>
-      <c r="O42" s="71" t="s">
+      <c r="O42" s="70" t="s">
         <v>17</v>
       </c>
       <c r="P42" s="56"/>
@@ -7290,19 +7462,19 @@
         <v>50:##,</v>
       </c>
       <c r="S42" s="58" t="str">
+        <f t="shared" si="47"/>
+        <v>50:##,MotionButton1-2 states (disarm,arm),</v>
+      </c>
+      <c r="T42" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="X42" s="59" t="str">
         <f t="shared" si="46"/>
-        <v>50:##,MotionButton1-2 states (disarm,arm),</v>
-      </c>
-      <c r="T42" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="X42" s="59" t="str">
-        <f t="shared" si="45"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y42" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z42" s="60" t="str">
         <f t="shared" si="26"/>
@@ -7317,11 +7489,11 @@
       </c>
       <c r="AC42" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD42" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE42" s="61" t="str">
         <f t="shared" si="30"/>
@@ -7336,11 +7508,11 @@
       </c>
       <c r="AH42" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI42" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ42" s="51" t="str">
         <f t="shared" si="34"/>
@@ -7361,7 +7533,7 @@
       <c r="B43" s="51">
         <v>51</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="69" t="s">
         <v>42</v>
       </c>
       <c r="D43" s="65" t="s">
@@ -7380,11 +7552,11 @@
       <c r="K43" s="54"/>
       <c r="L43" s="54"/>
       <c r="M43" s="55" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>51:####,</v>
       </c>
-      <c r="N43" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N43" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>51:Time (military time to minute),</v>
       </c>
       <c r="O43" s="55" t="s">
@@ -7398,12 +7570,12 @@
         <v>1</v>
       </c>
       <c r="X43" s="59" t="str">
-        <f t="shared" si="45"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <f t="shared" si="46"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y43" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z43" s="60" t="str">
         <f t="shared" si="26"/>
@@ -7418,11 +7590,11 @@
       </c>
       <c r="AC43" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD43" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE43" s="61" t="str">
         <f t="shared" si="30"/>
@@ -7437,11 +7609,11 @@
       </c>
       <c r="AH43" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI43" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ43" s="51" t="str">
         <f t="shared" si="34"/>
@@ -7462,7 +7634,7 @@
       <c r="B44" s="51">
         <v>52</v>
       </c>
-      <c r="C44" s="73" t="s">
+      <c r="C44" s="72" t="s">
         <v>48</v>
       </c>
       <c r="D44" s="65" t="s">
@@ -7473,7 +7645,7 @@
       </c>
       <c r="F44" s="53"/>
       <c r="G44" s="53"/>
-      <c r="H44" s="74" t="str">
+      <c r="H44" s="73" t="str">
         <f>CONCATENATE($B44,":",$C44,",")</f>
         <v>52:##################################################,</v>
       </c>
@@ -7481,20 +7653,20 @@
         <f>CONCATENATE($H44,$D44,",")</f>
         <v>52:##################################################,NoticeWord (Notifications),</v>
       </c>
-      <c r="J44" s="69" t="s">
+      <c r="J44" s="68" t="s">
         <v>15</v>
       </c>
       <c r="K44" s="54"/>
       <c r="L44" s="54"/>
-      <c r="M44" s="75" t="str">
-        <f t="shared" si="41"/>
+      <c r="M44" s="74" t="str">
+        <f t="shared" si="42"/>
         <v>52:##################################################,</v>
       </c>
-      <c r="N44" s="67" t="str">
-        <f t="shared" si="42"/>
+      <c r="N44" s="66" t="str">
+        <f t="shared" si="43"/>
         <v>52:NoticeWord (Notifications),</v>
       </c>
-      <c r="O44" s="71" t="s">
+      <c r="O44" s="70" t="s">
         <v>22</v>
       </c>
       <c r="P44" s="56"/>
@@ -7505,12 +7677,12 @@
         <v>1</v>
       </c>
       <c r="X44" s="59" t="str">
-        <f t="shared" si="45"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <f t="shared" si="46"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="Y44" s="59" t="str">
-        <f t="shared" si="40"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <f t="shared" si="41"/>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
       <c r="Z44" s="60" t="str">
         <f t="shared" si="26"/>
@@ -7525,11 +7697,11 @@
       </c>
       <c r="AC44" s="60" t="str">
         <f t="shared" si="28"/>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="AD44" s="60" t="str">
         <f t="shared" si="29"/>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
       <c r="AE44" s="61" t="str">
         <f t="shared" si="30"/>
@@ -7544,11 +7716,11 @@
       </c>
       <c r="AH44" s="61" t="str">
         <f t="shared" si="32"/>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="AI44" s="61" t="str">
         <f t="shared" si="33"/>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
       <c r="AJ44" s="51" t="str">
         <f t="shared" si="34"/>
@@ -7611,7 +7783,7 @@
     <row r="47" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F47" s="41" t="str">
         <f>+Y44</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,27:,,28:,,29:,,30:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,30:,,31:,,32:,,</v>
       </c>
     </row>
     <row r="48" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7620,14 +7792,14 @@
       </c>
       <c r="F48" s="27" t="str">
         <f>X44</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,27:,28:,29:,30:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,30:,31:,32:,</v>
       </c>
       <c r="G48" s="27"/>
     </row>
     <row r="49" spans="6:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F49" s="28">
         <f>LEN(F48)</f>
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="H49" s="26" t="str">
         <f>Z44</f>
@@ -7655,16 +7827,16 @@
       <c r="H53" s="43"/>
       <c r="K53" s="37" t="str">
         <f>+AD44</f>
-        <v>11:#,Everything Enable,12:#,Sound Enable,13:#,Light Enable,14:#,Motion Enable,15:#,Clock Enable,16:####,Room Light Sensor Trigger Value,17:##,Performance number,18:#,Light Pinky,19:#,Light Clyde,20:#,Light Cherry,21:#,Light PacMan,22:#,Light Blinky,23:#,Light Inky,24:,,25:,,26:,,31:,,32:,,</v>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Alarm Time,17:#,Performance number,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,31:,,32:,,</v>
       </c>
     </row>
     <row r="54" spans="6:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>AC44</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:####,17:##,18:#,19:#,20:#,21:#,22:#,23:#,24:,25:,26:,31:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:####,24:#,25:#,26:#,27:######,28:######,29:##,31:,32:,</v>
       </c>
       <c r="L54" s="24"/>
       <c r="R54" s="8"/>
@@ -7677,7 +7849,7 @@
       </c>
       <c r="K55" s="25">
         <f>LEN(K54)</f>
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="23" t="str">
@@ -7707,20 +7879,20 @@
     <row r="59" spans="6:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P59" s="18" t="str">
         <f>+AI44</f>
-        <v>23:#,Light Inky,24:,,25:,,26:,,32:,,</v>
+        <v>23:####,Light Sensor trigger value,24:#,Night Light Enable,25:#,Location (SF=1, Brkgs=2) (ip address),26:#,Alarm Enable,27:######,Alarm Date,28:######,Alarm Time,29:##,Performance number,32:,,</v>
       </c>
     </row>
     <row r="60" spans="6:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P60" s="17" t="str">
         <f>AH44</f>
-        <v>&gt;&gt;&gt;&gt;&gt;23:#,24:,25:,26:,32:,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;23:####,24:#,25:#,26:#,27:######,28:######,29:##,32:,</v>
       </c>
       <c r="Q60" s="17"/>
     </row>
     <row r="61" spans="6:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P61" s="16">
         <f>LEN(P60)</f>
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="Q61" s="16"/>
       <c r="R61" s="19" t="str">

</xml_diff>

<commit_message>
many variables to receive and report back set up.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265"/>
   </bookViews>
   <sheets>
-    <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId1"/>
-    <sheet name="TABLE" sheetId="1" r:id="rId2"/>
-    <sheet name="StayinAliveComms" sheetId="3" r:id="rId3"/>
+    <sheet name="COMBINED" sheetId="5" r:id="rId1"/>
+    <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId2"/>
+    <sheet name="TABLE" sheetId="1" r:id="rId3"/>
+    <sheet name="StayinAliveComms" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="113">
   <si>
     <t>App use only</t>
   </si>
@@ -458,6 +458,54 @@
   </si>
   <si>
     <t>Attack_or_Donate Clyde</t>
+  </si>
+  <si>
+    <t>Night Light Enable and mode</t>
+  </si>
+  <si>
+    <t>9####</t>
+  </si>
+  <si>
+    <t>#######</t>
+  </si>
+  <si>
+    <t>Mirror_Balances_Pinky_Values</t>
+  </si>
+  <si>
+    <t>Mirror_Balances_Clyde_Values</t>
+  </si>
+  <si>
+    <t>Mirror_Balances_Cherry_Values</t>
+  </si>
+  <si>
+    <t>Mirror_Balances_Pacman_Values</t>
+  </si>
+  <si>
+    <t>Mirror_Balances_Blinky_Values</t>
+  </si>
+  <si>
+    <t>Mirror_Balances_Inky_Values</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate_Flag (Pinky-Inky)</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate Pinky_Amnt</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate Clyde_Amnt</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate Cherry_Amnt</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate PacMan_Amnt</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate Blinky_Amnt</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate Inky_Amnt</t>
   </si>
 </sst>
 </file>
@@ -2621,6 +2669,1315 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor theme="8" tint="0.39997558519241921"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:H54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="7" max="8" width="29.28515625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="7"/>
+      <c r="D2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="59" t="str">
+        <f>CONCATENATE(G1,E2)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;</v>
+      </c>
+      <c r="H2" s="59" t="str">
+        <f>CONCATENATE(H1,F2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75">
+        <v>1</v>
+      </c>
+      <c r="B3" s="75">
+        <v>11</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="79" t="str">
+        <f t="shared" ref="E3:E41" si="0">CONCATENATE($B3,":",$C3,",")</f>
+        <v>11:#,</v>
+      </c>
+      <c r="F3" s="80" t="str">
+        <f>CONCATENATE($E3,$D3,",")</f>
+        <v>11:#,Master Enable,</v>
+      </c>
+      <c r="G3" s="59" t="str">
+        <f>CONCATENATE(G2,E3)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,</v>
+      </c>
+      <c r="H3" s="59" t="str">
+        <f>CONCATENATE(H2,F3)</f>
+        <v>11:#,Master Enable,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75">
+        <v>2</v>
+      </c>
+      <c r="B4" s="75">
+        <v>12</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>12:#,</v>
+      </c>
+      <c r="F4" s="80" t="str">
+        <f>CONCATENATE($E4,$D4,",")</f>
+        <v>12:#,Light Enable,</v>
+      </c>
+      <c r="G4" s="59" t="str">
+        <f>CONCATENATE(G3,E4)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,</v>
+      </c>
+      <c r="H4" s="59" t="str">
+        <f>CONCATENATE(H3,F4)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="75">
+        <v>3</v>
+      </c>
+      <c r="B5" s="75">
+        <v>13</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>13:#,</v>
+      </c>
+      <c r="F5" s="80" t="str">
+        <f>CONCATENATE($E5,$D5,",")</f>
+        <v>13:#,Sound Enable,</v>
+      </c>
+      <c r="G5" s="59" t="str">
+        <f>CONCATENATE(G4,E5)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,</v>
+      </c>
+      <c r="H5" s="59" t="str">
+        <f>CONCATENATE(H4,F5)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
+        <v>4</v>
+      </c>
+      <c r="B6" s="75">
+        <v>14</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>14:#,</v>
+      </c>
+      <c r="F6" s="80" t="str">
+        <f>CONCATENATE($E6,$D6,",")</f>
+        <v>14:#,Motion Enable,</v>
+      </c>
+      <c r="G6" s="59" t="str">
+        <f>CONCATENATE(G5,E6)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,</v>
+      </c>
+      <c r="H6" s="59" t="str">
+        <f>CONCATENATE(H5,F6)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="75">
+        <v>5</v>
+      </c>
+      <c r="B7" s="75">
+        <v>15</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>15:#,</v>
+      </c>
+      <c r="F7" s="80" t="str">
+        <f>CONCATENATE($E7,$D7,",")</f>
+        <v>15:#,Clock Enable,</v>
+      </c>
+      <c r="G7" s="59" t="str">
+        <f>CONCATENATE(G6,E7)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,</v>
+      </c>
+      <c r="H7" s="59" t="str">
+        <f>CONCATENATE(H6,F7)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="75">
+        <v>6</v>
+      </c>
+      <c r="B8" s="75">
+        <v>16</v>
+      </c>
+      <c r="C8" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>16:#,</v>
+      </c>
+      <c r="F8" s="80" t="str">
+        <f t="shared" ref="F8:F41" si="1">CONCATENATE($E8,$D8,",")</f>
+        <v>16:#,Light Pinky,</v>
+      </c>
+      <c r="G8" s="59" t="str">
+        <f>CONCATENATE(G7,E8)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,</v>
+      </c>
+      <c r="H8" s="59" t="str">
+        <f>CONCATENATE(H7,F8)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="75">
+        <v>7</v>
+      </c>
+      <c r="B9" s="75">
+        <v>17</v>
+      </c>
+      <c r="C9" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>17:#,</v>
+      </c>
+      <c r="F9" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>17:#,Light Clyde,</v>
+      </c>
+      <c r="G9" s="59" t="str">
+        <f>CONCATENATE(G8,E9)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,</v>
+      </c>
+      <c r="H9" s="59" t="str">
+        <f>CONCATENATE(H8,F9)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="75">
+        <v>8</v>
+      </c>
+      <c r="B10" s="75">
+        <v>18</v>
+      </c>
+      <c r="C10" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>18:#,</v>
+      </c>
+      <c r="F10" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>18:#,Light Cherry,</v>
+      </c>
+      <c r="G10" s="59" t="str">
+        <f>CONCATENATE(G9,E10)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,</v>
+      </c>
+      <c r="H10" s="59" t="str">
+        <f>CONCATENATE(H9,F10)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="75">
+        <v>9</v>
+      </c>
+      <c r="B11" s="75">
+        <v>19</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>19:#,</v>
+      </c>
+      <c r="F11" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>19:#,Light PacMan,</v>
+      </c>
+      <c r="G11" s="59" t="str">
+        <f>CONCATENATE(G10,E11)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,</v>
+      </c>
+      <c r="H11" s="59" t="str">
+        <f>CONCATENATE(H10,F11)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="75">
+        <v>10</v>
+      </c>
+      <c r="B12" s="75">
+        <v>20</v>
+      </c>
+      <c r="C12" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>20:#,</v>
+      </c>
+      <c r="F12" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>20:#,Light Blinky,</v>
+      </c>
+      <c r="G12" s="59" t="str">
+        <f>CONCATENATE(G11,E12)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,</v>
+      </c>
+      <c r="H12" s="59" t="str">
+        <f>CONCATENATE(H11,F12)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="75">
+        <v>11</v>
+      </c>
+      <c r="B13" s="75">
+        <v>21</v>
+      </c>
+      <c r="C13" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>21:#,</v>
+      </c>
+      <c r="F13" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>21:#,Light Inky,</v>
+      </c>
+      <c r="G13" s="59" t="str">
+        <f>CONCATENATE(G12,E13)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,</v>
+      </c>
+      <c r="H13" s="59" t="str">
+        <f>CONCATENATE(H12,F13)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="75">
+        <v>12</v>
+      </c>
+      <c r="B14" s="75">
+        <v>22</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>22:#,</v>
+      </c>
+      <c r="F14" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>22:#,Light Sensor Enable,</v>
+      </c>
+      <c r="G14" s="59" t="str">
+        <f>CONCATENATE(G13,E14)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,</v>
+      </c>
+      <c r="H14" s="59" t="str">
+        <f>CONCATENATE(H13,F14)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="75">
+        <v>13</v>
+      </c>
+      <c r="B15" s="75">
+        <v>23</v>
+      </c>
+      <c r="C15" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>23:9####,</v>
+      </c>
+      <c r="F15" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>23:9####,Light Sensor trigger value,</v>
+      </c>
+      <c r="G15" s="59" t="str">
+        <f>CONCATENATE(G14,E15)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,</v>
+      </c>
+      <c r="H15" s="59" t="str">
+        <f>CONCATENATE(H14,F15)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="75">
+        <v>14</v>
+      </c>
+      <c r="B16" s="75">
+        <v>24</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>24:#,</v>
+      </c>
+      <c r="F16" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>24:#,Night Light Enable and mode,</v>
+      </c>
+      <c r="G16" s="59" t="str">
+        <f>CONCATENATE(G15,E16)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,</v>
+      </c>
+      <c r="H16" s="59" t="str">
+        <f>CONCATENATE(H15,F16)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="75">
+        <v>15</v>
+      </c>
+      <c r="B17" s="75">
+        <v>25</v>
+      </c>
+      <c r="C17" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>25:#,</v>
+      </c>
+      <c r="F17" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>25:#,(ip address preset),</v>
+      </c>
+      <c r="G17" s="59" t="str">
+        <f>CONCATENATE(G16,E17)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,</v>
+      </c>
+      <c r="H17" s="59" t="str">
+        <f>CONCATENATE(H16,F17)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="75">
+        <v>16</v>
+      </c>
+      <c r="B18" s="75">
+        <v>26</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>26:#,</v>
+      </c>
+      <c r="F18" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>26:#,Alarm Enable,</v>
+      </c>
+      <c r="G18" s="59" t="str">
+        <f>CONCATENATE(G17,E18)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,</v>
+      </c>
+      <c r="H18" s="59" t="str">
+        <f>CONCATENATE(H17,F18)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="75">
+        <v>17</v>
+      </c>
+      <c r="B19" s="75">
+        <v>27</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>27:9######,</v>
+      </c>
+      <c r="F19" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>27:9######,Alarm Date,</v>
+      </c>
+      <c r="G19" s="59" t="str">
+        <f>CONCATENATE(G18,E19)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,</v>
+      </c>
+      <c r="H19" s="59" t="str">
+        <f>CONCATENATE(H18,F19)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="75">
+        <v>18</v>
+      </c>
+      <c r="B20" s="75">
+        <v>28</v>
+      </c>
+      <c r="C20" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>28:9######,</v>
+      </c>
+      <c r="F20" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>28:9######,Alarm Time,</v>
+      </c>
+      <c r="G20" s="59" t="str">
+        <f>CONCATENATE(G19,E20)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,</v>
+      </c>
+      <c r="H20" s="59" t="str">
+        <f>CONCATENATE(H19,F20)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="75">
+        <v>19</v>
+      </c>
+      <c r="B21" s="75">
+        <v>29</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>29:##,</v>
+      </c>
+      <c r="F21" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>29:##,Performance number,</v>
+      </c>
+      <c r="G21" s="59" t="str">
+        <f>CONCATENATE(G20,E21)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,</v>
+      </c>
+      <c r="H21" s="59" t="str">
+        <f>CONCATENATE(H20,F21)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="75">
+        <v>20</v>
+      </c>
+      <c r="B22" s="75">
+        <v>41</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="77" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>41:#,</v>
+      </c>
+      <c r="F22" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>41:#,Stayin_Game_Status (0,1 = not,ingame),</v>
+      </c>
+      <c r="G22" s="59" t="str">
+        <f>CONCATENATE(G21,E22)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,</v>
+      </c>
+      <c r="H22" s="59" t="str">
+        <f>CONCATENATE(H21,F22)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="75">
+        <v>21</v>
+      </c>
+      <c r="B23" s="75">
+        <v>42</v>
+      </c>
+      <c r="C23" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>42:#,</v>
+      </c>
+      <c r="F23" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>42:#,myCharNum (1, 2, 3, 4, 5, or 6),</v>
+      </c>
+      <c r="G23" s="59" t="str">
+        <f>CONCATENATE(G22,E23)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,</v>
+      </c>
+      <c r="H23" s="59" t="str">
+        <f>CONCATENATE(H22,F23)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="75">
+        <v>22</v>
+      </c>
+      <c r="B24" s="75">
+        <v>43</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>43:#######,</v>
+      </c>
+      <c r="F24" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>43:#######,ActualName,</v>
+      </c>
+      <c r="G24" s="59" t="str">
+        <f>CONCATENATE(G23,E24)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,</v>
+      </c>
+      <c r="H24" s="59" t="str">
+        <f>CONCATENATE(H23,F24)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="75">
+        <v>23</v>
+      </c>
+      <c r="B25" s="75">
+        <v>44</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>44:###,</v>
+      </c>
+      <c r="F25" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>44:###,BankAfterSpend,</v>
+      </c>
+      <c r="G25" s="22" t="str">
+        <f>CONCATENATE(G24,E25)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,</v>
+      </c>
+      <c r="H25" s="22" t="str">
+        <f>CONCATENATE(H24,F25)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="75">
+        <v>24</v>
+      </c>
+      <c r="B26" s="75">
+        <v>45</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>45:###,</v>
+      </c>
+      <c r="F26" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>45:###,Attack_balance,</v>
+      </c>
+      <c r="G26" s="59" t="str">
+        <f>CONCATENATE(G25,E26)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,</v>
+      </c>
+      <c r="H26" s="59" t="str">
+        <f>CONCATENATE(H25,F26)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="75">
+        <v>25</v>
+      </c>
+      <c r="B27" s="75">
+        <v>46</v>
+      </c>
+      <c r="C27" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>46:9######,</v>
+      </c>
+      <c r="F27" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>46:9######,Attack_or_Donate_Flag (Pinky-Inky),</v>
+      </c>
+      <c r="G27" s="59" t="str">
+        <f>CONCATENATE(G26,E27)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,</v>
+      </c>
+      <c r="H27" s="59" t="str">
+        <f>CONCATENATE(H26,F27)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="75">
+        <v>26</v>
+      </c>
+      <c r="B28" s="75">
+        <v>47</v>
+      </c>
+      <c r="C28" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>47:9######,</v>
+      </c>
+      <c r="F28" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>47:9######,Will_or_No (Pinky-Inky),</v>
+      </c>
+      <c r="G28" s="59" t="str">
+        <f>CONCATENATE(G27,E28)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,</v>
+      </c>
+      <c r="H28" s="59" t="str">
+        <f>CONCATENATE(H27,F28)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="75">
+        <v>27</v>
+      </c>
+      <c r="B29" s="75">
+        <v>48</v>
+      </c>
+      <c r="C29" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>48:9######,</v>
+      </c>
+      <c r="F29" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>48:9######,Mirror_or_No (Pinky-Inky),</v>
+      </c>
+      <c r="G29" s="59" t="str">
+        <f>CONCATENATE(G28,E29)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,</v>
+      </c>
+      <c r="H29" s="59" t="str">
+        <f>CONCATENATE(H28,F29)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="75">
+        <v>28</v>
+      </c>
+      <c r="B30" s="75">
+        <v>49</v>
+      </c>
+      <c r="C30" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>49:###,</v>
+      </c>
+      <c r="F30" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>49:###,Attack_or_Donate Pinky_Amnt,</v>
+      </c>
+      <c r="G30" s="59" t="str">
+        <f>CONCATENATE(G29,E30)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,</v>
+      </c>
+      <c r="H30" s="59" t="str">
+        <f>CONCATENATE(H29,F30)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="75">
+        <v>29</v>
+      </c>
+      <c r="B31" s="75">
+        <v>50</v>
+      </c>
+      <c r="C31" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>50:###,</v>
+      </c>
+      <c r="F31" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>50:###,Attack_or_Donate Clyde_Amnt,</v>
+      </c>
+      <c r="G31" s="59" t="str">
+        <f>CONCATENATE(G30,E31)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,</v>
+      </c>
+      <c r="H31" s="59" t="str">
+        <f>CONCATENATE(H30,F31)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="75">
+        <v>30</v>
+      </c>
+      <c r="B32" s="75">
+        <v>51</v>
+      </c>
+      <c r="C32" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>51:###,</v>
+      </c>
+      <c r="F32" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>51:###,Attack_or_Donate Cherry_Amnt,</v>
+      </c>
+      <c r="G32" s="59" t="str">
+        <f>CONCATENATE(G31,E32)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,</v>
+      </c>
+      <c r="H32" s="59" t="str">
+        <f>CONCATENATE(H31,F32)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="75">
+        <v>31</v>
+      </c>
+      <c r="B33" s="75">
+        <v>52</v>
+      </c>
+      <c r="C33" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>52:###,</v>
+      </c>
+      <c r="F33" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>52:###,Attack_or_Donate PacMan_Amnt,</v>
+      </c>
+      <c r="G33" s="59" t="str">
+        <f>CONCATENATE(G32,E33)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,</v>
+      </c>
+      <c r="H33" s="59" t="str">
+        <f>CONCATENATE(H32,F33)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="75">
+        <v>32</v>
+      </c>
+      <c r="B34" s="75">
+        <v>53</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>53:###,</v>
+      </c>
+      <c r="F34" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>53:###,Attack_or_Donate Blinky_Amnt,</v>
+      </c>
+      <c r="G34" s="59" t="str">
+        <f>CONCATENATE(G33,E34)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,</v>
+      </c>
+      <c r="H34" s="59" t="str">
+        <f>CONCATENATE(H33,F34)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="75">
+        <v>33</v>
+      </c>
+      <c r="B35" s="75">
+        <v>54</v>
+      </c>
+      <c r="C35" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>54:###,</v>
+      </c>
+      <c r="F35" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>54:###,Attack_or_Donate Inky_Amnt,</v>
+      </c>
+      <c r="G35" s="59" t="str">
+        <f>CONCATENATE(G34,E35)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,</v>
+      </c>
+      <c r="H35" s="59" t="str">
+        <f>CONCATENATE(H34,F35)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="75">
+        <v>34</v>
+      </c>
+      <c r="B36" s="75">
+        <v>55</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="77" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>55:9######,</v>
+      </c>
+      <c r="F36" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>55:9######,Mirror_Balances_Pinky_Values,</v>
+      </c>
+      <c r="G36" s="59" t="str">
+        <f>CONCATENATE(G35,E36)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,</v>
+      </c>
+      <c r="H36" s="59" t="str">
+        <f>CONCATENATE(H35,F36)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="75">
+        <v>35</v>
+      </c>
+      <c r="B37" s="75">
+        <v>56</v>
+      </c>
+      <c r="C37" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>56:9######,</v>
+      </c>
+      <c r="F37" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>56:9######,Mirror_Balances_Clyde_Values,</v>
+      </c>
+      <c r="G37" s="59" t="str">
+        <f>CONCATENATE(G36,E37)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,</v>
+      </c>
+      <c r="H37" s="59" t="str">
+        <f>CONCATENATE(H36,F37)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="75">
+        <v>36</v>
+      </c>
+      <c r="B38" s="75">
+        <v>57</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>57:9######,</v>
+      </c>
+      <c r="F38" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>57:9######,Mirror_Balances_Cherry_Values,</v>
+      </c>
+      <c r="G38" s="59" t="str">
+        <f>CONCATENATE(G37,E38)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,</v>
+      </c>
+      <c r="H38" s="59" t="str">
+        <f>CONCATENATE(H37,F38)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="75"/>
+      <c r="B39" s="75">
+        <v>58</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>58:9######,</v>
+      </c>
+      <c r="F39" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>58:9######,Mirror_Balances_Pacman_Values,</v>
+      </c>
+      <c r="G39" s="59" t="str">
+        <f>CONCATENATE(G38,E39)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,</v>
+      </c>
+      <c r="H39" s="59" t="str">
+        <f>CONCATENATE(H38,F39)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="75"/>
+      <c r="B40" s="75">
+        <v>59</v>
+      </c>
+      <c r="C40" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>59:9######,</v>
+      </c>
+      <c r="F40" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>59:9######,Mirror_Balances_Blinky_Values,</v>
+      </c>
+      <c r="G40" s="59" t="str">
+        <f>CONCATENATE(G39,E40)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,</v>
+      </c>
+      <c r="H40" s="59" t="str">
+        <f>CONCATENATE(H39,F40)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="75"/>
+      <c r="B41" s="75">
+        <v>60</v>
+      </c>
+      <c r="C41" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>60:9######,</v>
+      </c>
+      <c r="F41" s="80" t="str">
+        <f t="shared" si="1"/>
+        <v>60:9######,Mirror_Balances_Inky_Values,</v>
+      </c>
+      <c r="G41" s="59" t="str">
+        <f>CONCATENATE(G40,E41)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+      </c>
+      <c r="H41" s="59" t="str">
+        <f>CONCATENATE(H40,F41)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="75"/>
+      <c r="B42" s="75">
+        <v>61</v>
+      </c>
+      <c r="C42" s="76"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="59" t="str">
+        <f>CONCATENATE(G41,E42)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+      </c>
+      <c r="H42" s="59" t="str">
+        <f>CONCATENATE(H41,F42)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="75"/>
+      <c r="B43" s="75">
+        <v>62</v>
+      </c>
+      <c r="C43" s="76"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="59" t="str">
+        <f>CONCATENATE(G42,E43)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+      </c>
+      <c r="H43" s="59" t="str">
+        <f>CONCATENATE(H42,F43)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="75"/>
+      <c r="B44" s="75">
+        <v>63</v>
+      </c>
+      <c r="C44" s="76"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="59" t="str">
+        <f>CONCATENATE(G43,E44)</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+      </c>
+      <c r="H44" s="59" t="str">
+        <f>CONCATENATE(H43,F44)</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="38"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="38"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="41" t="str">
+        <f>+H44</f>
+        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="27" t="str">
+        <f>G44</f>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+      </c>
+      <c r="F48" s="27"/>
+    </row>
+    <row r="50" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G50"/>
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51"/>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G52"/>
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G53"/>
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="7:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G54"/>
+      <c r="H54"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup scale="63" fitToWidth="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A3:A34"/>
@@ -2699,7 +4056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -2708,7 +4065,7 @@
   <dimension ref="A2:BC63"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:XFD1048576"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7971,12 +9328,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BC82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B20"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9122,7 +10479,7 @@
     </row>
     <row r="11" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="75">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="75">
         <v>49</v>
@@ -9246,7 +10603,7 @@
     </row>
     <row r="12" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="75">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="75">
         <v>50</v>
@@ -9370,7 +10727,7 @@
     </row>
     <row r="13" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="75">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="75">
         <v>51</v>
@@ -9494,7 +10851,7 @@
     </row>
     <row r="14" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="75">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="75">
         <v>52</v>
@@ -9616,7 +10973,7 @@
     </row>
     <row r="15" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="75">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="75">
         <v>53</v>
@@ -9740,7 +11097,7 @@
     </row>
     <row r="16" spans="1:55" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="75">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B16" s="75">
         <v>54</v>

</xml_diff>

<commit_message>
More status made towards reading and interpreting Android message.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="COMBINED" sheetId="5" r:id="rId1"/>
-    <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId2"/>
-    <sheet name="TABLE" sheetId="1" r:id="rId3"/>
-    <sheet name="StayinAliveComms" sheetId="3" r:id="rId4"/>
+    <sheet name="MESSAGE_PART_LENGTH" sheetId="6" r:id="rId2"/>
+    <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId3"/>
+    <sheet name="TABLE" sheetId="1" r:id="rId4"/>
+    <sheet name="StayinAliveComms" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="140">
   <si>
     <t>App use only</t>
   </si>
@@ -460,9 +461,6 @@
     <t>Attack_or_Donate Clyde</t>
   </si>
   <si>
-    <t>Night Light Enable and mode</t>
-  </si>
-  <si>
     <t>9####</t>
   </si>
   <si>
@@ -487,9 +485,6 @@
     <t>Mirror_Balances_Inky_Values</t>
   </si>
   <si>
-    <t>Attack_or_Donate_Flag (Pinky-Inky)</t>
-  </si>
-  <si>
     <t>Attack_or_Donate Pinky_Amnt</t>
   </si>
   <si>
@@ -507,12 +502,99 @@
   <si>
     <t>Attack_or_Donate Inky_Amnt</t>
   </si>
+  <si>
+    <t>MESSAGE_PART_LENGTH[</t>
+  </si>
+  <si>
+    <t>;  //</t>
+  </si>
+  <si>
+    <t xml:space="preserve">]= </t>
+  </si>
+  <si>
+    <t>9########</t>
+  </si>
+  <si>
+    <t>9###</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Master_Enable</t>
+  </si>
+  <si>
+    <t>Light_Enable</t>
+  </si>
+  <si>
+    <t>Sound_Enable</t>
+  </si>
+  <si>
+    <t>Motion_Enable</t>
+  </si>
+  <si>
+    <t>Clock_Enable</t>
+  </si>
+  <si>
+    <t>Light_Pinky</t>
+  </si>
+  <si>
+    <t>Light_Clyde</t>
+  </si>
+  <si>
+    <t>Light_Cherry</t>
+  </si>
+  <si>
+    <t>Light_PacMan</t>
+  </si>
+  <si>
+    <t>Light_Blinky</t>
+  </si>
+  <si>
+    <t>Light_Inky</t>
+  </si>
+  <si>
+    <t>Light_Sensor_Enable</t>
+  </si>
+  <si>
+    <t>Light_Sensor_trigger_value</t>
+  </si>
+  <si>
+    <t>Night_Light_Enable_and_mode</t>
+  </si>
+  <si>
+    <t>Alarm_Enable</t>
+  </si>
+  <si>
+    <t>Alarm_Date</t>
+  </si>
+  <si>
+    <t>Alarm_Time</t>
+  </si>
+  <si>
+    <t>Performance_number</t>
+  </si>
+  <si>
+    <t>Stayin_Game_Status</t>
+  </si>
+  <si>
+    <t>myCharNum</t>
+  </si>
+  <si>
+    <t>Attack_or_Donate_Flag</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,6 +798,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -879,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1067,6 +1157,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2674,14 +2765,14 @@
   </sheetPr>
   <dimension ref="A2:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="50" customWidth="1"/>
@@ -2698,11 +2789,11 @@
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="59" t="str">
-        <f>CONCATENATE(G1,E2)</f>
+        <f t="shared" ref="G2:G44" si="0">CONCATENATE(G1,E2)</f>
         <v>&gt;&gt;&gt;&gt;&gt;</v>
       </c>
       <c r="H2" s="59" t="str">
-        <f>CONCATENATE(H1,F2)</f>
+        <f t="shared" ref="H2:H44" si="1">CONCATENATE(H1,F2)</f>
         <v/>
       </c>
     </row>
@@ -2717,23 +2808,23 @@
         <v>33</v>
       </c>
       <c r="D3" s="77" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="E3" s="79" t="str">
-        <f t="shared" ref="E3:E41" si="0">CONCATENATE($B3,":",$C3,",")</f>
+        <f t="shared" ref="E3:E41" si="2">CONCATENATE($B3,":",$C3,",")</f>
         <v>11:#,</v>
       </c>
       <c r="F3" s="80" t="str">
         <f>CONCATENATE($E3,$D3,",")</f>
-        <v>11:#,Master Enable,</v>
+        <v>11:#,Master_Enable,</v>
       </c>
       <c r="G3" s="59" t="str">
-        <f>CONCATENATE(G2,E3)</f>
+        <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,</v>
       </c>
       <c r="H3" s="59" t="str">
-        <f>CONCATENATE(H2,F3)</f>
-        <v>11:#,Master Enable,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2747,23 +2838,23 @@
         <v>33</v>
       </c>
       <c r="D4" s="77" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="E4" s="79" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12:#,</v>
       </c>
       <c r="F4" s="80" t="str">
         <f>CONCATENATE($E4,$D4,",")</f>
-        <v>12:#,Light Enable,</v>
+        <v>12:#,Light_Enable,</v>
       </c>
       <c r="G4" s="59" t="str">
-        <f>CONCATENATE(G3,E4)</f>
+        <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,</v>
       </c>
       <c r="H4" s="59" t="str">
-        <f>CONCATENATE(H3,F4)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2777,23 +2868,23 @@
         <v>33</v>
       </c>
       <c r="D5" s="77" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="E5" s="79" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13:#,</v>
       </c>
       <c r="F5" s="80" t="str">
         <f>CONCATENATE($E5,$D5,",")</f>
-        <v>13:#,Sound Enable,</v>
+        <v>13:#,Sound_Enable,</v>
       </c>
       <c r="G5" s="59" t="str">
-        <f>CONCATENATE(G4,E5)</f>
+        <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,</v>
       </c>
       <c r="H5" s="59" t="str">
-        <f>CONCATENATE(H4,F5)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2807,23 +2898,23 @@
         <v>33</v>
       </c>
       <c r="D6" s="77" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="E6" s="79" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>14:#,</v>
       </c>
       <c r="F6" s="80" t="str">
         <f>CONCATENATE($E6,$D6,",")</f>
-        <v>14:#,Motion Enable,</v>
+        <v>14:#,Motion_Enable,</v>
       </c>
       <c r="G6" s="59" t="str">
-        <f>CONCATENATE(G5,E6)</f>
+        <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,</v>
       </c>
       <c r="H6" s="59" t="str">
-        <f>CONCATENATE(H5,F6)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2837,23 +2928,23 @@
         <v>33</v>
       </c>
       <c r="D7" s="77" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="E7" s="79" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15:#,</v>
       </c>
       <c r="F7" s="80" t="str">
         <f>CONCATENATE($E7,$D7,",")</f>
-        <v>15:#,Clock Enable,</v>
+        <v>15:#,Clock_Enable,</v>
       </c>
       <c r="G7" s="59" t="str">
-        <f>CONCATENATE(G6,E7)</f>
+        <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,</v>
       </c>
       <c r="H7" s="59" t="str">
-        <f>CONCATENATE(H6,F7)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2867,23 +2958,23 @@
         <v>33</v>
       </c>
       <c r="D8" s="77" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="E8" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>16:#,</v>
+      </c>
+      <c r="F8" s="80" t="str">
+        <f t="shared" ref="F8:F41" si="3">CONCATENATE($E8,$D8,",")</f>
+        <v>16:#,Light_Pinky,</v>
+      </c>
+      <c r="G8" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>16:#,</v>
-      </c>
-      <c r="F8" s="80" t="str">
-        <f t="shared" ref="F8:F41" si="1">CONCATENATE($E8,$D8,",")</f>
-        <v>16:#,Light Pinky,</v>
-      </c>
-      <c r="G8" s="59" t="str">
-        <f>CONCATENATE(G7,E8)</f>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,</v>
       </c>
       <c r="H8" s="59" t="str">
-        <f>CONCATENATE(H7,F8)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2897,23 +2988,23 @@
         <v>33</v>
       </c>
       <c r="D9" s="77" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="E9" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>17:#,</v>
+      </c>
+      <c r="F9" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>17:#,Light_Clyde,</v>
+      </c>
+      <c r="G9" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>17:#,</v>
-      </c>
-      <c r="F9" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,</v>
+      </c>
+      <c r="H9" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>17:#,Light Clyde,</v>
-      </c>
-      <c r="G9" s="59" t="str">
-        <f>CONCATENATE(G8,E9)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,</v>
-      </c>
-      <c r="H9" s="59" t="str">
-        <f>CONCATENATE(H8,F9)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2927,23 +3018,23 @@
         <v>33</v>
       </c>
       <c r="D10" s="77" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="E10" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>18:#,</v>
+      </c>
+      <c r="F10" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>18:#,Light_Cherry,</v>
+      </c>
+      <c r="G10" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>18:#,</v>
-      </c>
-      <c r="F10" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,</v>
+      </c>
+      <c r="H10" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>18:#,Light Cherry,</v>
-      </c>
-      <c r="G10" s="59" t="str">
-        <f>CONCATENATE(G9,E10)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,</v>
-      </c>
-      <c r="H10" s="59" t="str">
-        <f>CONCATENATE(H9,F10)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2957,23 +3048,23 @@
         <v>33</v>
       </c>
       <c r="D11" s="77" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="E11" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>19:#,</v>
+      </c>
+      <c r="F11" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>19:#,Light_PacMan,</v>
+      </c>
+      <c r="G11" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>19:#,</v>
-      </c>
-      <c r="F11" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,</v>
+      </c>
+      <c r="H11" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>19:#,Light PacMan,</v>
-      </c>
-      <c r="G11" s="59" t="str">
-        <f>CONCATENATE(G10,E11)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,</v>
-      </c>
-      <c r="H11" s="59" t="str">
-        <f>CONCATENATE(H10,F11)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2987,23 +3078,23 @@
         <v>33</v>
       </c>
       <c r="D12" s="77" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="E12" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>20:#,</v>
+      </c>
+      <c r="F12" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>20:#,Light_Blinky,</v>
+      </c>
+      <c r="G12" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>20:#,</v>
-      </c>
-      <c r="F12" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,</v>
+      </c>
+      <c r="H12" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>20:#,Light Blinky,</v>
-      </c>
-      <c r="G12" s="59" t="str">
-        <f>CONCATENATE(G11,E12)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,</v>
-      </c>
-      <c r="H12" s="59" t="str">
-        <f>CONCATENATE(H11,F12)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3017,23 +3108,23 @@
         <v>33</v>
       </c>
       <c r="D13" s="77" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="E13" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>21:#,</v>
+      </c>
+      <c r="F13" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>21:#,Light_Inky,</v>
+      </c>
+      <c r="G13" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>21:#,</v>
-      </c>
-      <c r="F13" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,</v>
+      </c>
+      <c r="H13" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>21:#,Light Inky,</v>
-      </c>
-      <c r="G13" s="59" t="str">
-        <f>CONCATENATE(G12,E13)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,</v>
-      </c>
-      <c r="H13" s="59" t="str">
-        <f>CONCATENATE(H12,F13)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3047,23 +3138,23 @@
         <v>33</v>
       </c>
       <c r="D14" s="77" t="s">
-        <v>78</v>
+        <v>128</v>
       </c>
       <c r="E14" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>22:#,</v>
+      </c>
+      <c r="F14" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>22:#,Light_Sensor_Enable,</v>
+      </c>
+      <c r="G14" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>22:#,</v>
-      </c>
-      <c r="F14" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,</v>
+      </c>
+      <c r="H14" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>22:#,Light Sensor Enable,</v>
-      </c>
-      <c r="G14" s="59" t="str">
-        <f>CONCATENATE(G13,E14)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,</v>
-      </c>
-      <c r="H14" s="59" t="str">
-        <f>CONCATENATE(H13,F14)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3074,26 +3165,26 @@
         <v>23</v>
       </c>
       <c r="C15" s="76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="77" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="E15" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>23:9####,</v>
+      </c>
+      <c r="F15" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>23:9####,Light_Sensor_trigger_value,</v>
+      </c>
+      <c r="G15" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>23:9####,</v>
-      </c>
-      <c r="F15" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,</v>
+      </c>
+      <c r="H15" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>23:9####,Light Sensor trigger value,</v>
-      </c>
-      <c r="G15" s="59" t="str">
-        <f>CONCATENATE(G14,E15)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,</v>
-      </c>
-      <c r="H15" s="59" t="str">
-        <f>CONCATENATE(H14,F15)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3107,23 +3198,23 @@
         <v>33</v>
       </c>
       <c r="D16" s="77" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="E16" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>24:#,</v>
+      </c>
+      <c r="F16" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>24:#,Night_Light_Enable_and_mode,</v>
+      </c>
+      <c r="G16" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>24:#,</v>
-      </c>
-      <c r="F16" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,</v>
+      </c>
+      <c r="H16" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>24:#,Night Light Enable and mode,</v>
-      </c>
-      <c r="G16" s="59" t="str">
-        <f>CONCATENATE(G15,E16)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,</v>
-      </c>
-      <c r="H16" s="59" t="str">
-        <f>CONCATENATE(H15,F16)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3140,20 +3231,20 @@
         <v>81</v>
       </c>
       <c r="E17" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>25:#,</v>
+      </c>
+      <c r="F17" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>25:#,(ip address preset),</v>
+      </c>
+      <c r="G17" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>25:#,</v>
-      </c>
-      <c r="F17" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,</v>
+      </c>
+      <c r="H17" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>25:#,(ip address preset),</v>
-      </c>
-      <c r="G17" s="59" t="str">
-        <f>CONCATENATE(G16,E17)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,</v>
-      </c>
-      <c r="H17" s="59" t="str">
-        <f>CONCATENATE(H16,F17)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3167,23 +3258,23 @@
         <v>33</v>
       </c>
       <c r="D18" s="77" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="E18" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>26:#,</v>
+      </c>
+      <c r="F18" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>26:#,Alarm_Enable,</v>
+      </c>
+      <c r="G18" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>26:#,</v>
-      </c>
-      <c r="F18" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,</v>
+      </c>
+      <c r="H18" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>26:#,Alarm Enable,</v>
-      </c>
-      <c r="G18" s="59" t="str">
-        <f>CONCATENATE(G17,E18)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,</v>
-      </c>
-      <c r="H18" s="59" t="str">
-        <f>CONCATENATE(H17,F18)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3194,26 +3285,26 @@
         <v>27</v>
       </c>
       <c r="C19" s="76" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="D19" s="77" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="E19" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>27:9########,</v>
+      </c>
+      <c r="F19" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>27:9########,Alarm_Date,</v>
+      </c>
+      <c r="G19" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>27:9######,</v>
-      </c>
-      <c r="F19" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,</v>
+      </c>
+      <c r="H19" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>27:9######,Alarm Date,</v>
-      </c>
-      <c r="G19" s="59" t="str">
-        <f>CONCATENATE(G18,E19)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,</v>
-      </c>
-      <c r="H19" s="59" t="str">
-        <f>CONCATENATE(H18,F19)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3224,26 +3315,26 @@
         <v>28</v>
       </c>
       <c r="C20" s="76" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="D20" s="77" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="E20" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>28:9########,</v>
+      </c>
+      <c r="F20" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>28:9########,Alarm_Time,</v>
+      </c>
+      <c r="G20" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>28:9######,</v>
-      </c>
-      <c r="F20" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,</v>
+      </c>
+      <c r="H20" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>28:9######,Alarm Time,</v>
-      </c>
-      <c r="G20" s="59" t="str">
-        <f>CONCATENATE(G19,E20)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,</v>
-      </c>
-      <c r="H20" s="59" t="str">
-        <f>CONCATENATE(H19,F20)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3257,23 +3348,23 @@
         <v>44</v>
       </c>
       <c r="D21" s="77" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="E21" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>29:##,</v>
+      </c>
+      <c r="F21" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>29:##,Performance_number,</v>
+      </c>
+      <c r="G21" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>29:##,</v>
-      </c>
-      <c r="F21" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,</v>
+      </c>
+      <c r="H21" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>29:##,Performance number,</v>
-      </c>
-      <c r="G21" s="59" t="str">
-        <f>CONCATENATE(G20,E21)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,</v>
-      </c>
-      <c r="H21" s="59" t="str">
-        <f>CONCATENATE(H20,F21)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3287,23 +3378,23 @@
         <v>33</v>
       </c>
       <c r="D22" s="77" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="E22" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>41:#,</v>
+      </c>
+      <c r="F22" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>41:#,Stayin_Game_Status,</v>
+      </c>
+      <c r="G22" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>41:#,</v>
-      </c>
-      <c r="F22" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,</v>
+      </c>
+      <c r="H22" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>41:#,Stayin_Game_Status (0,1 = not,ingame),</v>
-      </c>
-      <c r="G22" s="59" t="str">
-        <f>CONCATENATE(G21,E22)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,</v>
-      </c>
-      <c r="H22" s="59" t="str">
-        <f>CONCATENATE(H21,F22)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3317,23 +3408,23 @@
         <v>33</v>
       </c>
       <c r="D23" s="77" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="E23" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>42:#,</v>
+      </c>
+      <c r="F23" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>42:#,myCharNum,</v>
+      </c>
+      <c r="G23" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>42:#,</v>
-      </c>
-      <c r="F23" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,</v>
+      </c>
+      <c r="H23" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>42:#,myCharNum (1, 2, 3, 4, 5, or 6),</v>
-      </c>
-      <c r="G23" s="59" t="str">
-        <f>CONCATENATE(G22,E23)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,</v>
-      </c>
-      <c r="H23" s="59" t="str">
-        <f>CONCATENATE(H22,F23)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3344,26 +3435,26 @@
         <v>43</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="77" t="s">
         <v>92</v>
       </c>
       <c r="E24" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>43:#######,</v>
+      </c>
+      <c r="F24" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>43:#######,ActualName,</v>
+      </c>
+      <c r="G24" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>43:#######,</v>
-      </c>
-      <c r="F24" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,</v>
+      </c>
+      <c r="H24" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>43:#######,ActualName,</v>
-      </c>
-      <c r="G24" s="59" t="str">
-        <f>CONCATENATE(G23,E24)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,</v>
-      </c>
-      <c r="H24" s="59" t="str">
-        <f>CONCATENATE(H23,F24)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3374,26 +3465,26 @@
         <v>44</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D25" s="77" t="s">
         <v>83</v>
       </c>
       <c r="E25" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>44:9###,</v>
+      </c>
+      <c r="F25" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>44:9###,BankAfterSpend,</v>
+      </c>
+      <c r="G25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>44:###,</v>
-      </c>
-      <c r="F25" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,</v>
+      </c>
+      <c r="H25" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>44:###,BankAfterSpend,</v>
-      </c>
-      <c r="G25" s="22" t="str">
-        <f>CONCATENATE(G24,E25)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,</v>
-      </c>
-      <c r="H25" s="22" t="str">
-        <f>CONCATENATE(H24,F25)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3404,26 +3495,26 @@
         <v>45</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D26" s="77" t="s">
         <v>93</v>
       </c>
       <c r="E26" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>45:9###,</v>
+      </c>
+      <c r="F26" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>45:9###,Attack_balance,</v>
+      </c>
+      <c r="G26" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>45:###,</v>
-      </c>
-      <c r="F26" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,</v>
+      </c>
+      <c r="H26" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>45:###,Attack_balance,</v>
-      </c>
-      <c r="G26" s="59" t="str">
-        <f>CONCATENATE(G25,E26)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,</v>
-      </c>
-      <c r="H26" s="59" t="str">
-        <f>CONCATENATE(H25,F26)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3437,23 +3528,23 @@
         <v>94</v>
       </c>
       <c r="D27" s="77" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="E27" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>46:9######,</v>
+      </c>
+      <c r="F27" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>46:9######,Attack_or_Donate_Flag,</v>
+      </c>
+      <c r="G27" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>46:9######,</v>
-      </c>
-      <c r="F27" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,</v>
+      </c>
+      <c r="H27" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>46:9######,Attack_or_Donate_Flag (Pinky-Inky),</v>
-      </c>
-      <c r="G27" s="59" t="str">
-        <f>CONCATENATE(G26,E27)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,</v>
-      </c>
-      <c r="H27" s="59" t="str">
-        <f>CONCATENATE(H26,F27)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3470,20 +3561,20 @@
         <v>89</v>
       </c>
       <c r="E28" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>47:9######,</v>
+      </c>
+      <c r="F28" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>47:9######,Will_or_No (Pinky-Inky),</v>
+      </c>
+      <c r="G28" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>47:9######,</v>
-      </c>
-      <c r="F28" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,</v>
+      </c>
+      <c r="H28" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>47:9######,Will_or_No (Pinky-Inky),</v>
-      </c>
-      <c r="G28" s="59" t="str">
-        <f>CONCATENATE(G27,E28)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,</v>
-      </c>
-      <c r="H28" s="59" t="str">
-        <f>CONCATENATE(H27,F28)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3500,20 +3591,20 @@
         <v>91</v>
       </c>
       <c r="E29" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>48:9######,</v>
+      </c>
+      <c r="F29" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>48:9######,Mirror_or_No (Pinky-Inky),</v>
+      </c>
+      <c r="G29" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>48:9######,</v>
-      </c>
-      <c r="F29" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,</v>
+      </c>
+      <c r="H29" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>48:9######,Mirror_or_No (Pinky-Inky),</v>
-      </c>
-      <c r="G29" s="59" t="str">
-        <f>CONCATENATE(G28,E29)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,</v>
-      </c>
-      <c r="H29" s="59" t="str">
-        <f>CONCATENATE(H28,F29)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3524,26 +3615,26 @@
         <v>49</v>
       </c>
       <c r="C30" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D30" s="77" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E30" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>49:9###,</v>
+      </c>
+      <c r="F30" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>49:9###,Attack_or_Donate Pinky_Amnt,</v>
+      </c>
+      <c r="G30" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>49:###,</v>
-      </c>
-      <c r="F30" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,</v>
+      </c>
+      <c r="H30" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>49:###,Attack_or_Donate Pinky_Amnt,</v>
-      </c>
-      <c r="G30" s="59" t="str">
-        <f>CONCATENATE(G29,E30)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,</v>
-      </c>
-      <c r="H30" s="59" t="str">
-        <f>CONCATENATE(H29,F30)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3554,26 +3645,26 @@
         <v>50</v>
       </c>
       <c r="C31" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D31" s="77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E31" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>50:9###,</v>
+      </c>
+      <c r="F31" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>50:9###,Attack_or_Donate Clyde_Amnt,</v>
+      </c>
+      <c r="G31" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>50:###,</v>
-      </c>
-      <c r="F31" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,</v>
+      </c>
+      <c r="H31" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>50:###,Attack_or_Donate Clyde_Amnt,</v>
-      </c>
-      <c r="G31" s="59" t="str">
-        <f>CONCATENATE(G30,E31)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,</v>
-      </c>
-      <c r="H31" s="59" t="str">
-        <f>CONCATENATE(H30,F31)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3584,26 +3675,26 @@
         <v>51</v>
       </c>
       <c r="C32" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D32" s="77" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E32" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>51:9###,</v>
+      </c>
+      <c r="F32" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>51:9###,Attack_or_Donate Cherry_Amnt,</v>
+      </c>
+      <c r="G32" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>51:###,</v>
-      </c>
-      <c r="F32" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,</v>
+      </c>
+      <c r="H32" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>51:###,Attack_or_Donate Cherry_Amnt,</v>
-      </c>
-      <c r="G32" s="59" t="str">
-        <f>CONCATENATE(G31,E32)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,</v>
-      </c>
-      <c r="H32" s="59" t="str">
-        <f>CONCATENATE(H31,F32)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3614,26 +3705,26 @@
         <v>52</v>
       </c>
       <c r="C33" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D33" s="77" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E33" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>52:9###,</v>
+      </c>
+      <c r="F33" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>52:9###,Attack_or_Donate PacMan_Amnt,</v>
+      </c>
+      <c r="G33" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>52:###,</v>
-      </c>
-      <c r="F33" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,</v>
+      </c>
+      <c r="H33" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>52:###,Attack_or_Donate PacMan_Amnt,</v>
-      </c>
-      <c r="G33" s="59" t="str">
-        <f>CONCATENATE(G32,E33)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,</v>
-      </c>
-      <c r="H33" s="59" t="str">
-        <f>CONCATENATE(H32,F33)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3644,26 +3735,26 @@
         <v>53</v>
       </c>
       <c r="C34" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D34" s="77" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E34" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>53:9###,</v>
+      </c>
+      <c r="F34" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>53:9###,Attack_or_Donate Blinky_Amnt,</v>
+      </c>
+      <c r="G34" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>53:###,</v>
-      </c>
-      <c r="F34" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,</v>
+      </c>
+      <c r="H34" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>53:###,Attack_or_Donate Blinky_Amnt,</v>
-      </c>
-      <c r="G34" s="59" t="str">
-        <f>CONCATENATE(G33,E34)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,</v>
-      </c>
-      <c r="H34" s="59" t="str">
-        <f>CONCATENATE(H33,F34)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3674,26 +3765,26 @@
         <v>54</v>
       </c>
       <c r="C35" s="76" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D35" s="77" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E35" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>54:9###,</v>
+      </c>
+      <c r="F35" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>54:9###,Attack_or_Donate Inky_Amnt,</v>
+      </c>
+      <c r="G35" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>54:###,</v>
-      </c>
-      <c r="F35" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,</v>
+      </c>
+      <c r="H35" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>54:###,Attack_or_Donate Inky_Amnt,</v>
-      </c>
-      <c r="G35" s="59" t="str">
-        <f>CONCATENATE(G34,E35)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,</v>
-      </c>
-      <c r="H35" s="59" t="str">
-        <f>CONCATENATE(H34,F35)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3707,23 +3798,23 @@
         <v>94</v>
       </c>
       <c r="D36" s="77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E36" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>55:9######,</v>
+      </c>
+      <c r="F36" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>55:9######,Mirror_Balances_Pinky_Values,</v>
+      </c>
+      <c r="G36" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>55:9######,</v>
-      </c>
-      <c r="F36" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,</v>
+      </c>
+      <c r="H36" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>55:9######,Mirror_Balances_Pinky_Values,</v>
-      </c>
-      <c r="G36" s="59" t="str">
-        <f>CONCATENATE(G35,E36)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,</v>
-      </c>
-      <c r="H36" s="59" t="str">
-        <f>CONCATENATE(H35,F36)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3737,23 +3828,23 @@
         <v>94</v>
       </c>
       <c r="D37" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E37" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>56:9######,</v>
+      </c>
+      <c r="F37" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>56:9######,Mirror_Balances_Clyde_Values,</v>
+      </c>
+      <c r="G37" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>56:9######,</v>
-      </c>
-      <c r="F37" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,</v>
+      </c>
+      <c r="H37" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>56:9######,Mirror_Balances_Clyde_Values,</v>
-      </c>
-      <c r="G37" s="59" t="str">
-        <f>CONCATENATE(G36,E37)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,</v>
-      </c>
-      <c r="H37" s="59" t="str">
-        <f>CONCATENATE(H36,F37)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3767,23 +3858,23 @@
         <v>94</v>
       </c>
       <c r="D38" s="77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E38" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>57:9######,</v>
+      </c>
+      <c r="F38" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>57:9######,Mirror_Balances_Cherry_Values,</v>
+      </c>
+      <c r="G38" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>57:9######,</v>
-      </c>
-      <c r="F38" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,</v>
+      </c>
+      <c r="H38" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>57:9######,Mirror_Balances_Cherry_Values,</v>
-      </c>
-      <c r="G38" s="59" t="str">
-        <f>CONCATENATE(G37,E38)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,</v>
-      </c>
-      <c r="H38" s="59" t="str">
-        <f>CONCATENATE(H37,F38)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3795,23 +3886,23 @@
         <v>94</v>
       </c>
       <c r="D39" s="77" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E39" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>58:9######,</v>
+      </c>
+      <c r="F39" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>58:9######,Mirror_Balances_Pacman_Values,</v>
+      </c>
+      <c r="G39" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>58:9######,</v>
-      </c>
-      <c r="F39" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,</v>
+      </c>
+      <c r="H39" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>58:9######,Mirror_Balances_Pacman_Values,</v>
-      </c>
-      <c r="G39" s="59" t="str">
-        <f>CONCATENATE(G38,E39)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,</v>
-      </c>
-      <c r="H39" s="59" t="str">
-        <f>CONCATENATE(H38,F39)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3823,23 +3914,23 @@
         <v>94</v>
       </c>
       <c r="D40" s="77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E40" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>59:9######,</v>
+      </c>
+      <c r="F40" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>59:9######,Mirror_Balances_Blinky_Values,</v>
+      </c>
+      <c r="G40" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>59:9######,</v>
-      </c>
-      <c r="F40" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,</v>
+      </c>
+      <c r="H40" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>59:9######,Mirror_Balances_Blinky_Values,</v>
-      </c>
-      <c r="G40" s="59" t="str">
-        <f>CONCATENATE(G39,E40)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,</v>
-      </c>
-      <c r="H40" s="59" t="str">
-        <f>CONCATENATE(H39,F40)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3851,23 +3942,23 @@
         <v>94</v>
       </c>
       <c r="D41" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E41" s="79" t="str">
+        <f t="shared" si="2"/>
+        <v>60:9######,</v>
+      </c>
+      <c r="F41" s="80" t="str">
+        <f t="shared" si="3"/>
+        <v>60:9######,Mirror_Balances_Inky_Values,</v>
+      </c>
+      <c r="G41" s="59" t="str">
         <f t="shared" si="0"/>
-        <v>60:9######,</v>
-      </c>
-      <c r="F41" s="80" t="str">
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+      </c>
+      <c r="H41" s="59" t="str">
         <f t="shared" si="1"/>
-        <v>60:9######,Mirror_Balances_Inky_Values,</v>
-      </c>
-      <c r="G41" s="59" t="str">
-        <f>CONCATENATE(G40,E41)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
-      </c>
-      <c r="H41" s="59" t="str">
-        <f>CONCATENATE(H40,F41)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3880,12 +3971,12 @@
       <c r="E42" s="79"/>
       <c r="F42" s="80"/>
       <c r="G42" s="59" t="str">
-        <f>CONCATENATE(G41,E42)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+        <f t="shared" si="0"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
       </c>
       <c r="H42" s="59" t="str">
-        <f>CONCATENATE(H41,F42)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3898,12 +3989,12 @@
       <c r="E43" s="79"/>
       <c r="F43" s="80"/>
       <c r="G43" s="59" t="str">
-        <f>CONCATENATE(G42,E43)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+        <f t="shared" si="0"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
       </c>
       <c r="H43" s="59" t="str">
-        <f>CONCATENATE(H42,F43)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3916,12 +4007,12 @@
       <c r="E44" s="79"/>
       <c r="F44" s="80"/>
       <c r="G44" s="59" t="str">
-        <f>CONCATENATE(G43,E44)</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+        <f t="shared" si="0"/>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
       </c>
       <c r="H44" s="59" t="str">
-        <f>CONCATENATE(H43,F44)</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+        <f t="shared" si="1"/>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3939,13 +4030,13 @@
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E47" s="41" t="str">
         <f>+H44</f>
-        <v>11:#,Master Enable,12:#,Light Enable,13:#,Sound Enable,14:#,Motion Enable,15:#,Clock Enable,16:#,Light Pinky,17:#,Light Clyde,18:#,Light Cherry,19:#,Light PacMan,20:#,Light Blinky,21:#,Light Inky,22:#,Light Sensor Enable,23:9####,Light Sensor trigger value,24:#,Night Light Enable and mode,25:#,(ip address preset),26:#,Alarm Enable,27:9######,Alarm Date,28:9######,Alarm Time,29:##,Performance number,41:#,Stayin_Game_Status (0,1 = not,ingame),42:#,myCharNum (1, 2, 3, 4, 5, or 6),43:#######,ActualName,44:###,BankAfterSpend,45:###,Attack_balance,46:9######,Attack_or_Donate_Flag (Pinky-Inky),47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:###,Attack_or_Donate Pinky_Amnt,50:###,Attack_or_Donate Clyde_Amnt,51:###,Attack_or_Donate Cherry_Amnt,52:###,Attack_or_Donate PacMan_Amnt,53:###,Attack_or_Donate Blinky_Amnt,54:###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
+        <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E48" s="27" t="str">
         <f>G44</f>
-        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9######,28:9######,29:##,41:#,42:#,43:#######,44:###,45:###,46:9######,47:9######,48:9######,49:###,50:###,51:###,52:###,53:###,54:###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
+        <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
       </c>
       <c r="F48" s="27"/>
     </row>
@@ -3976,6 +4067,1353 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1"/>
+    <col min="9" max="9" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3">
+        <f>COMBINED!B3</f>
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3">
+        <f>LEN(COMBINED!C3)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" t="str">
+        <f>+COMBINED!D3</f>
+        <v>Master_Enable</v>
+      </c>
+      <c r="I3" s="87" t="str">
+        <f>CONCATENATE(A3,B3,C3,D3,E3,F3)</f>
+        <v>MESSAGE_PART_LENGTH[11]= 5;  //Master_Enable</v>
+      </c>
+      <c r="J3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" t="str">
+        <f>CONCATENATE(J3," ",F3,";")</f>
+        <v>int Master_Enable;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <f>COMBINED!B4</f>
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4">
+        <f>LEN(COMBINED!C4)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" t="str">
+        <f>+COMBINED!D4</f>
+        <v>Light_Enable</v>
+      </c>
+      <c r="I4" s="87" t="str">
+        <f t="shared" ref="I4:I27" si="0">CONCATENATE(A4,B4,C4,D4,E4,F4)</f>
+        <v>MESSAGE_PART_LENGTH[12]= 5;  //Light_Enable</v>
+      </c>
+      <c r="J4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K41" si="1">CONCATENATE(J4," ",F4,";")</f>
+        <v>int Light_Enable;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5">
+        <f>COMBINED!B5</f>
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5">
+        <f>LEN(COMBINED!C5)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" t="str">
+        <f>+COMBINED!D5</f>
+        <v>Sound_Enable</v>
+      </c>
+      <c r="I5" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[13]= 5;  //Sound_Enable</v>
+      </c>
+      <c r="J5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>int Sound_Enable;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6">
+        <f>COMBINED!B6</f>
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6">
+        <f>LEN(COMBINED!C6)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="str">
+        <f>+COMBINED!D6</f>
+        <v>Motion_Enable</v>
+      </c>
+      <c r="I6" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[14]= 5;  //Motion_Enable</v>
+      </c>
+      <c r="J6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>int Motion_Enable;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7">
+        <f>COMBINED!B7</f>
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7">
+        <f>LEN(COMBINED!C7)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" t="str">
+        <f>+COMBINED!D7</f>
+        <v>Clock_Enable</v>
+      </c>
+      <c r="I7" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[15]= 5;  //Clock_Enable</v>
+      </c>
+      <c r="J7" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>int Clock_Enable;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8">
+        <f>COMBINED!B8</f>
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8">
+        <f>LEN(COMBINED!C8)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" t="str">
+        <f>+COMBINED!D8</f>
+        <v>Light_Pinky</v>
+      </c>
+      <c r="I8" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[16]= 5;  //Light_Pinky</v>
+      </c>
+      <c r="J8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_Pinky;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9">
+        <f>COMBINED!B9</f>
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9">
+        <f>LEN(COMBINED!C9)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" t="str">
+        <f>+COMBINED!D9</f>
+        <v>Light_Clyde</v>
+      </c>
+      <c r="I9" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[17]= 5;  //Light_Clyde</v>
+      </c>
+      <c r="J9" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_Clyde;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10">
+        <f>COMBINED!B10</f>
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10">
+        <f>LEN(COMBINED!C10)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="str">
+        <f>+COMBINED!D10</f>
+        <v>Light_Cherry</v>
+      </c>
+      <c r="I10" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[18]= 5;  //Light_Cherry</v>
+      </c>
+      <c r="J10" t="s">
+        <v>116</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_Cherry;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11">
+        <f>COMBINED!B11</f>
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11">
+        <f>LEN(COMBINED!C11)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" t="str">
+        <f>+COMBINED!D11</f>
+        <v>Light_PacMan</v>
+      </c>
+      <c r="I11" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[19]= 5;  //Light_PacMan</v>
+      </c>
+      <c r="J11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_PacMan;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12">
+        <f>COMBINED!B12</f>
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12">
+        <f>LEN(COMBINED!C12)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" t="str">
+        <f>+COMBINED!D12</f>
+        <v>Light_Blinky</v>
+      </c>
+      <c r="I12" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[20]= 5;  //Light_Blinky</v>
+      </c>
+      <c r="J12" t="s">
+        <v>116</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_Blinky;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13">
+        <f>COMBINED!B13</f>
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13">
+        <f>LEN(COMBINED!C13)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" t="str">
+        <f>+COMBINED!D13</f>
+        <v>Light_Inky</v>
+      </c>
+      <c r="I13" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[21]= 5;  //Light_Inky</v>
+      </c>
+      <c r="J13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_Inky;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14">
+        <f>COMBINED!B14</f>
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14">
+        <f>LEN(COMBINED!C14)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" t="str">
+        <f>+COMBINED!D14</f>
+        <v>Light_Sensor_Enable</v>
+      </c>
+      <c r="I14" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[22]= 5;  //Light_Sensor_Enable</v>
+      </c>
+      <c r="J14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_Sensor_Enable;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15">
+        <f>COMBINED!B15</f>
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15">
+        <f>LEN(COMBINED!C15)+4</f>
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" t="str">
+        <f>+COMBINED!D15</f>
+        <v>Light_Sensor_trigger_value</v>
+      </c>
+      <c r="I15" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[23]= 9;  //Light_Sensor_trigger_value</v>
+      </c>
+      <c r="J15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>int Light_Sensor_trigger_value;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16">
+        <f>COMBINED!B16</f>
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16">
+        <f>LEN(COMBINED!C16)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" t="str">
+        <f>+COMBINED!D16</f>
+        <v>Night_Light_Enable_and_mode</v>
+      </c>
+      <c r="I16" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[24]= 5;  //Night_Light_Enable_and_mode</v>
+      </c>
+      <c r="J16" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>int Night_Light_Enable_and_mode;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17">
+        <f>COMBINED!B17</f>
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17">
+        <f>LEN(COMBINED!C17)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" t="str">
+        <f>+COMBINED!D17</f>
+        <v>(ip address preset)</v>
+      </c>
+      <c r="I17" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[25]= 5;  //(ip address preset)</v>
+      </c>
+      <c r="J17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>String (ip address preset);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18">
+        <f>COMBINED!B18</f>
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18">
+        <f>LEN(COMBINED!C18)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" t="str">
+        <f>+COMBINED!D18</f>
+        <v>Alarm_Enable</v>
+      </c>
+      <c r="I18" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[26]= 5;  //Alarm_Enable</v>
+      </c>
+      <c r="J18" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>int Alarm_Enable;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19">
+        <f>COMBINED!B19</f>
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19">
+        <f>LEN(COMBINED!C19)+4</f>
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" t="str">
+        <f>+COMBINED!D19</f>
+        <v>Alarm_Date</v>
+      </c>
+      <c r="I19" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[27]= 13;  //Alarm_Date</v>
+      </c>
+      <c r="J19" t="s">
+        <v>138</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>String Alarm_Date;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20">
+        <f>COMBINED!B20</f>
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20">
+        <f>LEN(COMBINED!C20)+4</f>
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" t="str">
+        <f>+COMBINED!D20</f>
+        <v>Alarm_Time</v>
+      </c>
+      <c r="I20" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[28]= 13;  //Alarm_Time</v>
+      </c>
+      <c r="J20" t="s">
+        <v>138</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>String Alarm_Time;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21">
+        <f>COMBINED!B21</f>
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21">
+        <f>LEN(COMBINED!C21)+4</f>
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" t="str">
+        <f>+COMBINED!D21</f>
+        <v>Performance_number</v>
+      </c>
+      <c r="I21" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[29]= 6;  //Performance_number</v>
+      </c>
+      <c r="J21" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>int Performance_number;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22">
+        <f>COMBINED!B22</f>
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22">
+        <f>LEN(COMBINED!C22)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" t="str">
+        <f>+COMBINED!D22</f>
+        <v>Stayin_Game_Status</v>
+      </c>
+      <c r="I22" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[41]= 5;  //Stayin_Game_Status</v>
+      </c>
+      <c r="J22" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>int Stayin_Game_Status;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23">
+        <f>COMBINED!B23</f>
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23">
+        <f>LEN(COMBINED!C23)+4</f>
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" t="str">
+        <f>+COMBINED!D23</f>
+        <v>myCharNum</v>
+      </c>
+      <c r="I23" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[42]= 5;  //myCharNum</v>
+      </c>
+      <c r="J23" t="s">
+        <v>116</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>int myCharNum;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24">
+        <f>COMBINED!B24</f>
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24">
+        <f>LEN(COMBINED!C24)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" t="str">
+        <f>+COMBINED!D24</f>
+        <v>ActualName</v>
+      </c>
+      <c r="I24" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[43]= 11;  //ActualName</v>
+      </c>
+      <c r="J24" t="s">
+        <v>138</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>String ActualName;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25">
+        <f>COMBINED!B25</f>
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25">
+        <f>LEN(COMBINED!C25)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" t="str">
+        <f>+COMBINED!D25</f>
+        <v>BankAfterSpend</v>
+      </c>
+      <c r="I25" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[44]= 8;  //BankAfterSpend</v>
+      </c>
+      <c r="J25" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>int BankAfterSpend;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26">
+        <f>COMBINED!B26</f>
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26">
+        <f>LEN(COMBINED!C26)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" t="str">
+        <f>+COMBINED!D26</f>
+        <v>Attack_balance</v>
+      </c>
+      <c r="I26" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[45]= 8;  //Attack_balance</v>
+      </c>
+      <c r="J26" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>int Attack_balance;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27">
+        <f>COMBINED!B27</f>
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27">
+        <f>LEN(COMBINED!C27)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" t="str">
+        <f>+COMBINED!D27</f>
+        <v>Attack_or_Donate_Flag</v>
+      </c>
+      <c r="I27" s="87" t="str">
+        <f t="shared" si="0"/>
+        <v>MESSAGE_PART_LENGTH[46]= 11;  //Attack_or_Donate_Flag</v>
+      </c>
+      <c r="J27" t="s">
+        <v>139</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>long Attack_or_Donate_Flag;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28">
+        <f>COMBINED!B28</f>
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28">
+        <f>LEN(COMBINED!C28)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" t="str">
+        <f>+COMBINED!D28</f>
+        <v>Will_or_No (Pinky-Inky)</v>
+      </c>
+      <c r="I28" s="87" t="str">
+        <f>CONCATENATE(A28,B28,C28,D28,E28,F28)</f>
+        <v>MESSAGE_PART_LENGTH[47]= 11;  //Will_or_No (Pinky-Inky)</v>
+      </c>
+      <c r="J28" t="s">
+        <v>139</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>long Will_or_No (Pinky-Inky);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29">
+        <f>COMBINED!B29</f>
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29">
+        <f>LEN(COMBINED!C29)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" t="str">
+        <f>+COMBINED!D29</f>
+        <v>Mirror_or_No (Pinky-Inky)</v>
+      </c>
+      <c r="I29" s="87" t="str">
+        <f t="shared" ref="I29:I35" si="2">CONCATENATE(A29,B29,C29,D29,E29,F29)</f>
+        <v>MESSAGE_PART_LENGTH[48]= 11;  //Mirror_or_No (Pinky-Inky)</v>
+      </c>
+      <c r="J29" t="s">
+        <v>139</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>long Mirror_or_No (Pinky-Inky);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30">
+        <f>COMBINED!B30</f>
+        <v>49</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30">
+        <f>LEN(COMBINED!C30)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" t="str">
+        <f>+COMBINED!D30</f>
+        <v>Attack_or_Donate Pinky_Amnt</v>
+      </c>
+      <c r="I30" s="87" t="str">
+        <f t="shared" si="2"/>
+        <v>MESSAGE_PART_LENGTH[49]= 8;  //Attack_or_Donate Pinky_Amnt</v>
+      </c>
+      <c r="J30" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>int Attack_or_Donate Pinky_Amnt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31">
+        <f>COMBINED!B31</f>
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31">
+        <f>LEN(COMBINED!C31)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" t="str">
+        <f>+COMBINED!D31</f>
+        <v>Attack_or_Donate Clyde_Amnt</v>
+      </c>
+      <c r="I31" s="87" t="str">
+        <f t="shared" si="2"/>
+        <v>MESSAGE_PART_LENGTH[50]= 8;  //Attack_or_Donate Clyde_Amnt</v>
+      </c>
+      <c r="J31" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>int Attack_or_Donate Clyde_Amnt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32">
+        <f>COMBINED!B32</f>
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32">
+        <f>LEN(COMBINED!C32)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" t="str">
+        <f>+COMBINED!D32</f>
+        <v>Attack_or_Donate Cherry_Amnt</v>
+      </c>
+      <c r="I32" s="87" t="str">
+        <f t="shared" si="2"/>
+        <v>MESSAGE_PART_LENGTH[51]= 8;  //Attack_or_Donate Cherry_Amnt</v>
+      </c>
+      <c r="J32" t="s">
+        <v>116</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>int Attack_or_Donate Cherry_Amnt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33">
+        <f>COMBINED!B33</f>
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33">
+        <f>LEN(COMBINED!C33)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" t="str">
+        <f>+COMBINED!D33</f>
+        <v>Attack_or_Donate PacMan_Amnt</v>
+      </c>
+      <c r="I33" s="87" t="str">
+        <f t="shared" si="2"/>
+        <v>MESSAGE_PART_LENGTH[52]= 8;  //Attack_or_Donate PacMan_Amnt</v>
+      </c>
+      <c r="J33" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>int Attack_or_Donate PacMan_Amnt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34">
+        <f>COMBINED!B34</f>
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34">
+        <f>LEN(COMBINED!C34)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" t="str">
+        <f>+COMBINED!D34</f>
+        <v>Attack_or_Donate Blinky_Amnt</v>
+      </c>
+      <c r="I34" s="87" t="str">
+        <f t="shared" si="2"/>
+        <v>MESSAGE_PART_LENGTH[53]= 8;  //Attack_or_Donate Blinky_Amnt</v>
+      </c>
+      <c r="J34" t="s">
+        <v>116</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>int Attack_or_Donate Blinky_Amnt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35">
+        <f>COMBINED!B35</f>
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35">
+        <f>LEN(COMBINED!C35)+4</f>
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" t="str">
+        <f>+COMBINED!D35</f>
+        <v>Attack_or_Donate Inky_Amnt</v>
+      </c>
+      <c r="I35" s="87" t="str">
+        <f t="shared" si="2"/>
+        <v>MESSAGE_PART_LENGTH[54]= 8;  //Attack_or_Donate Inky_Amnt</v>
+      </c>
+      <c r="J35" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>int Attack_or_Donate Inky_Amnt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36">
+        <f>COMBINED!B36</f>
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36">
+        <f>LEN(COMBINED!C36)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>112</v>
+      </c>
+      <c r="F36" t="str">
+        <f>+COMBINED!D36</f>
+        <v>Mirror_Balances_Pinky_Values</v>
+      </c>
+      <c r="I36" s="87" t="str">
+        <f>CONCATENATE(A36,B36,C36,D36,E36,F36)</f>
+        <v>MESSAGE_PART_LENGTH[55]= 11;  //Mirror_Balances_Pinky_Values</v>
+      </c>
+      <c r="J36" t="s">
+        <v>116</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>int Mirror_Balances_Pinky_Values;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37">
+        <f>COMBINED!B37</f>
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37">
+        <f>LEN(COMBINED!C37)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" t="str">
+        <f>+COMBINED!D37</f>
+        <v>Mirror_Balances_Clyde_Values</v>
+      </c>
+      <c r="I37" s="87" t="str">
+        <f t="shared" ref="I37:I38" si="3">CONCATENATE(A37,B37,C37,D37,E37,F37)</f>
+        <v>MESSAGE_PART_LENGTH[56]= 11;  //Mirror_Balances_Clyde_Values</v>
+      </c>
+      <c r="J37" t="s">
+        <v>116</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>int Mirror_Balances_Clyde_Values;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38">
+        <f>COMBINED!B38</f>
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38">
+        <f>LEN(COMBINED!C38)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" t="str">
+        <f>+COMBINED!D38</f>
+        <v>Mirror_Balances_Cherry_Values</v>
+      </c>
+      <c r="I38" s="87" t="str">
+        <f t="shared" si="3"/>
+        <v>MESSAGE_PART_LENGTH[57]= 11;  //Mirror_Balances_Cherry_Values</v>
+      </c>
+      <c r="J38" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>int Mirror_Balances_Cherry_Values;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39">
+        <f>COMBINED!B39</f>
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39">
+        <f>LEN(COMBINED!C39)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" t="str">
+        <f>+COMBINED!D39</f>
+        <v>Mirror_Balances_Pacman_Values</v>
+      </c>
+      <c r="I39" s="87" t="str">
+        <f>CONCATENATE(A39,B39,C39,D39,E39,F39)</f>
+        <v>MESSAGE_PART_LENGTH[58]= 11;  //Mirror_Balances_Pacman_Values</v>
+      </c>
+      <c r="J39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>int Mirror_Balances_Pacman_Values;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40">
+        <f>COMBINED!B40</f>
+        <v>59</v>
+      </c>
+      <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40">
+        <f>LEN(COMBINED!C40)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" t="str">
+        <f>+COMBINED!D40</f>
+        <v>Mirror_Balances_Blinky_Values</v>
+      </c>
+      <c r="I40" s="87" t="str">
+        <f>CONCATENATE(A40,B40,C40,D40,E40,F40)</f>
+        <v>MESSAGE_PART_LENGTH[59]= 11;  //Mirror_Balances_Blinky_Values</v>
+      </c>
+      <c r="J40" t="s">
+        <v>116</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>int Mirror_Balances_Blinky_Values;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41">
+        <f>COMBINED!B41</f>
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41">
+        <f>LEN(COMBINED!C41)+4</f>
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" t="str">
+        <f>+COMBINED!D41</f>
+        <v>Mirror_Balances_Inky_Values</v>
+      </c>
+      <c r="I41" s="87" t="str">
+        <f>CONCATENATE(A41,B41,C41,D41,E41,F41)</f>
+        <v>MESSAGE_PART_LENGTH[60]= 11;  //Mirror_Balances_Inky_Values</v>
+      </c>
+      <c r="J41" t="s">
+        <v>116</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>int Mirror_Balances_Inky_Values;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -4056,7 +5494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -9328,7 +10766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BC82"/>
   <sheetViews>

</xml_diff>

<commit_message>
rudimentary communications in new format built for Atmega.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COMBINED" sheetId="5" r:id="rId1"/>
-    <sheet name="MESSAGE_PART_LENGTH" sheetId="6" r:id="rId2"/>
-    <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId3"/>
-    <sheet name="TABLE" sheetId="1" r:id="rId4"/>
-    <sheet name="StayinAliveComms" sheetId="3" r:id="rId5"/>
-    <sheet name="Android_Global_Variables" sheetId="7" r:id="rId6"/>
+    <sheet name="ATMEGA_CMD_READS" sheetId="8" r:id="rId2"/>
+    <sheet name="MESSAGE_PART_LENGTH" sheetId="6" r:id="rId3"/>
+    <sheet name="Comm Diagram_Notes" sheetId="2" r:id="rId4"/>
+    <sheet name="TABLE" sheetId="1" r:id="rId5"/>
+    <sheet name="StayinAliveComms" sheetId="3" r:id="rId6"/>
+    <sheet name="Android_Global_Variables" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="248">
   <si>
     <t>App use only</t>
   </si>
@@ -766,6 +767,153 @@
   </si>
   <si>
     <t xml:space="preserve">:" + </t>
+  </si>
+  <si>
+    <t>AtmegaVariable</t>
+  </si>
+  <si>
+    <t>M_EN</t>
+  </si>
+  <si>
+    <t>L_EN</t>
+  </si>
+  <si>
+    <t>S_EN</t>
+  </si>
+  <si>
+    <t>MO_EN</t>
+  </si>
+  <si>
+    <t>CL_EN</t>
+  </si>
+  <si>
+    <t>PIN_EN</t>
+  </si>
+  <si>
+    <t>CLY_EN</t>
+  </si>
+  <si>
+    <t>CHE_EN</t>
+  </si>
+  <si>
+    <t>PAC_EN</t>
+  </si>
+  <si>
+    <t>BLI_EN</t>
+  </si>
+  <si>
+    <t>INK_EN</t>
+  </si>
+  <si>
+    <t>LS_EN</t>
+  </si>
+  <si>
+    <t>ALM_EN</t>
+  </si>
+  <si>
+    <t>ALM_DATE</t>
+  </si>
+  <si>
+    <t>ALM_TIME</t>
+  </si>
+  <si>
+    <t>PERF_NUM</t>
+  </si>
+  <si>
+    <t>GAME_STATUS</t>
+  </si>
+  <si>
+    <t>MY_CHAR_NUM</t>
+  </si>
+  <si>
+    <t>ACT_NAME</t>
+  </si>
+  <si>
+    <t>BANK_AFTER_SPEND</t>
+  </si>
+  <si>
+    <t>ATTACK_BAL</t>
+  </si>
+  <si>
+    <t>ATT_DON</t>
+  </si>
+  <si>
+    <t>WILL_NO</t>
+  </si>
+  <si>
+    <t>MIRROR_NO</t>
+  </si>
+  <si>
+    <t>AD_PIN</t>
+  </si>
+  <si>
+    <t>AD_CHE</t>
+  </si>
+  <si>
+    <t>AD_CLY</t>
+  </si>
+  <si>
+    <t>AD_PAC</t>
+  </si>
+  <si>
+    <t>AD_BLI</t>
+  </si>
+  <si>
+    <t>AD_INK</t>
+  </si>
+  <si>
+    <t>MB_PIN</t>
+  </si>
+  <si>
+    <t>MB_CLY</t>
+  </si>
+  <si>
+    <t>MB_CHE</t>
+  </si>
+  <si>
+    <t>MB_PAC</t>
+  </si>
+  <si>
+    <t>MB_BLI</t>
+  </si>
+  <si>
+    <t>MB_INK</t>
+  </si>
+  <si>
+    <t>PIN_RENAME</t>
+  </si>
+  <si>
+    <t>CLY_RENAME</t>
+  </si>
+  <si>
+    <t>CHE_RENAME</t>
+  </si>
+  <si>
+    <t>PAC_RENAME</t>
+  </si>
+  <si>
+    <t>BLI_RENAME</t>
+  </si>
+  <si>
+    <t>INK_RENAME</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = (data_line[</t>
+  </si>
+  <si>
+    <t>]-48);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   // </t>
+  </si>
+  <si>
+    <t>NL_EN</t>
+  </si>
+  <si>
+    <t>LS_VAL</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1057,6 +1205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1167,7 +1321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1363,6 +1517,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2968,1488 +3123,1631 @@
     <tabColor theme="8" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H61"/>
+  <dimension ref="A2:I61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:D47"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
-    <col min="7" max="8" width="29.28515625" style="22"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="50" customWidth="1"/>
+    <col min="8" max="9" width="29.28515625" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="C2" s="7"/>
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+      <c r="C2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="59" t="str">
-        <f t="shared" ref="G2:G42" si="0">CONCATENATE(G1,E2)</f>
+      <c r="G2" s="21"/>
+      <c r="H2" s="59" t="str">
+        <f t="shared" ref="H2:H42" si="0">CONCATENATE(H1,F2)</f>
         <v>&gt;&gt;&gt;&gt;&gt;</v>
       </c>
-      <c r="H2" s="59" t="str">
-        <f t="shared" ref="H2:H42" si="1">CONCATENATE(H1,F2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+      <c r="I2" s="59" t="str">
+        <f t="shared" ref="I2:I42" si="1">CONCATENATE(I1,G2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="75">
         <v>1</v>
       </c>
       <c r="B3" s="75">
         <v>11</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="77" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="E3" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="79" t="str">
-        <f t="shared" ref="E3:E47" si="2">CONCATENATE($B3,":",$C3,",")</f>
+      <c r="F3" s="79" t="str">
+        <f t="shared" ref="F3:F47" si="2">CONCATENATE($B3,":",$D3,",")</f>
         <v>11:#,</v>
       </c>
-      <c r="F3" s="80" t="str">
-        <f>CONCATENATE($E3,$D3,",")</f>
+      <c r="G3" s="80" t="str">
+        <f>CONCATENATE($F3,$E3,",")</f>
         <v>11:#,Master_Enable,</v>
       </c>
-      <c r="G3" s="59" t="str">
+      <c r="H3" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,</v>
       </c>
-      <c r="H3" s="59" t="str">
+      <c r="I3" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="4" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="75">
         <v>2</v>
       </c>
       <c r="B4" s="75">
         <v>12</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="77" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="E4" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="79" t="str">
+      <c r="F4" s="79" t="str">
         <f t="shared" si="2"/>
         <v>12:#,</v>
       </c>
-      <c r="F4" s="80" t="str">
-        <f>CONCATENATE($E4,$D4,",")</f>
+      <c r="G4" s="80" t="str">
+        <f>CONCATENATE($F4,$E4,",")</f>
         <v>12:#,Light_Enable,</v>
       </c>
-      <c r="G4" s="59" t="str">
+      <c r="H4" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,</v>
       </c>
-      <c r="H4" s="59" t="str">
+      <c r="I4" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="75">
         <v>3</v>
       </c>
       <c r="B5" s="75">
         <v>13</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="77" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="E5" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="79" t="str">
+      <c r="F5" s="79" t="str">
         <f t="shared" si="2"/>
         <v>13:#,</v>
       </c>
-      <c r="F5" s="80" t="str">
-        <f>CONCATENATE($E5,$D5,",")</f>
+      <c r="G5" s="80" t="str">
+        <f>CONCATENATE($F5,$E5,",")</f>
         <v>13:#,Sound_Enable,</v>
       </c>
-      <c r="G5" s="59" t="str">
+      <c r="H5" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,</v>
       </c>
-      <c r="H5" s="59" t="str">
+      <c r="I5" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="6" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="75">
         <v>4</v>
       </c>
       <c r="B6" s="75">
         <v>14</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="77" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="E6" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="79" t="str">
+      <c r="F6" s="79" t="str">
         <f t="shared" si="2"/>
         <v>14:#,</v>
       </c>
-      <c r="F6" s="80" t="str">
-        <f>CONCATENATE($E6,$D6,",")</f>
+      <c r="G6" s="80" t="str">
+        <f>CONCATENATE($F6,$E6,",")</f>
         <v>14:#,Motion_Enable,</v>
       </c>
-      <c r="G6" s="59" t="str">
+      <c r="H6" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,</v>
       </c>
-      <c r="H6" s="59" t="str">
+      <c r="I6" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="7" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="75">
         <v>5</v>
       </c>
       <c r="B7" s="75">
         <v>15</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="77" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="77" t="s">
+      <c r="E7" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="79" t="str">
+      <c r="F7" s="79" t="str">
         <f t="shared" si="2"/>
         <v>15:#,</v>
       </c>
-      <c r="F7" s="80" t="str">
-        <f>CONCATENATE($E7,$D7,",")</f>
+      <c r="G7" s="80" t="str">
+        <f>CONCATENATE($F7,$E7,",")</f>
         <v>15:#,Clock_Enable,</v>
       </c>
-      <c r="G7" s="59" t="str">
+      <c r="H7" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,</v>
       </c>
-      <c r="H7" s="59" t="str">
+      <c r="I7" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="75">
         <v>6</v>
       </c>
       <c r="B8" s="75">
         <v>16</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="77" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="E8" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="79" t="str">
+      <c r="F8" s="79" t="str">
         <f t="shared" si="2"/>
         <v>16:#,</v>
       </c>
-      <c r="F8" s="80" t="str">
-        <f t="shared" ref="F8:F47" si="3">CONCATENATE($E8,$D8,",")</f>
+      <c r="G8" s="80" t="str">
+        <f t="shared" ref="G8:G47" si="3">CONCATENATE($F8,$E8,",")</f>
         <v>16:#,Light_Pinky,</v>
       </c>
-      <c r="G8" s="59" t="str">
+      <c r="H8" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,</v>
       </c>
-      <c r="H8" s="59" t="str">
+      <c r="I8" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="75">
         <v>7</v>
       </c>
       <c r="B9" s="75">
         <v>17</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="77" t="s">
+      <c r="E9" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="79" t="str">
+      <c r="F9" s="79" t="str">
         <f t="shared" si="2"/>
         <v>17:#,</v>
       </c>
-      <c r="F9" s="80" t="str">
+      <c r="G9" s="80" t="str">
         <f t="shared" si="3"/>
         <v>17:#,Light_Clyde,</v>
       </c>
-      <c r="G9" s="59" t="str">
+      <c r="H9" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,</v>
       </c>
-      <c r="H9" s="59" t="str">
+      <c r="I9" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="75">
         <v>8</v>
       </c>
       <c r="B10" s="75">
         <v>18</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="77" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="E10" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="79" t="str">
+      <c r="F10" s="79" t="str">
         <f t="shared" si="2"/>
         <v>18:#,</v>
       </c>
-      <c r="F10" s="80" t="str">
+      <c r="G10" s="80" t="str">
         <f t="shared" si="3"/>
         <v>18:#,Light_Cherry,</v>
       </c>
-      <c r="G10" s="59" t="str">
+      <c r="H10" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,</v>
       </c>
-      <c r="H10" s="59" t="str">
+      <c r="I10" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="75">
         <v>9</v>
       </c>
       <c r="B11" s="75">
         <v>19</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="77" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="77" t="s">
+      <c r="E11" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="79" t="str">
+      <c r="F11" s="79" t="str">
         <f t="shared" si="2"/>
         <v>19:#,</v>
       </c>
-      <c r="F11" s="80" t="str">
+      <c r="G11" s="80" t="str">
         <f t="shared" si="3"/>
         <v>19:#,Light_PacMan,</v>
       </c>
-      <c r="G11" s="59" t="str">
+      <c r="H11" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,</v>
       </c>
-      <c r="H11" s="59" t="str">
+      <c r="I11" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="12" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="75">
         <v>10</v>
       </c>
       <c r="B12" s="75">
         <v>20</v>
       </c>
-      <c r="C12" s="76" t="s">
+      <c r="C12" s="77" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="E12" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="E12" s="79" t="str">
+      <c r="F12" s="79" t="str">
         <f t="shared" si="2"/>
         <v>20:#,</v>
       </c>
-      <c r="F12" s="80" t="str">
+      <c r="G12" s="80" t="str">
         <f t="shared" si="3"/>
         <v>20:#,Light_Blinky,</v>
       </c>
-      <c r="G12" s="59" t="str">
+      <c r="H12" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,</v>
       </c>
-      <c r="H12" s="59" t="str">
+      <c r="I12" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="13" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="75">
         <v>11</v>
       </c>
       <c r="B13" s="75">
         <v>21</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="77" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="E13" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="E13" s="79" t="str">
+      <c r="F13" s="79" t="str">
         <f t="shared" si="2"/>
         <v>21:#,</v>
       </c>
-      <c r="F13" s="80" t="str">
+      <c r="G13" s="80" t="str">
         <f t="shared" si="3"/>
         <v>21:#,Light_Inky,</v>
       </c>
-      <c r="G13" s="59" t="str">
+      <c r="H13" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,</v>
       </c>
-      <c r="H13" s="59" t="str">
+      <c r="I13" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="14" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="75">
         <v>12</v>
       </c>
       <c r="B14" s="75">
         <v>22</v>
       </c>
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="77" t="s">
+      <c r="E14" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="79" t="str">
+      <c r="F14" s="79" t="str">
         <f t="shared" si="2"/>
         <v>22:#,</v>
       </c>
-      <c r="F14" s="80" t="str">
+      <c r="G14" s="80" t="str">
         <f t="shared" si="3"/>
         <v>22:#,Light_Sensor_Enable,</v>
       </c>
-      <c r="G14" s="59" t="str">
+      <c r="H14" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,</v>
       </c>
-      <c r="H14" s="59" t="str">
+      <c r="I14" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="15" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="75">
         <v>13</v>
       </c>
       <c r="B15" s="75">
         <v>23</v>
       </c>
-      <c r="C15" s="76" t="s">
+      <c r="C15" s="77" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="77" t="s">
+      <c r="E15" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="79" t="str">
+      <c r="F15" s="79" t="str">
         <f t="shared" si="2"/>
         <v>23:9####,</v>
       </c>
-      <c r="F15" s="80" t="str">
+      <c r="G15" s="80" t="str">
         <f t="shared" si="3"/>
         <v>23:9####,Light_Sensor_trigger_value,</v>
       </c>
-      <c r="G15" s="59" t="str">
+      <c r="H15" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,</v>
       </c>
-      <c r="H15" s="59" t="str">
+      <c r="I15" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="16" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="75">
         <v>14</v>
       </c>
       <c r="B16" s="75">
         <v>24</v>
       </c>
-      <c r="C16" s="76" t="s">
+      <c r="C16" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="D16" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="77" t="s">
+      <c r="E16" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="79" t="str">
+      <c r="F16" s="79" t="str">
         <f t="shared" si="2"/>
         <v>24:#,</v>
       </c>
-      <c r="F16" s="80" t="str">
+      <c r="G16" s="80" t="str">
         <f t="shared" si="3"/>
         <v>24:#,Night_Light_Enable_and_mode,</v>
       </c>
-      <c r="G16" s="59" t="str">
+      <c r="H16" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,</v>
       </c>
-      <c r="H16" s="59" t="str">
+      <c r="I16" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A17" s="75">
         <v>15</v>
       </c>
       <c r="B17" s="75">
         <v>25</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="77"/>
+      <c r="D17" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="77" t="s">
+      <c r="E17" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="79" t="str">
+      <c r="F17" s="79" t="str">
         <f t="shared" si="2"/>
         <v>25:#,</v>
       </c>
-      <c r="F17" s="80" t="str">
+      <c r="G17" s="80" t="str">
         <f t="shared" si="3"/>
         <v>25:#,(ip address preset),</v>
       </c>
-      <c r="G17" s="59" t="str">
+      <c r="H17" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,</v>
       </c>
-      <c r="H17" s="59" t="str">
+      <c r="I17" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="75">
         <v>16</v>
       </c>
       <c r="B18" s="75">
         <v>26</v>
       </c>
-      <c r="C18" s="76" t="s">
+      <c r="C18" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="77" t="s">
+      <c r="E18" s="77" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="79" t="str">
+      <c r="F18" s="79" t="str">
         <f t="shared" si="2"/>
         <v>26:#,</v>
       </c>
-      <c r="F18" s="80" t="str">
+      <c r="G18" s="80" t="str">
         <f t="shared" si="3"/>
         <v>26:#,Alarm_Enable,</v>
       </c>
-      <c r="G18" s="59" t="str">
+      <c r="H18" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,</v>
       </c>
-      <c r="H18" s="59" t="str">
+      <c r="I18" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="75">
         <v>17</v>
       </c>
       <c r="B19" s="75">
         <v>27</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="77" t="s">
+      <c r="E19" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="79" t="str">
+      <c r="F19" s="79" t="str">
         <f t="shared" si="2"/>
         <v>27:9########,</v>
       </c>
-      <c r="F19" s="80" t="str">
+      <c r="G19" s="80" t="str">
         <f t="shared" si="3"/>
         <v>27:9########,Alarm_Date,</v>
       </c>
-      <c r="G19" s="59" t="str">
+      <c r="H19" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,</v>
       </c>
-      <c r="H19" s="59" t="str">
+      <c r="I19" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="75">
         <v>18</v>
       </c>
       <c r="B20" s="75">
         <v>28</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="D20" s="77" t="s">
+      <c r="E20" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="79" t="str">
+      <c r="F20" s="79" t="str">
         <f t="shared" si="2"/>
         <v>28:9########,</v>
       </c>
-      <c r="F20" s="80" t="str">
+      <c r="G20" s="80" t="str">
         <f t="shared" si="3"/>
         <v>28:9########,Alarm_Time,</v>
       </c>
-      <c r="G20" s="59" t="str">
+      <c r="H20" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,</v>
       </c>
-      <c r="H20" s="59" t="str">
+      <c r="I20" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="21" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="75">
         <v>19</v>
       </c>
       <c r="B21" s="75">
         <v>29</v>
       </c>
-      <c r="C21" s="76" t="s">
+      <c r="C21" s="77" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="77" t="s">
+      <c r="E21" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="79" t="str">
+      <c r="F21" s="79" t="str">
         <f t="shared" si="2"/>
         <v>29:##,</v>
       </c>
-      <c r="F21" s="80" t="str">
+      <c r="G21" s="80" t="str">
         <f t="shared" si="3"/>
         <v>29:##,Performance_number,</v>
       </c>
-      <c r="G21" s="59" t="str">
+      <c r="H21" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,</v>
       </c>
-      <c r="H21" s="59" t="str">
+      <c r="I21" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="75">
         <v>20</v>
       </c>
       <c r="B22" s="75">
         <v>41</v>
       </c>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="77" t="s">
+      <c r="E22" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="79" t="str">
+      <c r="F22" s="79" t="str">
         <f t="shared" si="2"/>
         <v>41:#,</v>
       </c>
-      <c r="F22" s="80" t="str">
+      <c r="G22" s="80" t="str">
         <f t="shared" si="3"/>
         <v>41:#,Stayin_Game_Status,</v>
       </c>
-      <c r="G22" s="59" t="str">
+      <c r="H22" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,</v>
       </c>
-      <c r="H22" s="59" t="str">
+      <c r="I22" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="75">
         <v>21</v>
       </c>
       <c r="B23" s="75">
         <v>42</v>
       </c>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="77" t="s">
+        <v>217</v>
+      </c>
+      <c r="D23" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="77" t="s">
+      <c r="E23" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="79" t="str">
+      <c r="F23" s="79" t="str">
         <f t="shared" si="2"/>
         <v>42:#,</v>
       </c>
-      <c r="F23" s="80" t="str">
+      <c r="G23" s="80" t="str">
         <f t="shared" si="3"/>
         <v>42:#,myCharNum,</v>
       </c>
-      <c r="G23" s="59" t="str">
+      <c r="H23" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,</v>
       </c>
-      <c r="H23" s="59" t="str">
+      <c r="I23" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="75">
         <v>22</v>
       </c>
       <c r="B24" s="75">
         <v>43</v>
       </c>
-      <c r="C24" s="76" t="s">
+      <c r="C24" s="77" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="77" t="s">
+      <c r="E24" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="79" t="str">
+      <c r="F24" s="79" t="str">
         <f t="shared" si="2"/>
         <v>43:#######,</v>
       </c>
-      <c r="F24" s="80" t="str">
+      <c r="G24" s="80" t="str">
         <f t="shared" si="3"/>
         <v>43:#######,ActualName,</v>
       </c>
-      <c r="G24" s="59" t="str">
+      <c r="H24" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,</v>
       </c>
-      <c r="H24" s="59" t="str">
+      <c r="I24" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="A25" s="75">
         <v>23</v>
       </c>
       <c r="B25" s="75">
         <v>44</v>
       </c>
-      <c r="C25" s="76" t="s">
+      <c r="C25" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="77" t="s">
+      <c r="E25" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="79" t="str">
+      <c r="F25" s="79" t="str">
         <f t="shared" si="2"/>
         <v>44:9###,</v>
       </c>
-      <c r="F25" s="80" t="str">
+      <c r="G25" s="80" t="str">
         <f t="shared" si="3"/>
         <v>44:9###,BankAfterSpend,</v>
       </c>
-      <c r="G25" s="22" t="str">
+      <c r="H25" s="22" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,</v>
       </c>
-      <c r="H25" s="22" t="str">
+      <c r="I25" s="22" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="75">
         <v>24</v>
       </c>
       <c r="B26" s="75">
         <v>45</v>
       </c>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="77" t="s">
+        <v>220</v>
+      </c>
+      <c r="D26" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="77" t="s">
+      <c r="E26" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="79" t="str">
+      <c r="F26" s="79" t="str">
         <f t="shared" si="2"/>
         <v>45:9###,</v>
       </c>
-      <c r="F26" s="80" t="str">
+      <c r="G26" s="80" t="str">
         <f t="shared" si="3"/>
         <v>45:9###,Attack_balance,</v>
       </c>
-      <c r="G26" s="59" t="str">
+      <c r="H26" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,</v>
       </c>
-      <c r="H26" s="59" t="str">
+      <c r="I26" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="75">
         <v>25</v>
       </c>
       <c r="B27" s="75">
         <v>46</v>
       </c>
-      <c r="C27" s="76" t="s">
+      <c r="C27" s="77" t="s">
+        <v>221</v>
+      </c>
+      <c r="D27" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="77" t="s">
+      <c r="E27" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="E27" s="79" t="str">
+      <c r="F27" s="79" t="str">
         <f t="shared" si="2"/>
         <v>46:9######,</v>
       </c>
-      <c r="F27" s="80" t="str">
+      <c r="G27" s="80" t="str">
         <f t="shared" si="3"/>
         <v>46:9######,Attack_or_Donate_Flag,</v>
       </c>
-      <c r="G27" s="59" t="str">
+      <c r="H27" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,</v>
       </c>
-      <c r="H27" s="59" t="str">
+      <c r="I27" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A28" s="75">
         <v>26</v>
       </c>
       <c r="B28" s="75">
         <v>47</v>
       </c>
-      <c r="C28" s="76" t="s">
+      <c r="C28" s="77" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="77" t="s">
+      <c r="E28" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="79" t="str">
+      <c r="F28" s="79" t="str">
         <f t="shared" si="2"/>
         <v>47:9######,</v>
       </c>
-      <c r="F28" s="80" t="str">
+      <c r="G28" s="80" t="str">
         <f t="shared" si="3"/>
         <v>47:9######,Will_or_No (Pinky-Inky),</v>
       </c>
-      <c r="G28" s="59" t="str">
+      <c r="H28" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,</v>
       </c>
-      <c r="H28" s="59" t="str">
+      <c r="I28" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="29" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="75">
         <v>27</v>
       </c>
       <c r="B29" s="75">
         <v>48</v>
       </c>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="77" t="s">
+        <v>223</v>
+      </c>
+      <c r="D29" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="77" t="s">
+      <c r="E29" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="79" t="str">
+      <c r="F29" s="79" t="str">
         <f t="shared" si="2"/>
         <v>48:9######,</v>
       </c>
-      <c r="F29" s="80" t="str">
+      <c r="G29" s="80" t="str">
         <f t="shared" si="3"/>
         <v>48:9######,Mirror_or_No (Pinky-Inky),</v>
       </c>
-      <c r="G29" s="59" t="str">
+      <c r="H29" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,</v>
       </c>
-      <c r="H29" s="59" t="str">
+      <c r="I29" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="30" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="75">
         <v>28</v>
       </c>
       <c r="B30" s="75">
         <v>49</v>
       </c>
-      <c r="C30" s="76" t="s">
+      <c r="C30" s="77" t="s">
+        <v>224</v>
+      </c>
+      <c r="D30" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="77" t="s">
+      <c r="E30" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="79" t="str">
+      <c r="F30" s="79" t="str">
         <f t="shared" si="2"/>
         <v>49:9###,</v>
       </c>
-      <c r="F30" s="80" t="str">
+      <c r="G30" s="80" t="str">
         <f t="shared" si="3"/>
         <v>49:9###,Attack_or_Donate Pinky_Amnt,</v>
       </c>
-      <c r="G30" s="59" t="str">
+      <c r="H30" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,</v>
       </c>
-      <c r="H30" s="59" t="str">
+      <c r="I30" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="75">
         <v>29</v>
       </c>
       <c r="B31" s="75">
         <v>50</v>
       </c>
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="77" t="s">
+        <v>226</v>
+      </c>
+      <c r="D31" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="77" t="s">
+      <c r="E31" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="79" t="str">
+      <c r="F31" s="79" t="str">
         <f t="shared" si="2"/>
         <v>50:9###,</v>
       </c>
-      <c r="F31" s="80" t="str">
+      <c r="G31" s="80" t="str">
         <f t="shared" si="3"/>
         <v>50:9###,Attack_or_Donate Clyde_Amnt,</v>
       </c>
-      <c r="G31" s="59" t="str">
+      <c r="H31" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,</v>
       </c>
-      <c r="H31" s="59" t="str">
+      <c r="I31" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="32" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="75">
         <v>30</v>
       </c>
       <c r="B32" s="75">
         <v>51</v>
       </c>
-      <c r="C32" s="76" t="s">
+      <c r="C32" s="77" t="s">
+        <v>225</v>
+      </c>
+      <c r="D32" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="77" t="s">
+      <c r="E32" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="E32" s="79" t="str">
+      <c r="F32" s="79" t="str">
         <f t="shared" si="2"/>
         <v>51:9###,</v>
       </c>
-      <c r="F32" s="80" t="str">
+      <c r="G32" s="80" t="str">
         <f t="shared" si="3"/>
         <v>51:9###,Attack_or_Donate Cherry_Amnt,</v>
       </c>
-      <c r="G32" s="59" t="str">
+      <c r="H32" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,</v>
       </c>
-      <c r="H32" s="59" t="str">
+      <c r="I32" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="75">
         <v>31</v>
       </c>
       <c r="B33" s="75">
         <v>52</v>
       </c>
-      <c r="C33" s="76" t="s">
+      <c r="C33" s="77" t="s">
+        <v>227</v>
+      </c>
+      <c r="D33" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="77" t="s">
+      <c r="E33" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="79" t="str">
+      <c r="F33" s="79" t="str">
         <f t="shared" si="2"/>
         <v>52:9###,</v>
       </c>
-      <c r="F33" s="80" t="str">
+      <c r="G33" s="80" t="str">
         <f t="shared" si="3"/>
         <v>52:9###,Attack_or_Donate PacMan_Amnt,</v>
       </c>
-      <c r="G33" s="59" t="str">
+      <c r="H33" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,</v>
       </c>
-      <c r="H33" s="59" t="str">
+      <c r="I33" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="75">
         <v>32</v>
       </c>
       <c r="B34" s="75">
         <v>53</v>
       </c>
-      <c r="C34" s="76" t="s">
+      <c r="C34" s="77" t="s">
+        <v>228</v>
+      </c>
+      <c r="D34" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="77" t="s">
+      <c r="E34" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="E34" s="79" t="str">
+      <c r="F34" s="79" t="str">
         <f t="shared" si="2"/>
         <v>53:9###,</v>
       </c>
-      <c r="F34" s="80" t="str">
+      <c r="G34" s="80" t="str">
         <f t="shared" si="3"/>
         <v>53:9###,Attack_or_Donate Blinky_Amnt,</v>
       </c>
-      <c r="G34" s="59" t="str">
+      <c r="H34" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,</v>
       </c>
-      <c r="H34" s="59" t="str">
+      <c r="I34" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="75">
         <v>33</v>
       </c>
       <c r="B35" s="75">
         <v>54</v>
       </c>
-      <c r="C35" s="76" t="s">
+      <c r="C35" s="77" t="s">
+        <v>229</v>
+      </c>
+      <c r="D35" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D35" s="77" t="s">
+      <c r="E35" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="E35" s="79" t="str">
+      <c r="F35" s="79" t="str">
         <f t="shared" si="2"/>
         <v>54:9###,</v>
       </c>
-      <c r="F35" s="80" t="str">
+      <c r="G35" s="80" t="str">
         <f t="shared" si="3"/>
         <v>54:9###,Attack_or_Donate Inky_Amnt,</v>
       </c>
-      <c r="G35" s="59" t="str">
+      <c r="H35" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,</v>
       </c>
-      <c r="H35" s="59" t="str">
+      <c r="I35" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="75">
         <v>34</v>
       </c>
       <c r="B36" s="75">
         <v>55</v>
       </c>
-      <c r="C36" s="76" t="s">
+      <c r="C36" s="77" t="s">
+        <v>230</v>
+      </c>
+      <c r="D36" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="77" t="s">
+      <c r="E36" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="79" t="str">
+      <c r="F36" s="79" t="str">
         <f t="shared" si="2"/>
         <v>55:9######,</v>
       </c>
-      <c r="F36" s="80" t="str">
+      <c r="G36" s="80" t="str">
         <f t="shared" si="3"/>
         <v>55:9######,Mirror_Balances_Pinky_Values,</v>
       </c>
-      <c r="G36" s="59" t="str">
+      <c r="H36" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,</v>
       </c>
-      <c r="H36" s="59" t="str">
+      <c r="I36" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="75">
         <v>35</v>
       </c>
       <c r="B37" s="75">
         <v>56</v>
       </c>
-      <c r="C37" s="76" t="s">
+      <c r="C37" s="77" t="s">
+        <v>231</v>
+      </c>
+      <c r="D37" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="77" t="s">
+      <c r="E37" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="79" t="str">
+      <c r="F37" s="79" t="str">
         <f t="shared" si="2"/>
         <v>56:9######,</v>
       </c>
-      <c r="F37" s="80" t="str">
+      <c r="G37" s="80" t="str">
         <f t="shared" si="3"/>
         <v>56:9######,Mirror_Balances_Clyde_Values,</v>
       </c>
-      <c r="G37" s="59" t="str">
+      <c r="H37" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,</v>
       </c>
-      <c r="H37" s="59" t="str">
+      <c r="I37" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A38" s="75">
         <v>36</v>
       </c>
       <c r="B38" s="75">
         <v>57</v>
       </c>
-      <c r="C38" s="76" t="s">
+      <c r="C38" s="77" t="s">
+        <v>232</v>
+      </c>
+      <c r="D38" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="77" t="s">
+      <c r="E38" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="79" t="str">
+      <c r="F38" s="79" t="str">
         <f t="shared" si="2"/>
         <v>57:9######,</v>
       </c>
-      <c r="F38" s="80" t="str">
+      <c r="G38" s="80" t="str">
         <f t="shared" si="3"/>
         <v>57:9######,Mirror_Balances_Cherry_Values,</v>
       </c>
-      <c r="G38" s="59" t="str">
+      <c r="H38" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,</v>
       </c>
-      <c r="H38" s="59" t="str">
+      <c r="I38" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="39" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="75"/>
       <c r="B39" s="75">
         <v>58</v>
       </c>
-      <c r="C39" s="76" t="s">
+      <c r="C39" s="77" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="77" t="s">
+      <c r="E39" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="E39" s="79" t="str">
+      <c r="F39" s="79" t="str">
         <f t="shared" si="2"/>
         <v>58:9######,</v>
       </c>
-      <c r="F39" s="80" t="str">
+      <c r="G39" s="80" t="str">
         <f t="shared" si="3"/>
         <v>58:9######,Mirror_Balances_Pacman_Values,</v>
       </c>
-      <c r="G39" s="59" t="str">
+      <c r="H39" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,</v>
       </c>
-      <c r="H39" s="59" t="str">
+      <c r="I39" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="75"/>
       <c r="B40" s="75">
         <v>59</v>
       </c>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="77" t="s">
+      <c r="E40" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="79" t="str">
+      <c r="F40" s="79" t="str">
         <f t="shared" si="2"/>
         <v>59:9######,</v>
       </c>
-      <c r="F40" s="80" t="str">
+      <c r="G40" s="80" t="str">
         <f t="shared" si="3"/>
         <v>59:9######,Mirror_Balances_Blinky_Values,</v>
       </c>
-      <c r="G40" s="59" t="str">
+      <c r="H40" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,</v>
       </c>
-      <c r="H40" s="59" t="str">
+      <c r="I40" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A41" s="75"/>
       <c r="B41" s="75">
         <v>60</v>
       </c>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="D41" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="77" t="s">
+      <c r="E41" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="E41" s="79" t="str">
+      <c r="F41" s="79" t="str">
         <f t="shared" si="2"/>
         <v>60:9######,</v>
       </c>
-      <c r="F41" s="80" t="str">
+      <c r="G41" s="80" t="str">
         <f t="shared" si="3"/>
         <v>60:9######,Mirror_Balances_Inky_Values,</v>
       </c>
-      <c r="G41" s="59" t="str">
+      <c r="H41" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,</v>
       </c>
-      <c r="H41" s="59" t="str">
+      <c r="I41" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="42" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A42" s="75"/>
       <c r="B42" s="75">
         <v>61</v>
       </c>
-      <c r="C42" s="76" t="s">
+      <c r="C42" s="77" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="77" t="s">
+      <c r="E42" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="E42" s="79" t="str">
+      <c r="F42" s="79" t="str">
         <f t="shared" si="2"/>
         <v>61:#######,</v>
       </c>
-      <c r="F42" s="80" t="str">
+      <c r="G42" s="80" t="str">
         <f t="shared" si="3"/>
         <v>61:#######,Pinky_Rename,</v>
       </c>
-      <c r="G42" s="59" t="str">
+      <c r="H42" s="59" t="str">
         <f t="shared" si="0"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,</v>
       </c>
-      <c r="H42" s="59" t="str">
+      <c r="I42" s="59" t="str">
         <f t="shared" si="1"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="75"/>
       <c r="B43" s="75">
         <v>62</v>
       </c>
-      <c r="C43" s="76" t="s">
+      <c r="C43" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="D43" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="77" t="s">
+      <c r="E43" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="79" t="str">
+      <c r="F43" s="79" t="str">
         <f t="shared" si="2"/>
         <v>62:#######,</v>
       </c>
-      <c r="F43" s="80" t="str">
+      <c r="G43" s="80" t="str">
         <f t="shared" si="3"/>
         <v>62:#######,Clyde_Rename,</v>
       </c>
-      <c r="G43" s="59" t="str">
-        <f t="shared" ref="G43:G51" si="4">CONCATENATE(G42,E43)</f>
+      <c r="H43" s="59" t="str">
+        <f t="shared" ref="H43:H51" si="4">CONCATENATE(H42,F43)</f>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,</v>
       </c>
-      <c r="H43" s="59" t="str">
-        <f t="shared" ref="H43:H51" si="5">CONCATENATE(H42,F43)</f>
+      <c r="I43" s="59" t="str">
+        <f t="shared" ref="I43:I51" si="5">CONCATENATE(I42,G43)</f>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="44" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A44" s="75"/>
       <c r="B44" s="75">
         <v>63</v>
       </c>
-      <c r="C44" s="76" t="s">
+      <c r="C44" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="77" t="s">
+      <c r="E44" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="79" t="str">
+      <c r="F44" s="79" t="str">
         <f t="shared" si="2"/>
         <v>63:#######,</v>
       </c>
-      <c r="F44" s="80" t="str">
+      <c r="G44" s="80" t="str">
         <f t="shared" si="3"/>
         <v>63:#######,Cherry_Rename,</v>
       </c>
-      <c r="G44" s="59" t="str">
+      <c r="H44" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,</v>
       </c>
-      <c r="H44" s="59" t="str">
+      <c r="I44" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="45" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A45" s="75"/>
       <c r="B45" s="75">
         <v>64</v>
       </c>
-      <c r="C45" s="76" t="s">
+      <c r="C45" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="D45" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="77" t="s">
+      <c r="E45" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="E45" s="79" t="str">
+      <c r="F45" s="79" t="str">
         <f t="shared" si="2"/>
         <v>64:#######,</v>
       </c>
-      <c r="F45" s="80" t="str">
+      <c r="G45" s="80" t="str">
         <f t="shared" si="3"/>
         <v>64:#######,PacMan_Rename,</v>
       </c>
-      <c r="G45" s="59" t="str">
+      <c r="H45" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,</v>
       </c>
-      <c r="H45" s="59" t="str">
+      <c r="I45" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="46" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="75"/>
       <c r="B46" s="75">
         <v>65</v>
       </c>
-      <c r="C46" s="76" t="s">
+      <c r="C46" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="D46" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="77" t="s">
+      <c r="E46" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="E46" s="79" t="str">
+      <c r="F46" s="79" t="str">
         <f t="shared" si="2"/>
         <v>65:#######,</v>
       </c>
-      <c r="F46" s="80" t="str">
+      <c r="G46" s="80" t="str">
         <f t="shared" si="3"/>
         <v>65:#######,Blinky_Rename,</v>
       </c>
-      <c r="G46" s="59" t="str">
+      <c r="H46" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,65:#######,</v>
       </c>
-      <c r="H46" s="59" t="str">
+      <c r="I46" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,65:#######,Blinky_Rename,</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="47" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A47" s="75"/>
       <c r="B47" s="75">
         <v>66</v>
       </c>
-      <c r="C47" s="76" t="s">
+      <c r="C47" s="77" t="s">
+        <v>241</v>
+      </c>
+      <c r="D47" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="77" t="s">
+      <c r="E47" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="E47" s="79" t="str">
+      <c r="F47" s="79" t="str">
         <f t="shared" si="2"/>
         <v>66:#######,</v>
       </c>
-      <c r="F47" s="80" t="str">
+      <c r="G47" s="80" t="str">
         <f t="shared" si="3"/>
         <v>66:#######,Inky_Rename,</v>
       </c>
-      <c r="G47" s="59" t="str">
+      <c r="H47" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,65:#######,66:#######,</v>
       </c>
-      <c r="H47" s="59" t="str">
+      <c r="I47" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,65:#######,Blinky_Rename,66:#######,Inky_Rename,</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="75"/>
       <c r="B48" s="75">
         <v>67</v>
       </c>
-      <c r="C48" s="76"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="79"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="59" t="str">
+      <c r="C48" s="77"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,65:#######,66:#######,</v>
       </c>
-      <c r="H48" s="59" t="str">
+      <c r="I48" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,65:#######,Blinky_Rename,66:#######,Inky_Rename,</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="49" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="75"/>
       <c r="B49" s="75">
         <v>68</v>
       </c>
-      <c r="C49" s="76"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="79"/>
-      <c r="F49" s="80"/>
-      <c r="G49" s="59" t="str">
+      <c r="C49" s="77"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,65:#######,66:#######,</v>
       </c>
-      <c r="H49" s="59" t="str">
+      <c r="I49" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,65:#######,Blinky_Rename,66:#######,Inky_Rename,</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="50" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="75"/>
       <c r="B50" s="75">
         <v>69</v>
       </c>
-      <c r="C50" s="76"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="80"/>
-      <c r="G50" s="59" t="str">
+      <c r="C50" s="77"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="77"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,65:#######,66:#######,</v>
       </c>
-      <c r="H50" s="59" t="str">
+      <c r="I50" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,65:#######,Blinky_Rename,66:#######,Inky_Rename,</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="51" customFormat="1" ht="15.75" customHeight="1">
+    <row r="51" spans="1:9" s="51" customFormat="1" ht="15.75" customHeight="1">
       <c r="A51" s="75"/>
       <c r="B51" s="75">
         <v>70</v>
       </c>
-      <c r="C51" s="76"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="79"/>
-      <c r="F51" s="80"/>
-      <c r="G51" s="59" t="str">
+      <c r="C51" s="77"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="80"/>
+      <c r="H51" s="59" t="str">
         <f t="shared" si="4"/>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,65:#######,66:#######,</v>
       </c>
-      <c r="H51" s="59" t="str">
+      <c r="I51" s="59" t="str">
         <f t="shared" si="5"/>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,65:#######,Blinky_Rename,66:#######,Inky_Rename,</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1">
-      <c r="C52" s="38"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="41"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1">
-      <c r="C53" s="38"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="41"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1">
-      <c r="E54" s="41" t="str">
-        <f>+H51</f>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1">
+      <c r="C52" s="39"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="41"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1">
+      <c r="C53" s="39"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="41"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1">
+      <c r="F54" s="41" t="str">
+        <f>+I51</f>
         <v>11:#,Master_Enable,12:#,Light_Enable,13:#,Sound_Enable,14:#,Motion_Enable,15:#,Clock_Enable,16:#,Light_Pinky,17:#,Light_Clyde,18:#,Light_Cherry,19:#,Light_PacMan,20:#,Light_Blinky,21:#,Light_Inky,22:#,Light_Sensor_Enable,23:9####,Light_Sensor_trigger_value,24:#,Night_Light_Enable_and_mode,25:#,(ip address preset),26:#,Alarm_Enable,27:9########,Alarm_Date,28:9########,Alarm_Time,29:##,Performance_number,41:#,Stayin_Game_Status,42:#,myCharNum,43:#######,ActualName,44:9###,BankAfterSpend,45:9###,Attack_balance,46:9######,Attack_or_Donate_Flag,47:9######,Will_or_No (Pinky-Inky),48:9######,Mirror_or_No (Pinky-Inky),49:9###,Attack_or_Donate Pinky_Amnt,50:9###,Attack_or_Donate Clyde_Amnt,51:9###,Attack_or_Donate Cherry_Amnt,52:9###,Attack_or_Donate PacMan_Amnt,53:9###,Attack_or_Donate Blinky_Amnt,54:9###,Attack_or_Donate Inky_Amnt,55:9######,Mirror_Balances_Pinky_Values,56:9######,Mirror_Balances_Clyde_Values,57:9######,Mirror_Balances_Cherry_Values,58:9######,Mirror_Balances_Pacman_Values,59:9######,Mirror_Balances_Blinky_Values,60:9######,Mirror_Balances_Inky_Values,61:#######,Pinky_Rename,62:#######,Clyde_Rename,63:#######,Cherry_Rename,64:#######,PacMan_Rename,65:#######,Blinky_Rename,66:#######,Inky_Rename,</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="E55" s="27" t="str">
-        <f>G51</f>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="F55" s="27" t="str">
+        <f>H51</f>
         <v>&gt;&gt;&gt;&gt;&gt;11:#,12:#,13:#,14:#,15:#,16:#,17:#,18:#,19:#,20:#,21:#,22:#,23:9####,24:#,25:#,26:#,27:9########,28:9########,29:##,41:#,42:#,43:#######,44:9###,45:9###,46:9######,47:9######,48:9######,49:9###,50:9###,51:9###,52:9###,53:9###,54:9###,55:9######,56:9######,57:9######,58:9######,59:9######,60:9######,61:#######,62:#######,63:#######,64:#######,65:#######,66:#######,</v>
       </c>
-      <c r="F55" s="27"/>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1">
-      <c r="G57"/>
+      <c r="G55" s="27"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" customHeight="1">
       <c r="H57"/>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" customHeight="1">
-      <c r="G58"/>
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1">
       <c r="H58"/>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" customHeight="1">
-      <c r="G59"/>
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1">
       <c r="H59"/>
-    </row>
-    <row r="60" spans="1:8" ht="15.75" customHeight="1">
-      <c r="G60"/>
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1">
       <c r="H60"/>
-    </row>
-    <row r="61" spans="1:8" ht="15.75" customHeight="1">
-      <c r="G61"/>
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" customHeight="1">
       <c r="H61"/>
+      <c r="I61"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
@@ -4459,10 +4757,1479 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11">
+      <c r="H2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <f>COMBINED!B3</f>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <f>LEN(COMBINED!D3)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="str">
+        <f>+COMBINED!E3</f>
+        <v>Master_Enable</v>
+      </c>
+      <c r="F3" t="str">
+        <f>COMBINED!C3</f>
+        <v>M_EN</v>
+      </c>
+      <c r="G3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>244</v>
+      </c>
+      <c r="J3" t="s">
+        <v>245</v>
+      </c>
+      <c r="K3" t="str">
+        <f>CONCATENATE(F3,G3,H3,I3,J3,D3)</f>
+        <v>M_EN = (data_line[9]-48);   // Master_Enable</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <f>COMBINED!B4</f>
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <f>LEN(COMBINED!D4)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" t="str">
+        <f>+COMBINED!E4</f>
+        <v>Light_Enable</v>
+      </c>
+      <c r="F4" t="str">
+        <f>COMBINED!C4</f>
+        <v>L_EN</v>
+      </c>
+      <c r="G4" t="s">
+        <v>243</v>
+      </c>
+      <c r="H4">
+        <f>+H3+5</f>
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>244</v>
+      </c>
+      <c r="J4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K15" si="0">CONCATENATE(F4,G4,H4,I4,J4,D4)</f>
+        <v>L_EN = (data_line[14]-48);   // Light_Enable</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <f>COMBINED!B5</f>
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <f>LEN(COMBINED!D5)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="str">
+        <f>+COMBINED!E5</f>
+        <v>Sound_Enable</v>
+      </c>
+      <c r="F5" t="str">
+        <f>COMBINED!C5</f>
+        <v>S_EN</v>
+      </c>
+      <c r="G5" t="s">
+        <v>243</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H40" si="1">+H4+5</f>
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>244</v>
+      </c>
+      <c r="J5" t="s">
+        <v>245</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>S_EN = (data_line[19]-48);   // Sound_Enable</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <f>COMBINED!B6</f>
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <f>LEN(COMBINED!D6)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" t="str">
+        <f>+COMBINED!E6</f>
+        <v>Motion_Enable</v>
+      </c>
+      <c r="F6" t="str">
+        <f>COMBINED!C6</f>
+        <v>MO_EN</v>
+      </c>
+      <c r="G6" t="s">
+        <v>243</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>244</v>
+      </c>
+      <c r="J6" t="s">
+        <v>245</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>MO_EN = (data_line[24]-48);   // Motion_Enable</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <f>COMBINED!B7</f>
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <f>LEN(COMBINED!D7)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" t="str">
+        <f>+COMBINED!E7</f>
+        <v>Clock_Enable</v>
+      </c>
+      <c r="F7" t="str">
+        <f>COMBINED!C7</f>
+        <v>CL_EN</v>
+      </c>
+      <c r="G7" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>244</v>
+      </c>
+      <c r="J7" t="s">
+        <v>245</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>CL_EN = (data_line[29]-48);   // Clock_Enable</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <f>COMBINED!B8</f>
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <f>LEN(COMBINED!D8)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" t="str">
+        <f>+COMBINED!E8</f>
+        <v>Light_Pinky</v>
+      </c>
+      <c r="F8" t="str">
+        <f>COMBINED!C8</f>
+        <v>PIN_EN</v>
+      </c>
+      <c r="G8" t="s">
+        <v>243</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>244</v>
+      </c>
+      <c r="J8" t="s">
+        <v>245</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>PIN_EN = (data_line[34]-48);   // Light_Pinky</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <f>COMBINED!B9</f>
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <f>LEN(COMBINED!D9)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" t="str">
+        <f>+COMBINED!E9</f>
+        <v>Light_Clyde</v>
+      </c>
+      <c r="F9" t="str">
+        <f>COMBINED!C9</f>
+        <v>CLY_EN</v>
+      </c>
+      <c r="G9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>244</v>
+      </c>
+      <c r="J9" t="s">
+        <v>245</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>CLY_EN = (data_line[39]-48);   // Light_Clyde</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <f>COMBINED!B10</f>
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <f>LEN(COMBINED!D10)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" t="str">
+        <f>+COMBINED!E10</f>
+        <v>Light_Cherry</v>
+      </c>
+      <c r="F10" t="str">
+        <f>COMBINED!C10</f>
+        <v>CHE_EN</v>
+      </c>
+      <c r="G10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>244</v>
+      </c>
+      <c r="J10" t="s">
+        <v>245</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>CHE_EN = (data_line[44]-48);   // Light_Cherry</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <f>COMBINED!B11</f>
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <f>LEN(COMBINED!D11)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="str">
+        <f>+COMBINED!E11</f>
+        <v>Light_PacMan</v>
+      </c>
+      <c r="F11" t="str">
+        <f>COMBINED!C11</f>
+        <v>PAC_EN</v>
+      </c>
+      <c r="G11" t="s">
+        <v>243</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I11" t="s">
+        <v>244</v>
+      </c>
+      <c r="J11" t="s">
+        <v>245</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>PAC_EN = (data_line[49]-48);   // Light_PacMan</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <f>COMBINED!B12</f>
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <f>LEN(COMBINED!D12)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" t="str">
+        <f>+COMBINED!E12</f>
+        <v>Light_Blinky</v>
+      </c>
+      <c r="F12" t="str">
+        <f>COMBINED!C12</f>
+        <v>BLI_EN</v>
+      </c>
+      <c r="G12" t="s">
+        <v>243</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>244</v>
+      </c>
+      <c r="J12" t="s">
+        <v>245</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>BLI_EN = (data_line[54]-48);   // Light_Blinky</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <f>COMBINED!B13</f>
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <f>LEN(COMBINED!D13)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" t="str">
+        <f>+COMBINED!E13</f>
+        <v>Light_Inky</v>
+      </c>
+      <c r="F13" t="str">
+        <f>COMBINED!C13</f>
+        <v>INK_EN</v>
+      </c>
+      <c r="G13" t="s">
+        <v>243</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>244</v>
+      </c>
+      <c r="J13" t="s">
+        <v>245</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>INK_EN = (data_line[59]-48);   // Light_Inky</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <f>COMBINED!B14</f>
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <f>LEN(COMBINED!D14)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" t="str">
+        <f>+COMBINED!E14</f>
+        <v>Light_Sensor_Enable</v>
+      </c>
+      <c r="F14" t="str">
+        <f>COMBINED!C14</f>
+        <v>LS_EN</v>
+      </c>
+      <c r="G14" t="s">
+        <v>243</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" t="s">
+        <v>245</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>LS_EN = (data_line[64]-48);   // Light_Sensor_Enable</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <f>COMBINED!B15</f>
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <f>LEN(COMBINED!D15)+4</f>
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" t="str">
+        <f>+COMBINED!E15</f>
+        <v>Light_Sensor_trigger_value</v>
+      </c>
+      <c r="F15" t="str">
+        <f>COMBINED!C15</f>
+        <v>LS_VAL</v>
+      </c>
+      <c r="G15" t="s">
+        <v>243</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="I15" t="s">
+        <v>244</v>
+      </c>
+      <c r="J15" t="s">
+        <v>245</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>LS_VAL = (data_line[69]-48);   // Light_Sensor_trigger_value</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <f>COMBINED!B16</f>
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <f>LEN(COMBINED!D16)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" t="str">
+        <f>+COMBINED!E16</f>
+        <v>Night_Light_Enable_and_mode</v>
+      </c>
+      <c r="F16" t="str">
+        <f>COMBINED!C16</f>
+        <v>NL_EN</v>
+      </c>
+      <c r="G16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H16" s="93">
+        <f>+H15+5+3</f>
+        <v>77</v>
+      </c>
+      <c r="I16" t="s">
+        <v>244</v>
+      </c>
+      <c r="J16" t="s">
+        <v>245</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" ref="K4:K40" si="2">CONCATENATE(F16,G16,H16,I16,J16,D16)</f>
+        <v>NL_EN = (data_line[77]-48);   // Night_Light_Enable_and_mode</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <f>COMBINED!B18</f>
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <f>LEN(COMBINED!D18)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" t="str">
+        <f>+COMBINED!E18</f>
+        <v>Alarm_Enable</v>
+      </c>
+      <c r="F17" t="str">
+        <f>COMBINED!C18</f>
+        <v>ALM_EN</v>
+      </c>
+      <c r="G17" t="s">
+        <v>243</v>
+      </c>
+      <c r="H17">
+        <f>+H16+5</f>
+        <v>82</v>
+      </c>
+      <c r="I17" t="s">
+        <v>244</v>
+      </c>
+      <c r="J17" t="s">
+        <v>245</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="2"/>
+        <v>ALM_EN = (data_line[82]-48);   // Alarm_Enable</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <f>COMBINED!B19</f>
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <f>LEN(COMBINED!D19)+4</f>
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" t="str">
+        <f>+COMBINED!E19</f>
+        <v>Alarm_Date</v>
+      </c>
+      <c r="F18" t="str">
+        <f>COMBINED!C19</f>
+        <v>ALM_DATE</v>
+      </c>
+      <c r="G18" t="s">
+        <v>243</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="I18" t="s">
+        <v>244</v>
+      </c>
+      <c r="J18" t="s">
+        <v>245</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="2"/>
+        <v>ALM_DATE = (data_line[87]-48);   // Alarm_Date</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <f>COMBINED!B20</f>
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <f>LEN(COMBINED!D20)+4</f>
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" t="str">
+        <f>+COMBINED!E20</f>
+        <v>Alarm_Time</v>
+      </c>
+      <c r="F19" t="str">
+        <f>COMBINED!C20</f>
+        <v>ALM_TIME</v>
+      </c>
+      <c r="G19" t="s">
+        <v>243</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="I19" t="s">
+        <v>244</v>
+      </c>
+      <c r="J19" t="s">
+        <v>245</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="2"/>
+        <v>ALM_TIME = (data_line[92]-48);   // Alarm_Time</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <f>COMBINED!B21</f>
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <f>LEN(COMBINED!D21)+4</f>
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" t="str">
+        <f>+COMBINED!E21</f>
+        <v>Performance_number</v>
+      </c>
+      <c r="F20" t="str">
+        <f>COMBINED!C21</f>
+        <v>PERF_NUM</v>
+      </c>
+      <c r="G20" t="s">
+        <v>243</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="I20" t="s">
+        <v>244</v>
+      </c>
+      <c r="J20" t="s">
+        <v>245</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="2"/>
+        <v>PERF_NUM = (data_line[97]-48);   // Performance_number</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <f>COMBINED!B22</f>
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <f>LEN(COMBINED!D22)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" t="str">
+        <f>+COMBINED!E22</f>
+        <v>Stayin_Game_Status</v>
+      </c>
+      <c r="F21" t="str">
+        <f>COMBINED!C22</f>
+        <v>GAME_STATUS</v>
+      </c>
+      <c r="G21" t="s">
+        <v>243</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="I21" t="s">
+        <v>244</v>
+      </c>
+      <c r="J21" t="s">
+        <v>245</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="2"/>
+        <v>GAME_STATUS = (data_line[102]-48);   // Stayin_Game_Status</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <f>COMBINED!B23</f>
+        <v>42</v>
+      </c>
+      <c r="B22">
+        <f>LEN(COMBINED!D23)+4</f>
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" t="str">
+        <f>+COMBINED!E23</f>
+        <v>myCharNum</v>
+      </c>
+      <c r="F22" t="str">
+        <f>COMBINED!C23</f>
+        <v>MY_CHAR_NUM</v>
+      </c>
+      <c r="G22" t="s">
+        <v>243</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="I22" t="s">
+        <v>244</v>
+      </c>
+      <c r="J22" t="s">
+        <v>245</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="2"/>
+        <v>MY_CHAR_NUM = (data_line[107]-48);   // myCharNum</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <f>COMBINED!B24</f>
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <f>LEN(COMBINED!D24)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="str">
+        <f>+COMBINED!E24</f>
+        <v>ActualName</v>
+      </c>
+      <c r="F23" t="str">
+        <f>COMBINED!C24</f>
+        <v>ACT_NAME</v>
+      </c>
+      <c r="G23" t="s">
+        <v>243</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="I23" t="s">
+        <v>244</v>
+      </c>
+      <c r="J23" t="s">
+        <v>245</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="2"/>
+        <v>ACT_NAME = (data_line[112]-48);   // ActualName</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <f>COMBINED!B25</f>
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <f>LEN(COMBINED!D25)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="str">
+        <f>+COMBINED!E25</f>
+        <v>BankAfterSpend</v>
+      </c>
+      <c r="F24" t="str">
+        <f>COMBINED!C25</f>
+        <v>BANK_AFTER_SPEND</v>
+      </c>
+      <c r="G24" t="s">
+        <v>243</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="I24" t="s">
+        <v>244</v>
+      </c>
+      <c r="J24" t="s">
+        <v>245</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="2"/>
+        <v>BANK_AFTER_SPEND = (data_line[117]-48);   // BankAfterSpend</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <f>COMBINED!B26</f>
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <f>LEN(COMBINED!D26)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="str">
+        <f>+COMBINED!E26</f>
+        <v>Attack_balance</v>
+      </c>
+      <c r="F25" t="str">
+        <f>COMBINED!C26</f>
+        <v>ATTACK_BAL</v>
+      </c>
+      <c r="G25" t="s">
+        <v>243</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="I25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J25" t="s">
+        <v>245</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="2"/>
+        <v>ATTACK_BAL = (data_line[122]-48);   // Attack_balance</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <f>COMBINED!B27</f>
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <f>LEN(COMBINED!D27)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="str">
+        <f>+COMBINED!E27</f>
+        <v>Attack_or_Donate_Flag</v>
+      </c>
+      <c r="F26" t="str">
+        <f>COMBINED!C27</f>
+        <v>ATT_DON</v>
+      </c>
+      <c r="G26" t="s">
+        <v>243</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="I26" t="s">
+        <v>244</v>
+      </c>
+      <c r="J26" t="s">
+        <v>245</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="2"/>
+        <v>ATT_DON = (data_line[127]-48);   // Attack_or_Donate_Flag</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <f>COMBINED!B28</f>
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <f>LEN(COMBINED!D28)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" t="str">
+        <f>+COMBINED!E28</f>
+        <v>Will_or_No (Pinky-Inky)</v>
+      </c>
+      <c r="F27" t="str">
+        <f>COMBINED!C28</f>
+        <v>WILL_NO</v>
+      </c>
+      <c r="G27" t="s">
+        <v>243</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="I27" t="s">
+        <v>244</v>
+      </c>
+      <c r="J27" t="s">
+        <v>245</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="2"/>
+        <v>WILL_NO = (data_line[132]-48);   // Will_or_No (Pinky-Inky)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <f>COMBINED!B29</f>
+        <v>48</v>
+      </c>
+      <c r="B28">
+        <f>LEN(COMBINED!D29)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="str">
+        <f>+COMBINED!E29</f>
+        <v>Mirror_or_No (Pinky-Inky)</v>
+      </c>
+      <c r="F28" t="str">
+        <f>COMBINED!C29</f>
+        <v>MIRROR_NO</v>
+      </c>
+      <c r="G28" t="s">
+        <v>243</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="I28" t="s">
+        <v>244</v>
+      </c>
+      <c r="J28" t="s">
+        <v>245</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="2"/>
+        <v>MIRROR_NO = (data_line[137]-48);   // Mirror_or_No (Pinky-Inky)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <f>COMBINED!B30</f>
+        <v>49</v>
+      </c>
+      <c r="B29">
+        <f>LEN(COMBINED!D30)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="str">
+        <f>+COMBINED!E30</f>
+        <v>Attack_or_Donate Pinky_Amnt</v>
+      </c>
+      <c r="F29" t="str">
+        <f>COMBINED!C30</f>
+        <v>AD_PIN</v>
+      </c>
+      <c r="G29" t="s">
+        <v>243</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>142</v>
+      </c>
+      <c r="I29" t="s">
+        <v>244</v>
+      </c>
+      <c r="J29" t="s">
+        <v>245</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="2"/>
+        <v>AD_PIN = (data_line[142]-48);   // Attack_or_Donate Pinky_Amnt</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <f>COMBINED!B31</f>
+        <v>50</v>
+      </c>
+      <c r="B30">
+        <f>LEN(COMBINED!D31)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" t="str">
+        <f>+COMBINED!E31</f>
+        <v>Attack_or_Donate Clyde_Amnt</v>
+      </c>
+      <c r="F30" t="str">
+        <f>COMBINED!C31</f>
+        <v>AD_CLY</v>
+      </c>
+      <c r="G30" t="s">
+        <v>243</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+      <c r="I30" t="s">
+        <v>244</v>
+      </c>
+      <c r="J30" t="s">
+        <v>245</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="2"/>
+        <v>AD_CLY = (data_line[147]-48);   // Attack_or_Donate Clyde_Amnt</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <f>COMBINED!B32</f>
+        <v>51</v>
+      </c>
+      <c r="B31">
+        <f>LEN(COMBINED!D32)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" t="str">
+        <f>+COMBINED!E32</f>
+        <v>Attack_or_Donate Cherry_Amnt</v>
+      </c>
+      <c r="F31" t="str">
+        <f>COMBINED!C32</f>
+        <v>AD_CHE</v>
+      </c>
+      <c r="G31" t="s">
+        <v>243</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>152</v>
+      </c>
+      <c r="I31" t="s">
+        <v>244</v>
+      </c>
+      <c r="J31" t="s">
+        <v>245</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="2"/>
+        <v>AD_CHE = (data_line[152]-48);   // Attack_or_Donate Cherry_Amnt</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32">
+        <f>COMBINED!B33</f>
+        <v>52</v>
+      </c>
+      <c r="B32">
+        <f>LEN(COMBINED!D33)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" t="str">
+        <f>+COMBINED!E33</f>
+        <v>Attack_or_Donate PacMan_Amnt</v>
+      </c>
+      <c r="F32" t="str">
+        <f>COMBINED!C33</f>
+        <v>AD_PAC</v>
+      </c>
+      <c r="G32" t="s">
+        <v>243</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+      <c r="I32" t="s">
+        <v>244</v>
+      </c>
+      <c r="J32" t="s">
+        <v>245</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="2"/>
+        <v>AD_PAC = (data_line[157]-48);   // Attack_or_Donate PacMan_Amnt</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33">
+        <f>COMBINED!B34</f>
+        <v>53</v>
+      </c>
+      <c r="B33">
+        <f>LEN(COMBINED!D34)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" t="str">
+        <f>+COMBINED!E34</f>
+        <v>Attack_or_Donate Blinky_Amnt</v>
+      </c>
+      <c r="F33" t="str">
+        <f>COMBINED!C34</f>
+        <v>AD_BLI</v>
+      </c>
+      <c r="G33" t="s">
+        <v>243</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="I33" t="s">
+        <v>244</v>
+      </c>
+      <c r="J33" t="s">
+        <v>245</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="2"/>
+        <v>AD_BLI = (data_line[162]-48);   // Attack_or_Donate Blinky_Amnt</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34">
+        <f>COMBINED!B35</f>
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <f>LEN(COMBINED!D35)+4</f>
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="str">
+        <f>+COMBINED!E35</f>
+        <v>Attack_or_Donate Inky_Amnt</v>
+      </c>
+      <c r="F34" t="str">
+        <f>COMBINED!C35</f>
+        <v>AD_INK</v>
+      </c>
+      <c r="G34" t="s">
+        <v>243</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+      <c r="I34" t="s">
+        <v>244</v>
+      </c>
+      <c r="J34" t="s">
+        <v>245</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="2"/>
+        <v>AD_INK = (data_line[167]-48);   // Attack_or_Donate Inky_Amnt</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <f>COMBINED!B36</f>
+        <v>55</v>
+      </c>
+      <c r="B35">
+        <f>LEN(COMBINED!D36)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" t="str">
+        <f>+COMBINED!E36</f>
+        <v>Mirror_Balances_Pinky_Values</v>
+      </c>
+      <c r="F35" t="str">
+        <f>COMBINED!C36</f>
+        <v>MB_PIN</v>
+      </c>
+      <c r="G35" t="s">
+        <v>243</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>172</v>
+      </c>
+      <c r="I35" t="s">
+        <v>244</v>
+      </c>
+      <c r="J35" t="s">
+        <v>245</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="2"/>
+        <v>MB_PIN = (data_line[172]-48);   // Mirror_Balances_Pinky_Values</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36">
+        <f>COMBINED!B37</f>
+        <v>56</v>
+      </c>
+      <c r="B36">
+        <f>LEN(COMBINED!D37)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="str">
+        <f>+COMBINED!E37</f>
+        <v>Mirror_Balances_Clyde_Values</v>
+      </c>
+      <c r="F36" t="str">
+        <f>COMBINED!C37</f>
+        <v>MB_CLY</v>
+      </c>
+      <c r="G36" t="s">
+        <v>243</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+      <c r="I36" t="s">
+        <v>244</v>
+      </c>
+      <c r="J36" t="s">
+        <v>245</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="2"/>
+        <v>MB_CLY = (data_line[177]-48);   // Mirror_Balances_Clyde_Values</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37">
+        <f>COMBINED!B38</f>
+        <v>57</v>
+      </c>
+      <c r="B37">
+        <f>LEN(COMBINED!D38)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="str">
+        <f>+COMBINED!E38</f>
+        <v>Mirror_Balances_Cherry_Values</v>
+      </c>
+      <c r="F37" t="str">
+        <f>COMBINED!C38</f>
+        <v>MB_CHE</v>
+      </c>
+      <c r="G37" t="s">
+        <v>243</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+      <c r="I37" t="s">
+        <v>244</v>
+      </c>
+      <c r="J37" t="s">
+        <v>245</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="2"/>
+        <v>MB_CHE = (data_line[182]-48);   // Mirror_Balances_Cherry_Values</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38">
+        <f>COMBINED!B39</f>
+        <v>58</v>
+      </c>
+      <c r="B38">
+        <f>LEN(COMBINED!D39)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" t="str">
+        <f>+COMBINED!E39</f>
+        <v>Mirror_Balances_Pacman_Values</v>
+      </c>
+      <c r="F38" t="str">
+        <f>COMBINED!C39</f>
+        <v>MB_PAC</v>
+      </c>
+      <c r="G38" t="s">
+        <v>243</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>187</v>
+      </c>
+      <c r="I38" t="s">
+        <v>244</v>
+      </c>
+      <c r="J38" t="s">
+        <v>245</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="2"/>
+        <v>MB_PAC = (data_line[187]-48);   // Mirror_Balances_Pacman_Values</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39">
+        <f>COMBINED!B40</f>
+        <v>59</v>
+      </c>
+      <c r="B39">
+        <f>LEN(COMBINED!D40)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" t="str">
+        <f>+COMBINED!E40</f>
+        <v>Mirror_Balances_Blinky_Values</v>
+      </c>
+      <c r="F39" t="str">
+        <f>COMBINED!C40</f>
+        <v>MB_BLI</v>
+      </c>
+      <c r="G39" t="s">
+        <v>243</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="I39" t="s">
+        <v>244</v>
+      </c>
+      <c r="J39" t="s">
+        <v>245</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="2"/>
+        <v>MB_BLI = (data_line[192]-48);   // Mirror_Balances_Blinky_Values</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40">
+        <f>COMBINED!B41</f>
+        <v>60</v>
+      </c>
+      <c r="B40">
+        <f>LEN(COMBINED!D41)+4</f>
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" t="str">
+        <f>+COMBINED!E41</f>
+        <v>Mirror_Balances_Inky_Values</v>
+      </c>
+      <c r="F40" t="str">
+        <f>COMBINED!C41</f>
+        <v>MB_INK</v>
+      </c>
+      <c r="G40" t="s">
+        <v>243</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>197</v>
+      </c>
+      <c r="I40" t="s">
+        <v>244</v>
+      </c>
+      <c r="J40" t="s">
+        <v>245</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="2"/>
+        <v>MB_INK = (data_line[197]-48);   // Mirror_Balances_Inky_Values</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4485,14 +6252,14 @@
         <v>113</v>
       </c>
       <c r="D3">
-        <f>LEN(COMBINED!C3)+4</f>
+        <f>LEN(COMBINED!D3)+4</f>
         <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>112</v>
       </c>
       <c r="F3" t="str">
-        <f>+COMBINED!D3</f>
+        <f>+COMBINED!E3</f>
         <v>Master_Enable</v>
       </c>
       <c r="I3" s="87" t="str">
@@ -4519,14 +6286,14 @@
         <v>113</v>
       </c>
       <c r="D4">
-        <f>LEN(COMBINED!C4)+4</f>
+        <f>LEN(COMBINED!D4)+4</f>
         <v>5</v>
       </c>
       <c r="E4" t="s">
         <v>112</v>
       </c>
       <c r="F4" t="str">
-        <f>+COMBINED!D4</f>
+        <f>+COMBINED!E4</f>
         <v>Light_Enable</v>
       </c>
       <c r="I4" s="87" t="str">
@@ -4553,14 +6320,14 @@
         <v>113</v>
       </c>
       <c r="D5">
-        <f>LEN(COMBINED!C5)+4</f>
+        <f>LEN(COMBINED!D5)+4</f>
         <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>112</v>
       </c>
       <c r="F5" t="str">
-        <f>+COMBINED!D5</f>
+        <f>+COMBINED!E5</f>
         <v>Sound_Enable</v>
       </c>
       <c r="I5" s="87" t="str">
@@ -4587,14 +6354,14 @@
         <v>113</v>
       </c>
       <c r="D6">
-        <f>LEN(COMBINED!C6)+4</f>
+        <f>LEN(COMBINED!D6)+4</f>
         <v>5</v>
       </c>
       <c r="E6" t="s">
         <v>112</v>
       </c>
       <c r="F6" t="str">
-        <f>+COMBINED!D6</f>
+        <f>+COMBINED!E6</f>
         <v>Motion_Enable</v>
       </c>
       <c r="I6" s="87" t="str">
@@ -4621,14 +6388,14 @@
         <v>113</v>
       </c>
       <c r="D7">
-        <f>LEN(COMBINED!C7)+4</f>
+        <f>LEN(COMBINED!D7)+4</f>
         <v>5</v>
       </c>
       <c r="E7" t="s">
         <v>112</v>
       </c>
       <c r="F7" t="str">
-        <f>+COMBINED!D7</f>
+        <f>+COMBINED!E7</f>
         <v>Clock_Enable</v>
       </c>
       <c r="I7" s="87" t="str">
@@ -4655,14 +6422,14 @@
         <v>113</v>
       </c>
       <c r="D8">
-        <f>LEN(COMBINED!C8)+4</f>
+        <f>LEN(COMBINED!D8)+4</f>
         <v>5</v>
       </c>
       <c r="E8" t="s">
         <v>112</v>
       </c>
       <c r="F8" t="str">
-        <f>+COMBINED!D8</f>
+        <f>+COMBINED!E8</f>
         <v>Light_Pinky</v>
       </c>
       <c r="I8" s="87" t="str">
@@ -4689,14 +6456,14 @@
         <v>113</v>
       </c>
       <c r="D9">
-        <f>LEN(COMBINED!C9)+4</f>
+        <f>LEN(COMBINED!D9)+4</f>
         <v>5</v>
       </c>
       <c r="E9" t="s">
         <v>112</v>
       </c>
       <c r="F9" t="str">
-        <f>+COMBINED!D9</f>
+        <f>+COMBINED!E9</f>
         <v>Light_Clyde</v>
       </c>
       <c r="I9" s="87" t="str">
@@ -4723,14 +6490,14 @@
         <v>113</v>
       </c>
       <c r="D10">
-        <f>LEN(COMBINED!C10)+4</f>
+        <f>LEN(COMBINED!D10)+4</f>
         <v>5</v>
       </c>
       <c r="E10" t="s">
         <v>112</v>
       </c>
       <c r="F10" t="str">
-        <f>+COMBINED!D10</f>
+        <f>+COMBINED!E10</f>
         <v>Light_Cherry</v>
       </c>
       <c r="I10" s="87" t="str">
@@ -4757,14 +6524,14 @@
         <v>113</v>
       </c>
       <c r="D11">
-        <f>LEN(COMBINED!C11)+4</f>
+        <f>LEN(COMBINED!D11)+4</f>
         <v>5</v>
       </c>
       <c r="E11" t="s">
         <v>112</v>
       </c>
       <c r="F11" t="str">
-        <f>+COMBINED!D11</f>
+        <f>+COMBINED!E11</f>
         <v>Light_PacMan</v>
       </c>
       <c r="I11" s="87" t="str">
@@ -4791,14 +6558,14 @@
         <v>113</v>
       </c>
       <c r="D12">
-        <f>LEN(COMBINED!C12)+4</f>
+        <f>LEN(COMBINED!D12)+4</f>
         <v>5</v>
       </c>
       <c r="E12" t="s">
         <v>112</v>
       </c>
       <c r="F12" t="str">
-        <f>+COMBINED!D12</f>
+        <f>+COMBINED!E12</f>
         <v>Light_Blinky</v>
       </c>
       <c r="I12" s="87" t="str">
@@ -4825,14 +6592,14 @@
         <v>113</v>
       </c>
       <c r="D13">
-        <f>LEN(COMBINED!C13)+4</f>
+        <f>LEN(COMBINED!D13)+4</f>
         <v>5</v>
       </c>
       <c r="E13" t="s">
         <v>112</v>
       </c>
       <c r="F13" t="str">
-        <f>+COMBINED!D13</f>
+        <f>+COMBINED!E13</f>
         <v>Light_Inky</v>
       </c>
       <c r="I13" s="87" t="str">
@@ -4859,14 +6626,14 @@
         <v>113</v>
       </c>
       <c r="D14">
-        <f>LEN(COMBINED!C14)+4</f>
+        <f>LEN(COMBINED!D14)+4</f>
         <v>5</v>
       </c>
       <c r="E14" t="s">
         <v>112</v>
       </c>
       <c r="F14" t="str">
-        <f>+COMBINED!D14</f>
+        <f>+COMBINED!E14</f>
         <v>Light_Sensor_Enable</v>
       </c>
       <c r="I14" s="87" t="str">
@@ -4893,14 +6660,14 @@
         <v>113</v>
       </c>
       <c r="D15">
-        <f>LEN(COMBINED!C15)+4</f>
+        <f>LEN(COMBINED!D15)+4</f>
         <v>9</v>
       </c>
       <c r="E15" t="s">
         <v>112</v>
       </c>
       <c r="F15" t="str">
-        <f>+COMBINED!D15</f>
+        <f>+COMBINED!E15</f>
         <v>Light_Sensor_trigger_value</v>
       </c>
       <c r="I15" s="87" t="str">
@@ -4927,14 +6694,14 @@
         <v>113</v>
       </c>
       <c r="D16">
-        <f>LEN(COMBINED!C16)+4</f>
+        <f>LEN(COMBINED!D16)+4</f>
         <v>5</v>
       </c>
       <c r="E16" t="s">
         <v>112</v>
       </c>
       <c r="F16" t="str">
-        <f>+COMBINED!D16</f>
+        <f>+COMBINED!E16</f>
         <v>Night_Light_Enable_and_mode</v>
       </c>
       <c r="I16" s="87" t="str">
@@ -4961,14 +6728,14 @@
         <v>113</v>
       </c>
       <c r="D17">
-        <f>LEN(COMBINED!C17)+4</f>
+        <f>LEN(COMBINED!D17)+4</f>
         <v>5</v>
       </c>
       <c r="E17" t="s">
         <v>112</v>
       </c>
       <c r="F17" t="str">
-        <f>+COMBINED!D17</f>
+        <f>+COMBINED!E17</f>
         <v>(ip address preset)</v>
       </c>
       <c r="I17" s="87" t="str">
@@ -4995,14 +6762,14 @@
         <v>113</v>
       </c>
       <c r="D18">
-        <f>LEN(COMBINED!C18)+4</f>
+        <f>LEN(COMBINED!D18)+4</f>
         <v>5</v>
       </c>
       <c r="E18" t="s">
         <v>112</v>
       </c>
       <c r="F18" t="str">
-        <f>+COMBINED!D18</f>
+        <f>+COMBINED!E18</f>
         <v>Alarm_Enable</v>
       </c>
       <c r="I18" s="87" t="str">
@@ -5029,14 +6796,14 @@
         <v>113</v>
       </c>
       <c r="D19">
-        <f>LEN(COMBINED!C19)+4</f>
+        <f>LEN(COMBINED!D19)+4</f>
         <v>13</v>
       </c>
       <c r="E19" t="s">
         <v>112</v>
       </c>
       <c r="F19" t="str">
-        <f>+COMBINED!D19</f>
+        <f>+COMBINED!E19</f>
         <v>Alarm_Date</v>
       </c>
       <c r="I19" s="87" t="str">
@@ -5063,14 +6830,14 @@
         <v>113</v>
       </c>
       <c r="D20">
-        <f>LEN(COMBINED!C20)+4</f>
+        <f>LEN(COMBINED!D20)+4</f>
         <v>13</v>
       </c>
       <c r="E20" t="s">
         <v>112</v>
       </c>
       <c r="F20" t="str">
-        <f>+COMBINED!D20</f>
+        <f>+COMBINED!E20</f>
         <v>Alarm_Time</v>
       </c>
       <c r="I20" s="87" t="str">
@@ -5097,14 +6864,14 @@
         <v>113</v>
       </c>
       <c r="D21">
-        <f>LEN(COMBINED!C21)+4</f>
+        <f>LEN(COMBINED!D21)+4</f>
         <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>112</v>
       </c>
       <c r="F21" t="str">
-        <f>+COMBINED!D21</f>
+        <f>+COMBINED!E21</f>
         <v>Performance_number</v>
       </c>
       <c r="I21" s="87" t="str">
@@ -5131,14 +6898,14 @@
         <v>113</v>
       </c>
       <c r="D22">
-        <f>LEN(COMBINED!C22)+4</f>
+        <f>LEN(COMBINED!D22)+4</f>
         <v>5</v>
       </c>
       <c r="E22" t="s">
         <v>112</v>
       </c>
       <c r="F22" t="str">
-        <f>+COMBINED!D22</f>
+        <f>+COMBINED!E22</f>
         <v>Stayin_Game_Status</v>
       </c>
       <c r="I22" s="87" t="str">
@@ -5165,14 +6932,14 @@
         <v>113</v>
       </c>
       <c r="D23">
-        <f>LEN(COMBINED!C23)+4</f>
+        <f>LEN(COMBINED!D23)+4</f>
         <v>5</v>
       </c>
       <c r="E23" t="s">
         <v>112</v>
       </c>
       <c r="F23" t="str">
-        <f>+COMBINED!D23</f>
+        <f>+COMBINED!E23</f>
         <v>myCharNum</v>
       </c>
       <c r="I23" s="87" t="str">
@@ -5199,14 +6966,14 @@
         <v>113</v>
       </c>
       <c r="D24">
-        <f>LEN(COMBINED!C24)+4</f>
+        <f>LEN(COMBINED!D24)+4</f>
         <v>11</v>
       </c>
       <c r="E24" t="s">
         <v>112</v>
       </c>
       <c r="F24" t="str">
-        <f>+COMBINED!D24</f>
+        <f>+COMBINED!E24</f>
         <v>ActualName</v>
       </c>
       <c r="I24" s="87" t="str">
@@ -5233,14 +7000,14 @@
         <v>113</v>
       </c>
       <c r="D25">
-        <f>LEN(COMBINED!C25)+4</f>
+        <f>LEN(COMBINED!D25)+4</f>
         <v>8</v>
       </c>
       <c r="E25" t="s">
         <v>112</v>
       </c>
       <c r="F25" t="str">
-        <f>+COMBINED!D25</f>
+        <f>+COMBINED!E25</f>
         <v>BankAfterSpend</v>
       </c>
       <c r="I25" s="87" t="str">
@@ -5267,14 +7034,14 @@
         <v>113</v>
       </c>
       <c r="D26">
-        <f>LEN(COMBINED!C26)+4</f>
+        <f>LEN(COMBINED!D26)+4</f>
         <v>8</v>
       </c>
       <c r="E26" t="s">
         <v>112</v>
       </c>
       <c r="F26" t="str">
-        <f>+COMBINED!D26</f>
+        <f>+COMBINED!E26</f>
         <v>Attack_balance</v>
       </c>
       <c r="I26" s="87" t="str">
@@ -5301,14 +7068,14 @@
         <v>113</v>
       </c>
       <c r="D27">
-        <f>LEN(COMBINED!C27)+4</f>
+        <f>LEN(COMBINED!D27)+4</f>
         <v>11</v>
       </c>
       <c r="E27" t="s">
         <v>112</v>
       </c>
       <c r="F27" t="str">
-        <f>+COMBINED!D27</f>
+        <f>+COMBINED!E27</f>
         <v>Attack_or_Donate_Flag</v>
       </c>
       <c r="I27" s="87" t="str">
@@ -5335,14 +7102,14 @@
         <v>113</v>
       </c>
       <c r="D28">
-        <f>LEN(COMBINED!C28)+4</f>
+        <f>LEN(COMBINED!D28)+4</f>
         <v>11</v>
       </c>
       <c r="E28" t="s">
         <v>112</v>
       </c>
       <c r="F28" t="str">
-        <f>+COMBINED!D28</f>
+        <f>+COMBINED!E28</f>
         <v>Will_or_No (Pinky-Inky)</v>
       </c>
       <c r="I28" s="87" t="str">
@@ -5369,14 +7136,14 @@
         <v>113</v>
       </c>
       <c r="D29">
-        <f>LEN(COMBINED!C29)+4</f>
+        <f>LEN(COMBINED!D29)+4</f>
         <v>11</v>
       </c>
       <c r="E29" t="s">
         <v>112</v>
       </c>
       <c r="F29" t="str">
-        <f>+COMBINED!D29</f>
+        <f>+COMBINED!E29</f>
         <v>Mirror_or_No (Pinky-Inky)</v>
       </c>
       <c r="I29" s="87" t="str">
@@ -5403,14 +7170,14 @@
         <v>113</v>
       </c>
       <c r="D30">
-        <f>LEN(COMBINED!C30)+4</f>
+        <f>LEN(COMBINED!D30)+4</f>
         <v>8</v>
       </c>
       <c r="E30" t="s">
         <v>112</v>
       </c>
       <c r="F30" t="str">
-        <f>+COMBINED!D30</f>
+        <f>+COMBINED!E30</f>
         <v>Attack_or_Donate Pinky_Amnt</v>
       </c>
       <c r="I30" s="87" t="str">
@@ -5437,14 +7204,14 @@
         <v>113</v>
       </c>
       <c r="D31">
-        <f>LEN(COMBINED!C31)+4</f>
+        <f>LEN(COMBINED!D31)+4</f>
         <v>8</v>
       </c>
       <c r="E31" t="s">
         <v>112</v>
       </c>
       <c r="F31" t="str">
-        <f>+COMBINED!D31</f>
+        <f>+COMBINED!E31</f>
         <v>Attack_or_Donate Clyde_Amnt</v>
       </c>
       <c r="I31" s="87" t="str">
@@ -5471,14 +7238,14 @@
         <v>113</v>
       </c>
       <c r="D32">
-        <f>LEN(COMBINED!C32)+4</f>
+        <f>LEN(COMBINED!D32)+4</f>
         <v>8</v>
       </c>
       <c r="E32" t="s">
         <v>112</v>
       </c>
       <c r="F32" t="str">
-        <f>+COMBINED!D32</f>
+        <f>+COMBINED!E32</f>
         <v>Attack_or_Donate Cherry_Amnt</v>
       </c>
       <c r="I32" s="87" t="str">
@@ -5505,14 +7272,14 @@
         <v>113</v>
       </c>
       <c r="D33">
-        <f>LEN(COMBINED!C33)+4</f>
+        <f>LEN(COMBINED!D33)+4</f>
         <v>8</v>
       </c>
       <c r="E33" t="s">
         <v>112</v>
       </c>
       <c r="F33" t="str">
-        <f>+COMBINED!D33</f>
+        <f>+COMBINED!E33</f>
         <v>Attack_or_Donate PacMan_Amnt</v>
       </c>
       <c r="I33" s="87" t="str">
@@ -5539,14 +7306,14 @@
         <v>113</v>
       </c>
       <c r="D34">
-        <f>LEN(COMBINED!C34)+4</f>
+        <f>LEN(COMBINED!D34)+4</f>
         <v>8</v>
       </c>
       <c r="E34" t="s">
         <v>112</v>
       </c>
       <c r="F34" t="str">
-        <f>+COMBINED!D34</f>
+        <f>+COMBINED!E34</f>
         <v>Attack_or_Donate Blinky_Amnt</v>
       </c>
       <c r="I34" s="87" t="str">
@@ -5573,14 +7340,14 @@
         <v>113</v>
       </c>
       <c r="D35">
-        <f>LEN(COMBINED!C35)+4</f>
+        <f>LEN(COMBINED!D35)+4</f>
         <v>8</v>
       </c>
       <c r="E35" t="s">
         <v>112</v>
       </c>
       <c r="F35" t="str">
-        <f>+COMBINED!D35</f>
+        <f>+COMBINED!E35</f>
         <v>Attack_or_Donate Inky_Amnt</v>
       </c>
       <c r="I35" s="87" t="str">
@@ -5607,14 +7374,14 @@
         <v>113</v>
       </c>
       <c r="D36">
-        <f>LEN(COMBINED!C36)+4</f>
+        <f>LEN(COMBINED!D36)+4</f>
         <v>11</v>
       </c>
       <c r="E36" t="s">
         <v>112</v>
       </c>
       <c r="F36" t="str">
-        <f>+COMBINED!D36</f>
+        <f>+COMBINED!E36</f>
         <v>Mirror_Balances_Pinky_Values</v>
       </c>
       <c r="I36" s="87" t="str">
@@ -5641,14 +7408,14 @@
         <v>113</v>
       </c>
       <c r="D37">
-        <f>LEN(COMBINED!C37)+4</f>
+        <f>LEN(COMBINED!D37)+4</f>
         <v>11</v>
       </c>
       <c r="E37" t="s">
         <v>112</v>
       </c>
       <c r="F37" t="str">
-        <f>+COMBINED!D37</f>
+        <f>+COMBINED!E37</f>
         <v>Mirror_Balances_Clyde_Values</v>
       </c>
       <c r="I37" s="87" t="str">
@@ -5675,14 +7442,14 @@
         <v>113</v>
       </c>
       <c r="D38">
-        <f>LEN(COMBINED!C38)+4</f>
+        <f>LEN(COMBINED!D38)+4</f>
         <v>11</v>
       </c>
       <c r="E38" t="s">
         <v>112</v>
       </c>
       <c r="F38" t="str">
-        <f>+COMBINED!D38</f>
+        <f>+COMBINED!E38</f>
         <v>Mirror_Balances_Cherry_Values</v>
       </c>
       <c r="I38" s="87" t="str">
@@ -5709,14 +7476,14 @@
         <v>113</v>
       </c>
       <c r="D39">
-        <f>LEN(COMBINED!C39)+4</f>
+        <f>LEN(COMBINED!D39)+4</f>
         <v>11</v>
       </c>
       <c r="E39" t="s">
         <v>112</v>
       </c>
       <c r="F39" t="str">
-        <f>+COMBINED!D39</f>
+        <f>+COMBINED!E39</f>
         <v>Mirror_Balances_Pacman_Values</v>
       </c>
       <c r="I39" s="87" t="str">
@@ -5743,14 +7510,14 @@
         <v>113</v>
       </c>
       <c r="D40">
-        <f>LEN(COMBINED!C40)+4</f>
+        <f>LEN(COMBINED!D40)+4</f>
         <v>11</v>
       </c>
       <c r="E40" t="s">
         <v>112</v>
       </c>
       <c r="F40" t="str">
-        <f>+COMBINED!D40</f>
+        <f>+COMBINED!E40</f>
         <v>Mirror_Balances_Blinky_Values</v>
       </c>
       <c r="I40" s="87" t="str">
@@ -5777,14 +7544,14 @@
         <v>113</v>
       </c>
       <c r="D41">
-        <f>LEN(COMBINED!C41)+4</f>
+        <f>LEN(COMBINED!D41)+4</f>
         <v>11</v>
       </c>
       <c r="E41" t="s">
         <v>112</v>
       </c>
       <c r="F41" t="str">
-        <f>+COMBINED!D41</f>
+        <f>+COMBINED!E41</f>
         <v>Mirror_Balances_Inky_Values</v>
       </c>
       <c r="I41" s="87" t="str">
@@ -5804,7 +7571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -5885,7 +7652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -11157,7 +12924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BC82"/>
   <sheetViews>
@@ -17688,11 +19455,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pre-Zach delivery.  New comms set up.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -1153,7 +1153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1211,6 +1211,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1321,7 +1333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1518,6 +1530,8 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4759,8 +4773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5303,7 +5317,7 @@
         <v>245</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" ref="K4:K40" si="2">CONCATENATE(F16,G16,H16,I16,J16,D16)</f>
+        <f t="shared" ref="K16:K40" si="2">CONCATENATE(F16,G16,H16,I16,J16,D16)</f>
         <v>NL_EN = (data_line[77]-48);   // Night_Light_Enable_and_mode</v>
       </c>
     </row>
@@ -5406,9 +5420,9 @@
       <c r="G19" t="s">
         <v>243</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
-        <v>92</v>
+      <c r="H19" s="95">
+        <f>+H18+14</f>
+        <v>101</v>
       </c>
       <c r="I19" t="s">
         <v>244</v>
@@ -5418,7 +5432,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
-        <v>ALM_TIME = (data_line[92]-48);   // Alarm_Time</v>
+        <v>ALM_TIME = (data_line[101]-48);   // Alarm_Time</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -5444,9 +5458,9 @@
       <c r="G20" t="s">
         <v>243</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
-        <v>97</v>
+      <c r="H20" s="94">
+        <f>+H19+12</f>
+        <v>113</v>
       </c>
       <c r="I20" t="s">
         <v>244</v>
@@ -5456,7 +5470,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="2"/>
-        <v>PERF_NUM = (data_line[97]-48);   // Performance_number</v>
+        <v>PERF_NUM = (data_line[113]-48);   // Performance_number</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -5484,7 +5498,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="I21" t="s">
         <v>244</v>
@@ -5494,7 +5508,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="2"/>
-        <v>GAME_STATUS = (data_line[102]-48);   // Stayin_Game_Status</v>
+        <v>GAME_STATUS = (data_line[118]-48);   // Stayin_Game_Status</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -5522,7 +5536,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="I22" t="s">
         <v>244</v>
@@ -5532,7 +5546,7 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="2"/>
-        <v>MY_CHAR_NUM = (data_line[107]-48);   // myCharNum</v>
+        <v>MY_CHAR_NUM = (data_line[123]-48);   // myCharNum</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -5560,7 +5574,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="I23" t="s">
         <v>244</v>
@@ -5570,7 +5584,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="2"/>
-        <v>ACT_NAME = (data_line[112]-48);   // ActualName</v>
+        <v>ACT_NAME = (data_line[128]-48);   // ActualName</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -5598,7 +5612,7 @@
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="I24" t="s">
         <v>244</v>
@@ -5608,7 +5622,7 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="2"/>
-        <v>BANK_AFTER_SPEND = (data_line[117]-48);   // BankAfterSpend</v>
+        <v>BANK_AFTER_SPEND = (data_line[133]-48);   // BankAfterSpend</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -5636,7 +5650,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="I25" t="s">
         <v>244</v>
@@ -5646,7 +5660,7 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="2"/>
-        <v>ATTACK_BAL = (data_line[122]-48);   // Attack_balance</v>
+        <v>ATTACK_BAL = (data_line[138]-48);   // Attack_balance</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -5674,7 +5688,7 @@
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="I26" t="s">
         <v>244</v>
@@ -5684,7 +5698,7 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="2"/>
-        <v>ATT_DON = (data_line[127]-48);   // Attack_or_Donate_Flag</v>
+        <v>ATT_DON = (data_line[143]-48);   // Attack_or_Donate_Flag</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -5712,7 +5726,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="I27" t="s">
         <v>244</v>
@@ -5722,7 +5736,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="2"/>
-        <v>WILL_NO = (data_line[132]-48);   // Will_or_No (Pinky-Inky)</v>
+        <v>WILL_NO = (data_line[148]-48);   // Will_or_No (Pinky-Inky)</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -5750,7 +5764,7 @@
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="I28" t="s">
         <v>244</v>
@@ -5760,7 +5774,7 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="2"/>
-        <v>MIRROR_NO = (data_line[137]-48);   // Mirror_or_No (Pinky-Inky)</v>
+        <v>MIRROR_NO = (data_line[153]-48);   // Mirror_or_No (Pinky-Inky)</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -5788,7 +5802,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="I29" t="s">
         <v>244</v>
@@ -5798,7 +5812,7 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="2"/>
-        <v>AD_PIN = (data_line[142]-48);   // Attack_or_Donate Pinky_Amnt</v>
+        <v>AD_PIN = (data_line[158]-48);   // Attack_or_Donate Pinky_Amnt</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -5826,7 +5840,7 @@
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="I30" t="s">
         <v>244</v>
@@ -5836,7 +5850,7 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="2"/>
-        <v>AD_CLY = (data_line[147]-48);   // Attack_or_Donate Clyde_Amnt</v>
+        <v>AD_CLY = (data_line[163]-48);   // Attack_or_Donate Clyde_Amnt</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -5864,7 +5878,7 @@
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="I31" t="s">
         <v>244</v>
@@ -5874,7 +5888,7 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" si="2"/>
-        <v>AD_CHE = (data_line[152]-48);   // Attack_or_Donate Cherry_Amnt</v>
+        <v>AD_CHE = (data_line[168]-48);   // Attack_or_Donate Cherry_Amnt</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -5902,7 +5916,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="I32" t="s">
         <v>244</v>
@@ -5912,7 +5926,7 @@
       </c>
       <c r="K32" t="str">
         <f t="shared" si="2"/>
-        <v>AD_PAC = (data_line[157]-48);   // Attack_or_Donate PacMan_Amnt</v>
+        <v>AD_PAC = (data_line[173]-48);   // Attack_or_Donate PacMan_Amnt</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -5940,7 +5954,7 @@
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="I33" t="s">
         <v>244</v>
@@ -5950,7 +5964,7 @@
       </c>
       <c r="K33" t="str">
         <f t="shared" si="2"/>
-        <v>AD_BLI = (data_line[162]-48);   // Attack_or_Donate Blinky_Amnt</v>
+        <v>AD_BLI = (data_line[178]-48);   // Attack_or_Donate Blinky_Amnt</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -5978,7 +5992,7 @@
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="I34" t="s">
         <v>244</v>
@@ -5988,7 +6002,7 @@
       </c>
       <c r="K34" t="str">
         <f t="shared" si="2"/>
-        <v>AD_INK = (data_line[167]-48);   // Attack_or_Donate Inky_Amnt</v>
+        <v>AD_INK = (data_line[183]-48);   // Attack_or_Donate Inky_Amnt</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -6016,7 +6030,7 @@
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="I35" t="s">
         <v>244</v>
@@ -6026,7 +6040,7 @@
       </c>
       <c r="K35" t="str">
         <f t="shared" si="2"/>
-        <v>MB_PIN = (data_line[172]-48);   // Mirror_Balances_Pinky_Values</v>
+        <v>MB_PIN = (data_line[188]-48);   // Mirror_Balances_Pinky_Values</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -6054,7 +6068,7 @@
       </c>
       <c r="H36">
         <f t="shared" si="1"/>
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="I36" t="s">
         <v>244</v>
@@ -6064,7 +6078,7 @@
       </c>
       <c r="K36" t="str">
         <f t="shared" si="2"/>
-        <v>MB_CLY = (data_line[177]-48);   // Mirror_Balances_Clyde_Values</v>
+        <v>MB_CLY = (data_line[193]-48);   // Mirror_Balances_Clyde_Values</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -6092,7 +6106,7 @@
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="I37" t="s">
         <v>244</v>
@@ -6102,7 +6116,7 @@
       </c>
       <c r="K37" t="str">
         <f t="shared" si="2"/>
-        <v>MB_CHE = (data_line[182]-48);   // Mirror_Balances_Cherry_Values</v>
+        <v>MB_CHE = (data_line[198]-48);   // Mirror_Balances_Cherry_Values</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -6130,7 +6144,7 @@
       </c>
       <c r="H38">
         <f t="shared" si="1"/>
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="I38" t="s">
         <v>244</v>
@@ -6140,7 +6154,7 @@
       </c>
       <c r="K38" t="str">
         <f t="shared" si="2"/>
-        <v>MB_PAC = (data_line[187]-48);   // Mirror_Balances_Pacman_Values</v>
+        <v>MB_PAC = (data_line[203]-48);   // Mirror_Balances_Pacman_Values</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -6168,7 +6182,7 @@
       </c>
       <c r="H39">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="I39" t="s">
         <v>244</v>
@@ -6178,7 +6192,7 @@
       </c>
       <c r="K39" t="str">
         <f t="shared" si="2"/>
-        <v>MB_BLI = (data_line[192]-48);   // Mirror_Balances_Blinky_Values</v>
+        <v>MB_BLI = (data_line[208]-48);   // Mirror_Balances_Blinky_Values</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -6206,7 +6220,7 @@
       </c>
       <c r="H40">
         <f t="shared" si="1"/>
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="I40" t="s">
         <v>244</v>
@@ -6216,7 +6230,7 @@
       </c>
       <c r="K40" t="str">
         <f t="shared" si="2"/>
-        <v>MB_INK = (data_line[197]-48);   // Mirror_Balances_Inky_Values</v>
+        <v>MB_INK = (data_line[213]-48);   // Mirror_Balances_Inky_Values</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added game setting variabes to global variables.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="8265" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="COMBINED" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="275">
   <si>
     <t>App use only</t>
   </si>
@@ -739,9 +739,6 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>Long</t>
-  </si>
-  <si>
     <t>pinky_rename = "PINKY"</t>
   </si>
   <si>
@@ -914,6 +911,90 @@
   </si>
   <si>
     <t>LS_VAL</t>
+  </si>
+  <si>
+    <t>SA_game_guAtStart</t>
+  </si>
+  <si>
+    <t>SA_game_guIncome</t>
+  </si>
+  <si>
+    <t>SA_game_huAtStart</t>
+  </si>
+  <si>
+    <t>SA_game_huHealing</t>
+  </si>
+  <si>
+    <t>SA_game_hu4gu</t>
+  </si>
+  <si>
+    <t>SA_game_ou4gu</t>
+  </si>
+  <si>
+    <t>SA_game_lastStrikeBonus</t>
+  </si>
+  <si>
+    <t>SA_game_firstStrikeBonus</t>
+  </si>
+  <si>
+    <t>SA_game_firstKillBonus</t>
+  </si>
+  <si>
+    <t>SA_game_firstStrikeMult</t>
+  </si>
+  <si>
+    <t>SA_game_kastStrikeMult</t>
+  </si>
+  <si>
+    <t>SA_game_ReportAttackers</t>
+  </si>
+  <si>
+    <t>SA_game_ReportMirros</t>
+  </si>
+  <si>
+    <t>SA_game_ReportBeneficiaries</t>
+  </si>
+  <si>
+    <t>sa_game_guAtStart</t>
+  </si>
+  <si>
+    <t>sa_game_guIncome</t>
+  </si>
+  <si>
+    <t>sa_game_huAtStart</t>
+  </si>
+  <si>
+    <t>sa_game_huHealing</t>
+  </si>
+  <si>
+    <t>sa_game_hu4gu</t>
+  </si>
+  <si>
+    <t>sa_game_ou4gu</t>
+  </si>
+  <si>
+    <t>sa_game_firstStrikeBonus</t>
+  </si>
+  <si>
+    <t>sa_game_lastStrikeBonus</t>
+  </si>
+  <si>
+    <t>sa_game_firstKillBonus</t>
+  </si>
+  <si>
+    <t>sa_game_firstStrikeMult</t>
+  </si>
+  <si>
+    <t>sa_game_kastStrikeMult</t>
+  </si>
+  <si>
+    <t>sa_game_ReportAttackers</t>
+  </si>
+  <si>
+    <t>sa_game_ReportMirros</t>
+  </si>
+  <si>
+    <t>sa_game_ReportBeneficiaries</t>
   </si>
 </sst>
 </file>
@@ -3156,7 +3237,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="C2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="3" t="s">
@@ -3183,7 +3264,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D3" s="76" t="s">
         <v>33</v>
@@ -3216,7 +3297,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="76" t="s">
         <v>33</v>
@@ -3249,7 +3330,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="77" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" s="76" t="s">
         <v>33</v>
@@ -3282,7 +3363,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="77" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" s="76" t="s">
         <v>33</v>
@@ -3315,7 +3396,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D7" s="76" t="s">
         <v>33</v>
@@ -3348,7 +3429,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="76" t="s">
         <v>33</v>
@@ -3381,7 +3462,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="77" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D9" s="76" t="s">
         <v>33</v>
@@ -3414,7 +3495,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="77" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D10" s="76" t="s">
         <v>33</v>
@@ -3447,7 +3528,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="77" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D11" s="76" t="s">
         <v>33</v>
@@ -3480,7 +3561,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D12" s="76" t="s">
         <v>33</v>
@@ -3513,7 +3594,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D13" s="76" t="s">
         <v>33</v>
@@ -3546,7 +3627,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" s="76" t="s">
         <v>33</v>
@@ -3579,7 +3660,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="77" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D15" s="76" t="s">
         <v>97</v>
@@ -3612,7 +3693,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="77" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D16" s="76" t="s">
         <v>33</v>
@@ -3676,7 +3757,7 @@
         <v>26</v>
       </c>
       <c r="C18" s="77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D18" s="76" t="s">
         <v>33</v>
@@ -3709,7 +3790,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D19" s="76" t="s">
         <v>114</v>
@@ -3742,7 +3823,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D20" s="76" t="s">
         <v>114</v>
@@ -3775,7 +3856,7 @@
         <v>29</v>
       </c>
       <c r="C21" s="77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D21" s="76" t="s">
         <v>44</v>
@@ -3808,7 +3889,7 @@
         <v>41</v>
       </c>
       <c r="C22" s="77" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D22" s="76" t="s">
         <v>33</v>
@@ -3841,7 +3922,7 @@
         <v>42</v>
       </c>
       <c r="C23" s="77" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D23" s="76" t="s">
         <v>33</v>
@@ -3874,7 +3955,7 @@
         <v>43</v>
       </c>
       <c r="C24" s="77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D24" s="76" t="s">
         <v>98</v>
@@ -3907,7 +3988,7 @@
         <v>44</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D25" s="76" t="s">
         <v>115</v>
@@ -3940,7 +4021,7 @@
         <v>45</v>
       </c>
       <c r="C26" s="77" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D26" s="76" t="s">
         <v>115</v>
@@ -3973,7 +4054,7 @@
         <v>46</v>
       </c>
       <c r="C27" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D27" s="76" t="s">
         <v>94</v>
@@ -4006,7 +4087,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="77" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D28" s="76" t="s">
         <v>94</v>
@@ -4039,7 +4120,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="77" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D29" s="76" t="s">
         <v>94</v>
@@ -4072,7 +4153,7 @@
         <v>49</v>
       </c>
       <c r="C30" s="77" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D30" s="76" t="s">
         <v>115</v>
@@ -4105,7 +4186,7 @@
         <v>50</v>
       </c>
       <c r="C31" s="77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D31" s="76" t="s">
         <v>115</v>
@@ -4138,7 +4219,7 @@
         <v>51</v>
       </c>
       <c r="C32" s="77" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D32" s="76" t="s">
         <v>115</v>
@@ -4171,7 +4252,7 @@
         <v>52</v>
       </c>
       <c r="C33" s="77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D33" s="76" t="s">
         <v>115</v>
@@ -4204,7 +4285,7 @@
         <v>53</v>
       </c>
       <c r="C34" s="77" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D34" s="76" t="s">
         <v>115</v>
@@ -4237,7 +4318,7 @@
         <v>54</v>
       </c>
       <c r="C35" s="77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D35" s="76" t="s">
         <v>115</v>
@@ -4270,7 +4351,7 @@
         <v>55</v>
       </c>
       <c r="C36" s="77" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D36" s="76" t="s">
         <v>94</v>
@@ -4303,7 +4384,7 @@
         <v>56</v>
       </c>
       <c r="C37" s="77" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D37" s="76" t="s">
         <v>94</v>
@@ -4336,7 +4417,7 @@
         <v>57</v>
       </c>
       <c r="C38" s="77" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D38" s="76" t="s">
         <v>94</v>
@@ -4367,7 +4448,7 @@
         <v>58</v>
       </c>
       <c r="C39" s="77" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D39" s="76" t="s">
         <v>94</v>
@@ -4398,7 +4479,7 @@
         <v>59</v>
       </c>
       <c r="C40" s="77" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D40" s="76" t="s">
         <v>94</v>
@@ -4429,7 +4510,7 @@
         <v>60</v>
       </c>
       <c r="C41" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D41" s="76" t="s">
         <v>94</v>
@@ -4460,7 +4541,7 @@
         <v>61</v>
       </c>
       <c r="C42" s="77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D42" s="76" t="s">
         <v>98</v>
@@ -4491,7 +4572,7 @@
         <v>62</v>
       </c>
       <c r="C43" s="77" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D43" s="76" t="s">
         <v>98</v>
@@ -4522,7 +4603,7 @@
         <v>63</v>
       </c>
       <c r="C44" s="77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D44" s="76" t="s">
         <v>98</v>
@@ -4553,7 +4634,7 @@
         <v>64</v>
       </c>
       <c r="C45" s="77" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D45" s="76" t="s">
         <v>98</v>
@@ -4584,7 +4665,7 @@
         <v>65</v>
       </c>
       <c r="C46" s="77" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D46" s="76" t="s">
         <v>98</v>
@@ -4615,7 +4696,7 @@
         <v>66</v>
       </c>
       <c r="C47" s="77" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D47" s="76" t="s">
         <v>98</v>
@@ -4773,7 +4854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -4787,7 +4868,7 @@
   <sheetData>
     <row r="2" spans="1:11">
       <c r="H2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4811,16 +4892,16 @@
         <v>M_EN</v>
       </c>
       <c r="G3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H3">
         <v>9</v>
       </c>
       <c r="I3" t="s">
+        <v>243</v>
+      </c>
+      <c r="J3" t="s">
         <v>244</v>
-      </c>
-      <c r="J3" t="s">
-        <v>245</v>
       </c>
       <c r="K3" t="str">
         <f>CONCATENATE(F3,G3,H3,I3,J3,D3)</f>
@@ -4848,17 +4929,17 @@
         <v>L_EN</v>
       </c>
       <c r="G4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H4">
         <f>+H3+5</f>
         <v>14</v>
       </c>
       <c r="I4" t="s">
+        <v>243</v>
+      </c>
+      <c r="J4" t="s">
         <v>244</v>
-      </c>
-      <c r="J4" t="s">
-        <v>245</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" ref="K4:K15" si="0">CONCATENATE(F4,G4,H4,I4,J4,D4)</f>
@@ -4886,17 +4967,17 @@
         <v>S_EN</v>
       </c>
       <c r="G5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H40" si="1">+H4+5</f>
         <v>19</v>
       </c>
       <c r="I5" t="s">
+        <v>243</v>
+      </c>
+      <c r="J5" t="s">
         <v>244</v>
-      </c>
-      <c r="J5" t="s">
-        <v>245</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
@@ -4924,17 +5005,17 @@
         <v>MO_EN</v>
       </c>
       <c r="G6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I6" t="s">
+        <v>243</v>
+      </c>
+      <c r="J6" t="s">
         <v>244</v>
-      </c>
-      <c r="J6" t="s">
-        <v>245</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -4962,17 +5043,17 @@
         <v>CL_EN</v>
       </c>
       <c r="G7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="I7" t="s">
+        <v>243</v>
+      </c>
+      <c r="J7" t="s">
         <v>244</v>
-      </c>
-      <c r="J7" t="s">
-        <v>245</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -5000,17 +5081,17 @@
         <v>PIN_EN</v>
       </c>
       <c r="G8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="I8" t="s">
+        <v>243</v>
+      </c>
+      <c r="J8" t="s">
         <v>244</v>
-      </c>
-      <c r="J8" t="s">
-        <v>245</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -5038,17 +5119,17 @@
         <v>CLY_EN</v>
       </c>
       <c r="G9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="I9" t="s">
+        <v>243</v>
+      </c>
+      <c r="J9" t="s">
         <v>244</v>
-      </c>
-      <c r="J9" t="s">
-        <v>245</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -5076,17 +5157,17 @@
         <v>CHE_EN</v>
       </c>
       <c r="G10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="I10" t="s">
+        <v>243</v>
+      </c>
+      <c r="J10" t="s">
         <v>244</v>
-      </c>
-      <c r="J10" t="s">
-        <v>245</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -5114,17 +5195,17 @@
         <v>PAC_EN</v>
       </c>
       <c r="G11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="I11" t="s">
+        <v>243</v>
+      </c>
+      <c r="J11" t="s">
         <v>244</v>
-      </c>
-      <c r="J11" t="s">
-        <v>245</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
@@ -5152,17 +5233,17 @@
         <v>BLI_EN</v>
       </c>
       <c r="G12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="I12" t="s">
+        <v>243</v>
+      </c>
+      <c r="J12" t="s">
         <v>244</v>
-      </c>
-      <c r="J12" t="s">
-        <v>245</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -5190,17 +5271,17 @@
         <v>INK_EN</v>
       </c>
       <c r="G13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="I13" t="s">
+        <v>243</v>
+      </c>
+      <c r="J13" t="s">
         <v>244</v>
-      </c>
-      <c r="J13" t="s">
-        <v>245</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
@@ -5228,17 +5309,17 @@
         <v>LS_EN</v>
       </c>
       <c r="G14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="I14" t="s">
+        <v>243</v>
+      </c>
+      <c r="J14" t="s">
         <v>244</v>
-      </c>
-      <c r="J14" t="s">
-        <v>245</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
@@ -5266,17 +5347,17 @@
         <v>LS_VAL</v>
       </c>
       <c r="G15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="I15" t="s">
+        <v>243</v>
+      </c>
+      <c r="J15" t="s">
         <v>244</v>
-      </c>
-      <c r="J15" t="s">
-        <v>245</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
@@ -5304,17 +5385,17 @@
         <v>NL_EN</v>
       </c>
       <c r="G16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H16" s="93">
         <f>+H15+5+3</f>
         <v>77</v>
       </c>
       <c r="I16" t="s">
+        <v>243</v>
+      </c>
+      <c r="J16" t="s">
         <v>244</v>
-      </c>
-      <c r="J16" t="s">
-        <v>245</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ref="K16:K40" si="2">CONCATENATE(F16,G16,H16,I16,J16,D16)</f>
@@ -5342,17 +5423,17 @@
         <v>ALM_EN</v>
       </c>
       <c r="G17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H17">
         <f>+H16+5</f>
         <v>82</v>
       </c>
       <c r="I17" t="s">
+        <v>243</v>
+      </c>
+      <c r="J17" t="s">
         <v>244</v>
-      </c>
-      <c r="J17" t="s">
-        <v>245</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="2"/>
@@ -5380,17 +5461,17 @@
         <v>ALM_DATE</v>
       </c>
       <c r="G18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="I18" t="s">
+        <v>243</v>
+      </c>
+      <c r="J18" t="s">
         <v>244</v>
-      </c>
-      <c r="J18" t="s">
-        <v>245</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="2"/>
@@ -5418,17 +5499,17 @@
         <v>ALM_TIME</v>
       </c>
       <c r="G19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H19" s="95">
         <f>+H18+14</f>
         <v>101</v>
       </c>
       <c r="I19" t="s">
+        <v>243</v>
+      </c>
+      <c r="J19" t="s">
         <v>244</v>
-      </c>
-      <c r="J19" t="s">
-        <v>245</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
@@ -5456,17 +5537,17 @@
         <v>PERF_NUM</v>
       </c>
       <c r="G20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H20" s="94">
         <f>+H19+12</f>
         <v>113</v>
       </c>
       <c r="I20" t="s">
+        <v>243</v>
+      </c>
+      <c r="J20" t="s">
         <v>244</v>
-      </c>
-      <c r="J20" t="s">
-        <v>245</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="2"/>
@@ -5494,17 +5575,17 @@
         <v>GAME_STATUS</v>
       </c>
       <c r="G21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="I21" t="s">
+        <v>243</v>
+      </c>
+      <c r="J21" t="s">
         <v>244</v>
-      </c>
-      <c r="J21" t="s">
-        <v>245</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="2"/>
@@ -5532,17 +5613,17 @@
         <v>MY_CHAR_NUM</v>
       </c>
       <c r="G22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="I22" t="s">
+        <v>243</v>
+      </c>
+      <c r="J22" t="s">
         <v>244</v>
-      </c>
-      <c r="J22" t="s">
-        <v>245</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="2"/>
@@ -5570,17 +5651,17 @@
         <v>ACT_NAME</v>
       </c>
       <c r="G23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="I23" t="s">
+        <v>243</v>
+      </c>
+      <c r="J23" t="s">
         <v>244</v>
-      </c>
-      <c r="J23" t="s">
-        <v>245</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="2"/>
@@ -5608,17 +5689,17 @@
         <v>BANK_AFTER_SPEND</v>
       </c>
       <c r="G24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="I24" t="s">
+        <v>243</v>
+      </c>
+      <c r="J24" t="s">
         <v>244</v>
-      </c>
-      <c r="J24" t="s">
-        <v>245</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="2"/>
@@ -5646,17 +5727,17 @@
         <v>ATTACK_BAL</v>
       </c>
       <c r="G25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
         <v>138</v>
       </c>
       <c r="I25" t="s">
+        <v>243</v>
+      </c>
+      <c r="J25" t="s">
         <v>244</v>
-      </c>
-      <c r="J25" t="s">
-        <v>245</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="2"/>
@@ -5684,17 +5765,17 @@
         <v>ATT_DON</v>
       </c>
       <c r="G26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
         <v>143</v>
       </c>
       <c r="I26" t="s">
+        <v>243</v>
+      </c>
+      <c r="J26" t="s">
         <v>244</v>
-      </c>
-      <c r="J26" t="s">
-        <v>245</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="2"/>
@@ -5722,17 +5803,17 @@
         <v>WILL_NO</v>
       </c>
       <c r="G27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
         <v>148</v>
       </c>
       <c r="I27" t="s">
+        <v>243</v>
+      </c>
+      <c r="J27" t="s">
         <v>244</v>
-      </c>
-      <c r="J27" t="s">
-        <v>245</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="2"/>
@@ -5760,17 +5841,17 @@
         <v>MIRROR_NO</v>
       </c>
       <c r="G28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
         <v>153</v>
       </c>
       <c r="I28" t="s">
+        <v>243</v>
+      </c>
+      <c r="J28" t="s">
         <v>244</v>
-      </c>
-      <c r="J28" t="s">
-        <v>245</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="2"/>
@@ -5798,17 +5879,17 @@
         <v>AD_PIN</v>
       </c>
       <c r="G29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
         <v>158</v>
       </c>
       <c r="I29" t="s">
+        <v>243</v>
+      </c>
+      <c r="J29" t="s">
         <v>244</v>
-      </c>
-      <c r="J29" t="s">
-        <v>245</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="2"/>
@@ -5836,17 +5917,17 @@
         <v>AD_CLY</v>
       </c>
       <c r="G30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
         <v>163</v>
       </c>
       <c r="I30" t="s">
+        <v>243</v>
+      </c>
+      <c r="J30" t="s">
         <v>244</v>
-      </c>
-      <c r="J30" t="s">
-        <v>245</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="2"/>
@@ -5874,17 +5955,17 @@
         <v>AD_CHE</v>
       </c>
       <c r="G31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="I31" t="s">
+        <v>243</v>
+      </c>
+      <c r="J31" t="s">
         <v>244</v>
-      </c>
-      <c r="J31" t="s">
-        <v>245</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="2"/>
@@ -5912,17 +5993,17 @@
         <v>AD_PAC</v>
       </c>
       <c r="G32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
         <v>173</v>
       </c>
       <c r="I32" t="s">
+        <v>243</v>
+      </c>
+      <c r="J32" t="s">
         <v>244</v>
-      </c>
-      <c r="J32" t="s">
-        <v>245</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="2"/>
@@ -5950,17 +6031,17 @@
         <v>AD_BLI</v>
       </c>
       <c r="G33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
       <c r="I33" t="s">
+        <v>243</v>
+      </c>
+      <c r="J33" t="s">
         <v>244</v>
-      </c>
-      <c r="J33" t="s">
-        <v>245</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="2"/>
@@ -5988,17 +6069,17 @@
         <v>AD_INK</v>
       </c>
       <c r="G34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
       <c r="I34" t="s">
+        <v>243</v>
+      </c>
+      <c r="J34" t="s">
         <v>244</v>
-      </c>
-      <c r="J34" t="s">
-        <v>245</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="2"/>
@@ -6026,17 +6107,17 @@
         <v>MB_PIN</v>
       </c>
       <c r="G35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
         <v>188</v>
       </c>
       <c r="I35" t="s">
+        <v>243</v>
+      </c>
+      <c r="J35" t="s">
         <v>244</v>
-      </c>
-      <c r="J35" t="s">
-        <v>245</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="2"/>
@@ -6064,17 +6145,17 @@
         <v>MB_CLY</v>
       </c>
       <c r="G36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H36">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
       <c r="I36" t="s">
+        <v>243</v>
+      </c>
+      <c r="J36" t="s">
         <v>244</v>
-      </c>
-      <c r="J36" t="s">
-        <v>245</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="2"/>
@@ -6102,17 +6183,17 @@
         <v>MB_CHE</v>
       </c>
       <c r="G37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
         <v>198</v>
       </c>
       <c r="I37" t="s">
+        <v>243</v>
+      </c>
+      <c r="J37" t="s">
         <v>244</v>
-      </c>
-      <c r="J37" t="s">
-        <v>245</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="2"/>
@@ -6140,17 +6221,17 @@
         <v>MB_PAC</v>
       </c>
       <c r="G38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H38">
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
       <c r="I38" t="s">
+        <v>243</v>
+      </c>
+      <c r="J38" t="s">
         <v>244</v>
-      </c>
-      <c r="J38" t="s">
-        <v>245</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="2"/>
@@ -6178,17 +6259,17 @@
         <v>MB_BLI</v>
       </c>
       <c r="G39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H39">
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
       <c r="I39" t="s">
+        <v>243</v>
+      </c>
+      <c r="J39" t="s">
         <v>244</v>
-      </c>
-      <c r="J39" t="s">
-        <v>245</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="2"/>
@@ -6216,17 +6297,17 @@
         <v>MB_INK</v>
       </c>
       <c r="G40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H40">
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
       <c r="I40" t="s">
+        <v>243</v>
+      </c>
+      <c r="J40" t="s">
         <v>244</v>
-      </c>
-      <c r="J40" t="s">
-        <v>245</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="2"/>
@@ -19471,15 +19552,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z54"/>
+  <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="X7" workbookViewId="0">
+      <selection activeCell="Y68" sqref="Y10:Y68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="16" max="17" width="24.42578125" customWidth="1"/>
+    <col min="16" max="16" width="36.5703125" customWidth="1"/>
+    <col min="17" max="17" width="24.42578125" customWidth="1"/>
     <col min="18" max="18" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="22" width="40.85546875" customWidth="1"/>
     <col min="23" max="23" width="81.7109375" style="18" bestFit="1" customWidth="1"/>
@@ -19500,7 +19582,7 @@
     </row>
     <row r="6" spans="1:26">
       <c r="P6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -19511,7 +19593,7 @@
         <v>146</v>
       </c>
       <c r="V8" s="88" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z8" s="91"/>
     </row>
@@ -19520,7 +19602,7 @@
         <v>147</v>
       </c>
       <c r="V9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -19563,16 +19645,16 @@
         <v xml:space="preserve">+ ",11:" + </v>
       </c>
       <c r="W10" s="18" t="str">
-        <f>CONCATENATE("((GlobalVariables) this.getApplication()).set",T10,"(",S10,");")</f>
-        <v>((GlobalVariables) this.getApplication()).setComm_control_value(comm_control_value);</v>
+        <f>CONCATENATE("globalVariables.set",T10,"(",S10,");")</f>
+        <v>globalVariables.setComm_control_value(comm_control_value);</v>
       </c>
       <c r="X10" s="37" t="str">
         <f>CONCATENATE(N10," ",S10,";")</f>
         <v>Integer comm_control_value;</v>
       </c>
       <c r="Y10" s="92" t="str">
-        <f>CONCATENATE(S10," = ((GlobalVariables) this.getApplication()).get",T10,"();")</f>
-        <v>comm_control_value = ((GlobalVariables) this.getApplication()).getComm_control_value();</v>
+        <f t="shared" ref="Y10:Y51" si="0">CONCATENATE(S10," = globalVariables.get",T10,"();")</f>
+        <v>comm_control_value = globalVariables.getComm_control_value();</v>
       </c>
       <c r="Z10" s="90" t="str">
         <f>CONCATENATE("private ",N10," ",P10,"; public ",N10," get",T10,"(){return ",S10,";} public void set",T10,"(",N10," ",S10,"){this.",S10," = ",S10,";}")</f>
@@ -19587,27 +19669,27 @@
         <v>188</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O48" si="0">FIND(";",A11)</f>
+        <f t="shared" ref="O11:O48" si="1">FIND(";",A11)</f>
         <v>24</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" ref="P11:P48" si="1">LEFT(A11,O11-1)</f>
+        <f t="shared" ref="P11:P48" si="2">LEFT(A11,O11-1)</f>
         <v>master_enable_value = 1</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q54" si="2">PROPER(LEFT(P11,FIND("_",P11)-1))</f>
+        <f t="shared" ref="Q11:Q54" si="3">PROPER(LEFT(P11,FIND("_",P11)-1))</f>
         <v>Master</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" ref="R11:R54" si="3">CONCATENATE(Q11,RIGHT(P11,LEN(P11)-LEN(Q11)))</f>
+        <f t="shared" ref="R11:R68" si="4">CONCATENATE(Q11,RIGHT(P11,LEN(P11)-LEN(Q11)))</f>
         <v>Master_enable_value = 1</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" ref="S11:S54" si="4">LEFT(P11,FIND(" =",P11)-1)</f>
+        <f t="shared" ref="S11:S54" si="5">LEFT(P11,FIND(" =",P11)-1)</f>
         <v>master_enable_value</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" ref="T11:T54" si="5">LEFT(R11,FIND(" =",R11)-1)</f>
+        <f t="shared" ref="T11:T68" si="6">LEFT(R11,FIND(" =",R11)-1)</f>
         <v>Master_enable_value</v>
       </c>
       <c r="U11">
@@ -19615,19 +19697,19 @@
         <v>12</v>
       </c>
       <c r="W11" s="18" t="str">
-        <f t="shared" ref="W11:W54" si="6">CONCATENATE("((GlobalVariables) this.getApplication()).set",T11,"(",S11,");")</f>
-        <v>((GlobalVariables) this.getApplication()).setMaster_enable_value(master_enable_value);</v>
+        <f t="shared" ref="W11:W68" si="7">CONCATENATE("globalVariables.set",T11,"(",S11,");")</f>
+        <v>globalVariables.setMaster_enable_value(master_enable_value);</v>
       </c>
       <c r="X11" s="37" t="str">
-        <f t="shared" ref="X11:X54" si="7">CONCATENATE(N11," ",S11,";")</f>
+        <f t="shared" ref="X11:X68" si="8">CONCATENATE(N11," ",S11,";")</f>
         <v>Integer master_enable_value;</v>
       </c>
       <c r="Y11" s="92" t="str">
-        <f t="shared" ref="Y11:Y54" si="8">CONCATENATE(S11," = ((GlobalVariables) this.getApplication()).get",T11,"();")</f>
-        <v>master_enable_value = ((GlobalVariables) this.getApplication()).getMaster_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>master_enable_value = globalVariables.getMaster_enable_value();</v>
       </c>
       <c r="Z11" s="90" t="str">
-        <f t="shared" ref="Z11:Z54" si="9">CONCATENATE("private ",N11," ",P11,"; public ",N11," get",T11,"(){return ",S11,";} public void set",T11,"(",N11," ",S11,"){this.",S11," = ",S11,";}")</f>
+        <f t="shared" ref="Z11:Z68" si="9">CONCATENATE("private ",N11," ",P11,"; public ",N11," get",T11,"(){return ",S11,";} public void set",T11,"(",N11," ",S11,"){this.",S11," = ",S11,";}")</f>
         <v>private Integer master_enable_value = 1; public Integer getMaster_enable_value(){return master_enable_value;} public void setMaster_enable_value(Integer master_enable_value){this.master_enable_value = master_enable_value;}</v>
       </c>
     </row>
@@ -19639,27 +19721,27 @@
         <v>188</v>
       </c>
       <c r="O12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="P12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>light_enable_value = 1</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Light</v>
       </c>
       <c r="R12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Light_enable_value = 1</v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>light_enable_value</v>
       </c>
       <c r="T12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Light_enable_value</v>
       </c>
       <c r="U12">
@@ -19667,16 +19749,16 @@
         <v>13</v>
       </c>
       <c r="W12" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLight_enable_value(light_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLight_enable_value(light_enable_value);</v>
       </c>
       <c r="X12" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer light_enable_value;</v>
       </c>
       <c r="Y12" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>light_enable_value = ((GlobalVariables) this.getApplication()).getLight_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>light_enable_value = globalVariables.getLight_enable_value();</v>
       </c>
       <c r="Z12" s="90" t="str">
         <f t="shared" si="9"/>
@@ -19691,27 +19773,27 @@
         <v>188</v>
       </c>
       <c r="O13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>sound_enable_value = 1</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Sound</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Sound_enable_value = 1</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sound_enable_value</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Sound_enable_value</v>
       </c>
       <c r="U13">
@@ -19719,16 +19801,16 @@
         <v>14</v>
       </c>
       <c r="W13" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setSound_enable_value(sound_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSound_enable_value(sound_enable_value);</v>
       </c>
       <c r="X13" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer sound_enable_value;</v>
       </c>
       <c r="Y13" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>sound_enable_value = ((GlobalVariables) this.getApplication()).getSound_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>sound_enable_value = globalVariables.getSound_enable_value();</v>
       </c>
       <c r="Z13" s="90" t="str">
         <f t="shared" si="9"/>
@@ -19743,27 +19825,27 @@
         <v>188</v>
       </c>
       <c r="O14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>motion_enable_value = 1</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Motion</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Motion_enable_value = 1</v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>motion_enable_value</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Motion_enable_value</v>
       </c>
       <c r="U14">
@@ -19771,16 +19853,16 @@
         <v>15</v>
       </c>
       <c r="W14" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMotion_enable_value(motion_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMotion_enable_value(motion_enable_value);</v>
       </c>
       <c r="X14" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer motion_enable_value;</v>
       </c>
       <c r="Y14" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>motion_enable_value = ((GlobalVariables) this.getApplication()).getMotion_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>motion_enable_value = globalVariables.getMotion_enable_value();</v>
       </c>
       <c r="Z14" s="90" t="str">
         <f t="shared" si="9"/>
@@ -19795,27 +19877,27 @@
         <v>188</v>
       </c>
       <c r="O15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>clock_enable_value = 0</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Clock</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Clock_enable_value = 0</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>clock_enable_value</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Clock_enable_value</v>
       </c>
       <c r="U15">
@@ -19823,16 +19905,16 @@
         <v>16</v>
       </c>
       <c r="W15" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setClock_enable_value(clock_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setClock_enable_value(clock_enable_value);</v>
       </c>
       <c r="X15" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer clock_enable_value;</v>
       </c>
       <c r="Y15" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>clock_enable_value = ((GlobalVariables) this.getApplication()).getClock_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>clock_enable_value = globalVariables.getClock_enable_value();</v>
       </c>
       <c r="Z15" s="90" t="str">
         <f t="shared" si="9"/>
@@ -19847,27 +19929,27 @@
         <v>188</v>
       </c>
       <c r="O16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>light_pinky_enable_value = 1</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Light</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Light_pinky_enable_value = 1</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>light_pinky_enable_value</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Light_pinky_enable_value</v>
       </c>
       <c r="U16">
@@ -19875,16 +19957,16 @@
         <v>17</v>
       </c>
       <c r="W16" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLight_pinky_enable_value(light_pinky_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLight_pinky_enable_value(light_pinky_enable_value);</v>
       </c>
       <c r="X16" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer light_pinky_enable_value;</v>
       </c>
       <c r="Y16" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>light_pinky_enable_value = ((GlobalVariables) this.getApplication()).getLight_pinky_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>light_pinky_enable_value = globalVariables.getLight_pinky_enable_value();</v>
       </c>
       <c r="Z16" s="90" t="str">
         <f t="shared" si="9"/>
@@ -19899,27 +19981,27 @@
         <v>188</v>
       </c>
       <c r="O17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>light_clyde_enable_value = 1</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Light</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Light_clyde_enable_value = 1</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>light_clyde_enable_value</v>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Light_clyde_enable_value</v>
       </c>
       <c r="U17">
@@ -19927,16 +20009,16 @@
         <v>18</v>
       </c>
       <c r="W17" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLight_clyde_enable_value(light_clyde_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLight_clyde_enable_value(light_clyde_enable_value);</v>
       </c>
       <c r="X17" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer light_clyde_enable_value;</v>
       </c>
       <c r="Y17" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>light_clyde_enable_value = ((GlobalVariables) this.getApplication()).getLight_clyde_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>light_clyde_enable_value = globalVariables.getLight_clyde_enable_value();</v>
       </c>
       <c r="Z17" s="90" t="str">
         <f t="shared" si="9"/>
@@ -19951,27 +20033,27 @@
         <v>188</v>
       </c>
       <c r="O18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>light_cherry_enable_value = 1</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Light</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Light_cherry_enable_value = 1</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>light_cherry_enable_value</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Light_cherry_enable_value</v>
       </c>
       <c r="U18">
@@ -19979,16 +20061,16 @@
         <v>19</v>
       </c>
       <c r="W18" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLight_cherry_enable_value(light_cherry_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLight_cherry_enable_value(light_cherry_enable_value);</v>
       </c>
       <c r="X18" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer light_cherry_enable_value;</v>
       </c>
       <c r="Y18" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>light_cherry_enable_value = ((GlobalVariables) this.getApplication()).getLight_cherry_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>light_cherry_enable_value = globalVariables.getLight_cherry_enable_value();</v>
       </c>
       <c r="Z18" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20003,27 +20085,27 @@
         <v>188</v>
       </c>
       <c r="O19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>light_pacman_enable_value = 1</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Light</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Light_pacman_enable_value = 1</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>light_pacman_enable_value</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Light_pacman_enable_value</v>
       </c>
       <c r="U19">
@@ -20031,16 +20113,16 @@
         <v>20</v>
       </c>
       <c r="W19" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLight_pacman_enable_value(light_pacman_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLight_pacman_enable_value(light_pacman_enable_value);</v>
       </c>
       <c r="X19" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer light_pacman_enable_value;</v>
       </c>
       <c r="Y19" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>light_pacman_enable_value = ((GlobalVariables) this.getApplication()).getLight_pacman_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>light_pacman_enable_value = globalVariables.getLight_pacman_enable_value();</v>
       </c>
       <c r="Z19" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20055,27 +20137,27 @@
         <v>188</v>
       </c>
       <c r="O20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>light_blinky_enable_value = 1</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Light</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Light_blinky_enable_value = 1</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>light_blinky_enable_value</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Light_blinky_enable_value</v>
       </c>
       <c r="U20">
@@ -20083,16 +20165,16 @@
         <v>21</v>
       </c>
       <c r="W20" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLight_blinky_enable_value(light_blinky_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLight_blinky_enable_value(light_blinky_enable_value);</v>
       </c>
       <c r="X20" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer light_blinky_enable_value;</v>
       </c>
       <c r="Y20" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>light_blinky_enable_value = ((GlobalVariables) this.getApplication()).getLight_blinky_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>light_blinky_enable_value = globalVariables.getLight_blinky_enable_value();</v>
       </c>
       <c r="Z20" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20107,27 +20189,27 @@
         <v>188</v>
       </c>
       <c r="O21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>light_inky_enable_value = 1</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Light</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Light_inky_enable_value = 1</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>light_inky_enable_value</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Light_inky_enable_value</v>
       </c>
       <c r="U21">
@@ -20135,16 +20217,16 @@
         <v>22</v>
       </c>
       <c r="W21" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLight_inky_enable_value(light_inky_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLight_inky_enable_value(light_inky_enable_value);</v>
       </c>
       <c r="X21" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer light_inky_enable_value;</v>
       </c>
       <c r="Y21" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>light_inky_enable_value = ((GlobalVariables) this.getApplication()).getLight_inky_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>light_inky_enable_value = globalVariables.getLight_inky_enable_value();</v>
       </c>
       <c r="Z21" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20159,27 +20241,27 @@
         <v>188</v>
       </c>
       <c r="O22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="P22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>lightsensor_enable_value = 1</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Lightsensor</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Lightsensor_enable_value = 1</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>lightsensor_enable_value</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Lightsensor_enable_value</v>
       </c>
       <c r="U22">
@@ -20187,16 +20269,16 @@
         <v>23</v>
       </c>
       <c r="W22" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLightsensor_enable_value(lightsensor_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLightsensor_enable_value(lightsensor_enable_value);</v>
       </c>
       <c r="X22" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer lightsensor_enable_value;</v>
       </c>
       <c r="Y22" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>lightsensor_enable_value = ((GlobalVariables) this.getApplication()).getLightsensor_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>lightsensor_enable_value = globalVariables.getLightsensor_enable_value();</v>
       </c>
       <c r="Z22" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20211,27 +20293,27 @@
         <v>188</v>
       </c>
       <c r="O23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>lightsensor_trigger_value = 1550</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Lightsensor</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Lightsensor_trigger_value = 1550</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>lightsensor_trigger_value</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Lightsensor_trigger_value</v>
       </c>
       <c r="U23">
@@ -20239,16 +20321,16 @@
         <v>24</v>
       </c>
       <c r="W23" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setLightsensor_trigger_value(lightsensor_trigger_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setLightsensor_trigger_value(lightsensor_trigger_value);</v>
       </c>
       <c r="X23" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer lightsensor_trigger_value;</v>
       </c>
       <c r="Y23" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>lightsensor_trigger_value = ((GlobalVariables) this.getApplication()).getLightsensor_trigger_value();</v>
+        <f t="shared" si="0"/>
+        <v>lightsensor_trigger_value = globalVariables.getLightsensor_trigger_value();</v>
       </c>
       <c r="Z23" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20263,27 +20345,27 @@
         <v>188</v>
       </c>
       <c r="O24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>nightlight_enable_value = 1</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Nightlight</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Nightlight_enable_value = 1</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>nightlight_enable_value</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Nightlight_enable_value</v>
       </c>
       <c r="U24">
@@ -20291,16 +20373,16 @@
         <v>25</v>
       </c>
       <c r="W24" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setNightlight_enable_value(nightlight_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setNightlight_enable_value(nightlight_enable_value);</v>
       </c>
       <c r="X24" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer nightlight_enable_value;</v>
       </c>
       <c r="Y24" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>nightlight_enable_value = ((GlobalVariables) this.getApplication()).getNightlight_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>nightlight_enable_value = globalVariables.getNightlight_enable_value();</v>
       </c>
       <c r="Z24" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20315,27 +20397,27 @@
         <v>188</v>
       </c>
       <c r="O25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>alarm_enable_value = 1</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Alarm</v>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Alarm_enable_value = 1</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>alarm_enable_value</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Alarm_enable_value</v>
       </c>
       <c r="U25">
@@ -20343,16 +20425,16 @@
         <v>26</v>
       </c>
       <c r="W25" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAlarm_enable_value(alarm_enable_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAlarm_enable_value(alarm_enable_value);</v>
       </c>
       <c r="X25" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer alarm_enable_value;</v>
       </c>
       <c r="Y25" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>alarm_enable_value = ((GlobalVariables) this.getApplication()).getAlarm_enable_value();</v>
+        <f t="shared" si="0"/>
+        <v>alarm_enable_value = globalVariables.getAlarm_enable_value();</v>
       </c>
       <c r="Z25" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20367,27 +20449,27 @@
         <v>138</v>
       </c>
       <c r="O26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>alarm_date_value = "02/25/1963"</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Alarm</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Alarm_date_value = "02/25/1963"</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>alarm_date_value</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Alarm_date_value</v>
       </c>
       <c r="U26">
@@ -20395,16 +20477,16 @@
         <v>27</v>
       </c>
       <c r="W26" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAlarm_date_value(alarm_date_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAlarm_date_value(alarm_date_value);</v>
       </c>
       <c r="X26" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String alarm_date_value;</v>
       </c>
       <c r="Y26" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>alarm_date_value = ((GlobalVariables) this.getApplication()).getAlarm_date_value();</v>
+        <f t="shared" si="0"/>
+        <v>alarm_date_value = globalVariables.getAlarm_date_value();</v>
       </c>
       <c r="Z26" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20419,27 +20501,27 @@
         <v>138</v>
       </c>
       <c r="O27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>alarm_time_value = "12:00:00"</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Alarm</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Alarm_time_value = "12:00:00"</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>alarm_time_value</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Alarm_time_value</v>
       </c>
       <c r="U27">
@@ -20447,16 +20529,16 @@
         <v>28</v>
       </c>
       <c r="W27" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAlarm_time_value(alarm_time_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAlarm_time_value(alarm_time_value);</v>
       </c>
       <c r="X27" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String alarm_time_value;</v>
       </c>
       <c r="Y27" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>alarm_time_value = ((GlobalVariables) this.getApplication()).getAlarm_time_value();</v>
+        <f t="shared" si="0"/>
+        <v>alarm_time_value = globalVariables.getAlarm_time_value();</v>
       </c>
       <c r="Z27" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20471,27 +20553,27 @@
         <v>188</v>
       </c>
       <c r="O28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>performance_number_value = 71</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Performance</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Performance_number_value = 71</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>performance_number_value</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Performance_number_value</v>
       </c>
       <c r="U28">
@@ -20499,16 +20581,16 @@
         <v>29</v>
       </c>
       <c r="W28" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setPerformance_number_value(performance_number_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setPerformance_number_value(performance_number_value);</v>
       </c>
       <c r="X28" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer performance_number_value;</v>
       </c>
       <c r="Y28" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>performance_number_value = ((GlobalVariables) this.getApplication()).getPerformance_number_value();</v>
+        <f t="shared" si="0"/>
+        <v>performance_number_value = globalVariables.getPerformance_number_value();</v>
       </c>
       <c r="Z28" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20523,27 +20605,27 @@
         <v>188</v>
       </c>
       <c r="O29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>stayin_game_status_value = 0</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Stayin</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Stayin_game_status_value = 0</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>stayin_game_status_value</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Stayin_game_status_value</v>
       </c>
       <c r="U29">
@@ -20551,16 +20633,16 @@
         <v>41</v>
       </c>
       <c r="W29" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setStayin_game_status_value(stayin_game_status_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setStayin_game_status_value(stayin_game_status_value);</v>
       </c>
       <c r="X29" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer stayin_game_status_value;</v>
       </c>
       <c r="Y29" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>stayin_game_status_value = ((GlobalVariables) this.getApplication()).getStayin_game_status_value();</v>
+        <f t="shared" si="0"/>
+        <v>stayin_game_status_value = globalVariables.getStayin_game_status_value();</v>
       </c>
       <c r="Z29" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20575,27 +20657,27 @@
         <v>188</v>
       </c>
       <c r="O30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>my_char_number_value = 0</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>My</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>My_char_number_value = 0</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>my_char_number_value</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>My_char_number_value</v>
       </c>
       <c r="U30">
@@ -20603,16 +20685,16 @@
         <v>42</v>
       </c>
       <c r="W30" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMy_char_number_value(my_char_number_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMy_char_number_value(my_char_number_value);</v>
       </c>
       <c r="X30" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer my_char_number_value;</v>
       </c>
       <c r="Y30" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>my_char_number_value = ((GlobalVariables) this.getApplication()).getMy_char_number_value();</v>
+        <f t="shared" si="0"/>
+        <v>my_char_number_value = globalVariables.getMy_char_number_value();</v>
       </c>
       <c r="Z30" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20627,27 +20709,27 @@
         <v>138</v>
       </c>
       <c r="O31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>actual_name_value = "abcdefg"</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Actual</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Actual_name_value = "abcdefg"</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>actual_name_value</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Actual_name_value</v>
       </c>
       <c r="U31">
@@ -20655,16 +20737,16 @@
         <v>43</v>
       </c>
       <c r="W31" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setActual_name_value(actual_name_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setActual_name_value(actual_name_value);</v>
       </c>
       <c r="X31" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String actual_name_value;</v>
       </c>
       <c r="Y31" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>actual_name_value = ((GlobalVariables) this.getApplication()).getActual_name_value();</v>
+        <f t="shared" si="0"/>
+        <v>actual_name_value = globalVariables.getActual_name_value();</v>
       </c>
       <c r="Z31" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20679,27 +20761,27 @@
         <v>188</v>
       </c>
       <c r="O32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="P32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>bank_after_spende_value = 9100</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Bank</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Bank_after_spende_value = 9100</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>bank_after_spende_value</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Bank_after_spende_value</v>
       </c>
       <c r="U32">
@@ -20707,16 +20789,16 @@
         <v>44</v>
       </c>
       <c r="W32" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setBank_after_spende_value(bank_after_spende_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setBank_after_spende_value(bank_after_spende_value);</v>
       </c>
       <c r="X32" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer bank_after_spende_value;</v>
       </c>
       <c r="Y32" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>bank_after_spende_value = ((GlobalVariables) this.getApplication()).getBank_after_spende_value();</v>
+        <f t="shared" si="0"/>
+        <v>bank_after_spende_value = globalVariables.getBank_after_spende_value();</v>
       </c>
       <c r="Z32" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20731,27 +20813,27 @@
         <v>188</v>
       </c>
       <c r="O33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="P33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_balance_value = 9100</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_balance_value = 9100</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_balance_value</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_balance_value</v>
       </c>
       <c r="U33">
@@ -20759,16 +20841,16 @@
         <v>45</v>
       </c>
       <c r="W33" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_balance_value(attack_balance_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_balance_value(attack_balance_value);</v>
       </c>
       <c r="X33" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer attack_balance_value;</v>
       </c>
       <c r="Y33" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_balance_value = ((GlobalVariables) this.getApplication()).getAttack_balance_value();</v>
+        <f t="shared" si="0"/>
+        <v>attack_balance_value = globalVariables.getAttack_balance_value();</v>
       </c>
       <c r="Z33" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20780,30 +20862,30 @@
         <v>169</v>
       </c>
       <c r="N34" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_or_donate_character_flags = 9000000</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_or_donate_character_flags = 9000000</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_or_donate_character_flags</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_or_donate_character_flags</v>
       </c>
       <c r="U34">
@@ -20811,20 +20893,20 @@
         <v>46</v>
       </c>
       <c r="W34" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_or_donate_character_flags(attack_or_donate_character_flags);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_or_donate_character_flags(attack_or_donate_character_flags);</v>
       </c>
       <c r="X34" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long attack_or_donate_character_flags;</v>
+        <f t="shared" si="8"/>
+        <v>long attack_or_donate_character_flags;</v>
       </c>
       <c r="Y34" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_or_donate_character_flags = ((GlobalVariables) this.getApplication()).getAttack_or_donate_character_flags();</v>
+        <f t="shared" si="0"/>
+        <v>attack_or_donate_character_flags = globalVariables.getAttack_or_donate_character_flags();</v>
       </c>
       <c r="Z34" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long attack_or_donate_character_flags = 9000000; public Long getAttack_or_donate_character_flags(){return attack_or_donate_character_flags;} public void setAttack_or_donate_character_flags(Long attack_or_donate_character_flags){this.attack_or_donate_character_flags = attack_or_donate_character_flags;}</v>
+        <v>private long attack_or_donate_character_flags = 9000000; public long getAttack_or_donate_character_flags(){return attack_or_donate_character_flags;} public void setAttack_or_donate_character_flags(long attack_or_donate_character_flags){this.attack_or_donate_character_flags = attack_or_donate_character_flags;}</v>
       </c>
     </row>
     <row r="35" spans="1:26">
@@ -20832,30 +20914,30 @@
         <v>170</v>
       </c>
       <c r="N35" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>will_or_no_character_flags = 9000000</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Will</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Will_or_no_character_flags = 9000000</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>will_or_no_character_flags</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Will_or_no_character_flags</v>
       </c>
       <c r="U35">
@@ -20863,20 +20945,20 @@
         <v>47</v>
       </c>
       <c r="W35" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setWill_or_no_character_flags(will_or_no_character_flags);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setWill_or_no_character_flags(will_or_no_character_flags);</v>
       </c>
       <c r="X35" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long will_or_no_character_flags;</v>
+        <f t="shared" si="8"/>
+        <v>long will_or_no_character_flags;</v>
       </c>
       <c r="Y35" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>will_or_no_character_flags = ((GlobalVariables) this.getApplication()).getWill_or_no_character_flags();</v>
+        <f t="shared" si="0"/>
+        <v>will_or_no_character_flags = globalVariables.getWill_or_no_character_flags();</v>
       </c>
       <c r="Z35" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long will_or_no_character_flags = 9000000; public Long getWill_or_no_character_flags(){return will_or_no_character_flags;} public void setWill_or_no_character_flags(Long will_or_no_character_flags){this.will_or_no_character_flags = will_or_no_character_flags;}</v>
+        <v>private long will_or_no_character_flags = 9000000; public long getWill_or_no_character_flags(){return will_or_no_character_flags;} public void setWill_or_no_character_flags(long will_or_no_character_flags){this.will_or_no_character_flags = will_or_no_character_flags;}</v>
       </c>
     </row>
     <row r="36" spans="1:26">
@@ -20884,30 +20966,30 @@
         <v>171</v>
       </c>
       <c r="N36" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mirror_or_no_character_flags = 9111111</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Mirror</v>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mirror_or_no_character_flags = 9111111</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>mirror_or_no_character_flags</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Mirror_or_no_character_flags</v>
       </c>
       <c r="U36">
@@ -20915,20 +20997,20 @@
         <v>48</v>
       </c>
       <c r="W36" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMirror_or_no_character_flags(mirror_or_no_character_flags);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMirror_or_no_character_flags(mirror_or_no_character_flags);</v>
       </c>
       <c r="X36" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long mirror_or_no_character_flags;</v>
+        <f t="shared" si="8"/>
+        <v>long mirror_or_no_character_flags;</v>
       </c>
       <c r="Y36" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>mirror_or_no_character_flags = ((GlobalVariables) this.getApplication()).getMirror_or_no_character_flags();</v>
+        <f t="shared" si="0"/>
+        <v>mirror_or_no_character_flags = globalVariables.getMirror_or_no_character_flags();</v>
       </c>
       <c r="Z36" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long mirror_or_no_character_flags = 9111111; public Long getMirror_or_no_character_flags(){return mirror_or_no_character_flags;} public void setMirror_or_no_character_flags(Long mirror_or_no_character_flags){this.mirror_or_no_character_flags = mirror_or_no_character_flags;}</v>
+        <v>private long mirror_or_no_character_flags = 9111111; public long getMirror_or_no_character_flags(){return mirror_or_no_character_flags;} public void setMirror_or_no_character_flags(long mirror_or_no_character_flags){this.mirror_or_no_character_flags = mirror_or_no_character_flags;}</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -20939,27 +21021,27 @@
         <v>188</v>
       </c>
       <c r="O37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_or_donate_amnt_pinky = 9000</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_or_donate_amnt_pinky = 9000</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_or_donate_amnt_pinky</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_or_donate_amnt_pinky</v>
       </c>
       <c r="U37">
@@ -20967,16 +21049,16 @@
         <v>49</v>
       </c>
       <c r="W37" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_or_donate_amnt_pinky(attack_or_donate_amnt_pinky);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_or_donate_amnt_pinky(attack_or_donate_amnt_pinky);</v>
       </c>
       <c r="X37" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer attack_or_donate_amnt_pinky;</v>
       </c>
       <c r="Y37" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_or_donate_amnt_pinky = ((GlobalVariables) this.getApplication()).getAttack_or_donate_amnt_pinky();</v>
+        <f t="shared" si="0"/>
+        <v>attack_or_donate_amnt_pinky = globalVariables.getAttack_or_donate_amnt_pinky();</v>
       </c>
       <c r="Z37" s="90" t="str">
         <f t="shared" si="9"/>
@@ -20991,27 +21073,27 @@
         <v>188</v>
       </c>
       <c r="O38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_or_donate_amnt_clyde = 9000</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_or_donate_amnt_clyde = 9000</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_or_donate_amnt_clyde</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_or_donate_amnt_clyde</v>
       </c>
       <c r="U38">
@@ -21019,16 +21101,16 @@
         <v>50</v>
       </c>
       <c r="W38" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_or_donate_amnt_clyde(attack_or_donate_amnt_clyde);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_or_donate_amnt_clyde(attack_or_donate_amnt_clyde);</v>
       </c>
       <c r="X38" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer attack_or_donate_amnt_clyde;</v>
       </c>
       <c r="Y38" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_or_donate_amnt_clyde = ((GlobalVariables) this.getApplication()).getAttack_or_donate_amnt_clyde();</v>
+        <f t="shared" si="0"/>
+        <v>attack_or_donate_amnt_clyde = globalVariables.getAttack_or_donate_amnt_clyde();</v>
       </c>
       <c r="Z38" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21043,27 +21125,27 @@
         <v>188</v>
       </c>
       <c r="O39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="P39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_or_donate_amnt_cherry = 9000</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_or_donate_amnt_cherry = 9000</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_or_donate_amnt_cherry</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_or_donate_amnt_cherry</v>
       </c>
       <c r="U39">
@@ -21071,16 +21153,16 @@
         <v>51</v>
       </c>
       <c r="W39" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_or_donate_amnt_cherry(attack_or_donate_amnt_cherry);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_or_donate_amnt_cherry(attack_or_donate_amnt_cherry);</v>
       </c>
       <c r="X39" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer attack_or_donate_amnt_cherry;</v>
       </c>
       <c r="Y39" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_or_donate_amnt_cherry = ((GlobalVariables) this.getApplication()).getAttack_or_donate_amnt_cherry();</v>
+        <f t="shared" si="0"/>
+        <v>attack_or_donate_amnt_cherry = globalVariables.getAttack_or_donate_amnt_cherry();</v>
       </c>
       <c r="Z39" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21095,27 +21177,27 @@
         <v>188</v>
       </c>
       <c r="O40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="P40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_or_donate_amnt_pacman = 9000</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_or_donate_amnt_pacman = 9000</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_or_donate_amnt_pacman</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_or_donate_amnt_pacman</v>
       </c>
       <c r="U40">
@@ -21123,16 +21205,16 @@
         <v>52</v>
       </c>
       <c r="W40" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_or_donate_amnt_pacman(attack_or_donate_amnt_pacman);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_or_donate_amnt_pacman(attack_or_donate_amnt_pacman);</v>
       </c>
       <c r="X40" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer attack_or_donate_amnt_pacman;</v>
       </c>
       <c r="Y40" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_or_donate_amnt_pacman = ((GlobalVariables) this.getApplication()).getAttack_or_donate_amnt_pacman();</v>
+        <f t="shared" si="0"/>
+        <v>attack_or_donate_amnt_pacman = globalVariables.getAttack_or_donate_amnt_pacman();</v>
       </c>
       <c r="Z40" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21147,27 +21229,27 @@
         <v>188</v>
       </c>
       <c r="O41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="P41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_or_donate_amnt_blinky = 9000</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_or_donate_amnt_blinky = 9000</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_or_donate_amnt_blinky</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_or_donate_amnt_blinky</v>
       </c>
       <c r="U41">
@@ -21175,16 +21257,16 @@
         <v>53</v>
       </c>
       <c r="W41" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_or_donate_amnt_blinky(attack_or_donate_amnt_blinky);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_or_donate_amnt_blinky(attack_or_donate_amnt_blinky);</v>
       </c>
       <c r="X41" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer attack_or_donate_amnt_blinky;</v>
       </c>
       <c r="Y41" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_or_donate_amnt_blinky = ((GlobalVariables) this.getApplication()).getAttack_or_donate_amnt_blinky();</v>
+        <f t="shared" si="0"/>
+        <v>attack_or_donate_amnt_blinky = globalVariables.getAttack_or_donate_amnt_blinky();</v>
       </c>
       <c r="Z41" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21199,27 +21281,27 @@
         <v>188</v>
       </c>
       <c r="O42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>attack_or_donate_amnt_inky = 9000</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Attack</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Attack_or_donate_amnt_inky = 9000</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>attack_or_donate_amnt_inky</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Attack_or_donate_amnt_inky</v>
       </c>
       <c r="U42">
@@ -21227,16 +21309,16 @@
         <v>54</v>
       </c>
       <c r="W42" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setAttack_or_donate_amnt_inky(attack_or_donate_amnt_inky);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setAttack_or_donate_amnt_inky(attack_or_donate_amnt_inky);</v>
       </c>
       <c r="X42" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Integer attack_or_donate_amnt_inky;</v>
       </c>
       <c r="Y42" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>attack_or_donate_amnt_inky = ((GlobalVariables) this.getApplication()).getAttack_or_donate_amnt_inky();</v>
+        <f t="shared" si="0"/>
+        <v>attack_or_donate_amnt_inky = globalVariables.getAttack_or_donate_amnt_inky();</v>
       </c>
       <c r="Z42" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21248,30 +21330,30 @@
         <v>178</v>
       </c>
       <c r="N43" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="P43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mirror_balances_pinky_value = 9111111</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Mirror</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mirror_balances_pinky_value = 9111111</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>mirror_balances_pinky_value</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Mirror_balances_pinky_value</v>
       </c>
       <c r="U43">
@@ -21279,20 +21361,20 @@
         <v>55</v>
       </c>
       <c r="W43" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMirror_balances_pinky_value(mirror_balances_pinky_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMirror_balances_pinky_value(mirror_balances_pinky_value);</v>
       </c>
       <c r="X43" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long mirror_balances_pinky_value;</v>
+        <f t="shared" si="8"/>
+        <v>long mirror_balances_pinky_value;</v>
       </c>
       <c r="Y43" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>mirror_balances_pinky_value = ((GlobalVariables) this.getApplication()).getMirror_balances_pinky_value();</v>
+        <f t="shared" si="0"/>
+        <v>mirror_balances_pinky_value = globalVariables.getMirror_balances_pinky_value();</v>
       </c>
       <c r="Z43" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long mirror_balances_pinky_value = 9111111; public Long getMirror_balances_pinky_value(){return mirror_balances_pinky_value;} public void setMirror_balances_pinky_value(Long mirror_balances_pinky_value){this.mirror_balances_pinky_value = mirror_balances_pinky_value;}</v>
+        <v>private long mirror_balances_pinky_value = 9111111; public long getMirror_balances_pinky_value(){return mirror_balances_pinky_value;} public void setMirror_balances_pinky_value(long mirror_balances_pinky_value){this.mirror_balances_pinky_value = mirror_balances_pinky_value;}</v>
       </c>
     </row>
     <row r="44" spans="1:26">
@@ -21300,30 +21382,30 @@
         <v>179</v>
       </c>
       <c r="N44" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="P44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mirror_balances_clyde_value = 9111111</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Mirror</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mirror_balances_clyde_value = 9111111</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>mirror_balances_clyde_value</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Mirror_balances_clyde_value</v>
       </c>
       <c r="U44">
@@ -21331,20 +21413,20 @@
         <v>56</v>
       </c>
       <c r="W44" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMirror_balances_clyde_value(mirror_balances_clyde_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMirror_balances_clyde_value(mirror_balances_clyde_value);</v>
       </c>
       <c r="X44" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long mirror_balances_clyde_value;</v>
+        <f t="shared" si="8"/>
+        <v>long mirror_balances_clyde_value;</v>
       </c>
       <c r="Y44" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>mirror_balances_clyde_value = ((GlobalVariables) this.getApplication()).getMirror_balances_clyde_value();</v>
+        <f t="shared" si="0"/>
+        <v>mirror_balances_clyde_value = globalVariables.getMirror_balances_clyde_value();</v>
       </c>
       <c r="Z44" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long mirror_balances_clyde_value = 9111111; public Long getMirror_balances_clyde_value(){return mirror_balances_clyde_value;} public void setMirror_balances_clyde_value(Long mirror_balances_clyde_value){this.mirror_balances_clyde_value = mirror_balances_clyde_value;}</v>
+        <v>private long mirror_balances_clyde_value = 9111111; public long getMirror_balances_clyde_value(){return mirror_balances_clyde_value;} public void setMirror_balances_clyde_value(long mirror_balances_clyde_value){this.mirror_balances_clyde_value = mirror_balances_clyde_value;}</v>
       </c>
     </row>
     <row r="45" spans="1:26">
@@ -21352,30 +21434,30 @@
         <v>180</v>
       </c>
       <c r="N45" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="P45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mirror_balances_cherry_value = 9111111</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Mirror</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mirror_balances_cherry_value = 9111111</v>
       </c>
       <c r="S45" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>mirror_balances_cherry_value</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Mirror_balances_cherry_value</v>
       </c>
       <c r="U45">
@@ -21383,20 +21465,20 @@
         <v>57</v>
       </c>
       <c r="W45" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMirror_balances_cherry_value(mirror_balances_cherry_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMirror_balances_cherry_value(mirror_balances_cherry_value);</v>
       </c>
       <c r="X45" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long mirror_balances_cherry_value;</v>
+        <f t="shared" si="8"/>
+        <v>long mirror_balances_cherry_value;</v>
       </c>
       <c r="Y45" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>mirror_balances_cherry_value = ((GlobalVariables) this.getApplication()).getMirror_balances_cherry_value();</v>
+        <f t="shared" si="0"/>
+        <v>mirror_balances_cherry_value = globalVariables.getMirror_balances_cherry_value();</v>
       </c>
       <c r="Z45" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long mirror_balances_cherry_value = 9111111; public Long getMirror_balances_cherry_value(){return mirror_balances_cherry_value;} public void setMirror_balances_cherry_value(Long mirror_balances_cherry_value){this.mirror_balances_cherry_value = mirror_balances_cherry_value;}</v>
+        <v>private long mirror_balances_cherry_value = 9111111; public long getMirror_balances_cherry_value(){return mirror_balances_cherry_value;} public void setMirror_balances_cherry_value(long mirror_balances_cherry_value){this.mirror_balances_cherry_value = mirror_balances_cherry_value;}</v>
       </c>
     </row>
     <row r="46" spans="1:26">
@@ -21404,30 +21486,30 @@
         <v>181</v>
       </c>
       <c r="N46" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mirror_balances_pacman_value = 9111111</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Mirror</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mirror_balances_pacman_value = 9111111</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>mirror_balances_pacman_value</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Mirror_balances_pacman_value</v>
       </c>
       <c r="U46">
@@ -21435,20 +21517,20 @@
         <v>58</v>
       </c>
       <c r="W46" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMirror_balances_pacman_value(mirror_balances_pacman_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMirror_balances_pacman_value(mirror_balances_pacman_value);</v>
       </c>
       <c r="X46" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long mirror_balances_pacman_value;</v>
+        <f t="shared" si="8"/>
+        <v>long mirror_balances_pacman_value;</v>
       </c>
       <c r="Y46" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>mirror_balances_pacman_value = ((GlobalVariables) this.getApplication()).getMirror_balances_pacman_value();</v>
+        <f t="shared" si="0"/>
+        <v>mirror_balances_pacman_value = globalVariables.getMirror_balances_pacman_value();</v>
       </c>
       <c r="Z46" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long mirror_balances_pacman_value = 9111111; public Long getMirror_balances_pacman_value(){return mirror_balances_pacman_value;} public void setMirror_balances_pacman_value(Long mirror_balances_pacman_value){this.mirror_balances_pacman_value = mirror_balances_pacman_value;}</v>
+        <v>private long mirror_balances_pacman_value = 9111111; public long getMirror_balances_pacman_value(){return mirror_balances_pacman_value;} public void setMirror_balances_pacman_value(long mirror_balances_pacman_value){this.mirror_balances_pacman_value = mirror_balances_pacman_value;}</v>
       </c>
     </row>
     <row r="47" spans="1:26">
@@ -21456,30 +21538,30 @@
         <v>182</v>
       </c>
       <c r="N47" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mirror_balances_blinky_value = 9111111</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Mirror</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mirror_balances_blinky_value = 9111111</v>
       </c>
       <c r="S47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>mirror_balances_blinky_value</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Mirror_balances_blinky_value</v>
       </c>
       <c r="U47">
@@ -21487,20 +21569,20 @@
         <v>59</v>
       </c>
       <c r="W47" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMirror_balances_blinky_value(mirror_balances_blinky_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMirror_balances_blinky_value(mirror_balances_blinky_value);</v>
       </c>
       <c r="X47" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long mirror_balances_blinky_value;</v>
+        <f t="shared" si="8"/>
+        <v>long mirror_balances_blinky_value;</v>
       </c>
       <c r="Y47" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>mirror_balances_blinky_value = ((GlobalVariables) this.getApplication()).getMirror_balances_blinky_value();</v>
+        <f t="shared" si="0"/>
+        <v>mirror_balances_blinky_value = globalVariables.getMirror_balances_blinky_value();</v>
       </c>
       <c r="Z47" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long mirror_balances_blinky_value = 9111111; public Long getMirror_balances_blinky_value(){return mirror_balances_blinky_value;} public void setMirror_balances_blinky_value(Long mirror_balances_blinky_value){this.mirror_balances_blinky_value = mirror_balances_blinky_value;}</v>
+        <v>private long mirror_balances_blinky_value = 9111111; public long getMirror_balances_blinky_value(){return mirror_balances_blinky_value;} public void setMirror_balances_blinky_value(long mirror_balances_blinky_value){this.mirror_balances_blinky_value = mirror_balances_blinky_value;}</v>
       </c>
     </row>
     <row r="48" spans="1:26">
@@ -21508,30 +21590,30 @@
         <v>183</v>
       </c>
       <c r="N48" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mirror_balances_inky_value = 9111111</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Mirror</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mirror_balances_inky_value = 9111111</v>
       </c>
       <c r="S48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>mirror_balances_inky_value</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Mirror_balances_inky_value</v>
       </c>
       <c r="U48">
@@ -21539,20 +21621,20 @@
         <v>60</v>
       </c>
       <c r="W48" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setMirror_balances_inky_value(mirror_balances_inky_value);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setMirror_balances_inky_value(mirror_balances_inky_value);</v>
       </c>
       <c r="X48" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v>Long mirror_balances_inky_value;</v>
+        <f t="shared" si="8"/>
+        <v>long mirror_balances_inky_value;</v>
       </c>
       <c r="Y48" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>mirror_balances_inky_value = ((GlobalVariables) this.getApplication()).getMirror_balances_inky_value();</v>
+        <f t="shared" si="0"/>
+        <v>mirror_balances_inky_value = globalVariables.getMirror_balances_inky_value();</v>
       </c>
       <c r="Z48" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private Long mirror_balances_inky_value = 9111111; public Long getMirror_balances_inky_value(){return mirror_balances_inky_value;} public void setMirror_balances_inky_value(Long mirror_balances_inky_value){this.mirror_balances_inky_value = mirror_balances_inky_value;}</v>
+        <v>private long mirror_balances_inky_value = 9111111; public long getMirror_balances_inky_value(){return mirror_balances_inky_value;} public void setMirror_balances_inky_value(long mirror_balances_inky_value){this.mirror_balances_inky_value = mirror_balances_inky_value;}</v>
       </c>
     </row>
     <row r="49" spans="14:26">
@@ -21560,22 +21642,22 @@
         <v>138</v>
       </c>
       <c r="P49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Pinky</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Pinky_rename = "PINKY"</v>
       </c>
       <c r="S49" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>pinky_rename</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pinky_rename</v>
       </c>
       <c r="U49">
@@ -21583,16 +21665,16 @@
         <v>61</v>
       </c>
       <c r="W49" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setPinky_rename(pinky_rename);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setPinky_rename(pinky_rename);</v>
       </c>
       <c r="X49" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String pinky_rename;</v>
       </c>
       <c r="Y49" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>pinky_rename = ((GlobalVariables) this.getApplication()).getPinky_rename();</v>
+        <f t="shared" si="0"/>
+        <v>pinky_rename = globalVariables.getPinky_rename();</v>
       </c>
       <c r="Z49" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21604,22 +21686,22 @@
         <v>138</v>
       </c>
       <c r="P50" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Clyde</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Clyde_rename = "CLYDE"</v>
       </c>
       <c r="S50" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>clyde_rename</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Clyde_rename</v>
       </c>
       <c r="U50">
@@ -21627,16 +21709,16 @@
         <v>62</v>
       </c>
       <c r="W50" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setClyde_rename(clyde_rename);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setClyde_rename(clyde_rename);</v>
       </c>
       <c r="X50" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String clyde_rename;</v>
       </c>
       <c r="Y50" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>clyde_rename = ((GlobalVariables) this.getApplication()).getClyde_rename();</v>
+        <f t="shared" si="0"/>
+        <v>clyde_rename = globalVariables.getClyde_rename();</v>
       </c>
       <c r="Z50" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21648,22 +21730,22 @@
         <v>138</v>
       </c>
       <c r="P51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Cherry</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Cherry_rename = "CHERRY"</v>
       </c>
       <c r="S51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>cherry_rename</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Cherry_rename</v>
       </c>
       <c r="U51">
@@ -21671,16 +21753,16 @@
         <v>63</v>
       </c>
       <c r="W51" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setCherry_rename(cherry_rename);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setCherry_rename(cherry_rename);</v>
       </c>
       <c r="X51" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String cherry_rename;</v>
       </c>
       <c r="Y51" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>cherry_rename = ((GlobalVariables) this.getApplication()).getCherry_rename();</v>
+        <f t="shared" si="0"/>
+        <v>cherry_rename = globalVariables.getCherry_rename();</v>
       </c>
       <c r="Z51" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21692,22 +21774,22 @@
         <v>138</v>
       </c>
       <c r="P52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Pacman</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Pacman_rename = "PACMAN"</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>pacMan_rename</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pacman_rename</v>
       </c>
       <c r="U52">
@@ -21715,16 +21797,16 @@
         <v>64</v>
       </c>
       <c r="W52" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setPacman_rename(pacMan_rename);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setPacman_rename(pacMan_rename);</v>
       </c>
       <c r="X52" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String pacMan_rename;</v>
       </c>
       <c r="Y52" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>pacMan_rename = ((GlobalVariables) this.getApplication()).getPacman_rename();</v>
+        <f t="shared" ref="Y52:Y67" si="10">CONCATENATE(S52," = globalVariables.get",T52,"();")</f>
+        <v>pacMan_rename = globalVariables.getPacman_rename();</v>
       </c>
       <c r="Z52" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21736,22 +21818,22 @@
         <v>138</v>
       </c>
       <c r="P53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Blinky</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Blinky_rename = "BLINKY"</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>blinky_rename</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Blinky_rename</v>
       </c>
       <c r="U53">
@@ -21759,16 +21841,16 @@
         <v>65</v>
       </c>
       <c r="W53" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setBlinky_rename(blinky_rename);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setBlinky_rename(blinky_rename);</v>
       </c>
       <c r="X53" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String blinky_rename;</v>
       </c>
       <c r="Y53" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>blinky_rename = ((GlobalVariables) this.getApplication()).getBlinky_rename();</v>
+        <f t="shared" si="10"/>
+        <v>blinky_rename = globalVariables.getBlinky_rename();</v>
       </c>
       <c r="Z53" s="90" t="str">
         <f t="shared" si="9"/>
@@ -21780,22 +21862,22 @@
         <v>138</v>
       </c>
       <c r="P54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Inky</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Inky_rename = "INKY"</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inky_rename</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Inky_rename</v>
       </c>
       <c r="U54">
@@ -21803,20 +21885,496 @@
         <v>66</v>
       </c>
       <c r="W54" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>((GlobalVariables) this.getApplication()).setInky_rename(inky_rename);</v>
+        <f t="shared" si="7"/>
+        <v>globalVariables.setInky_rename(inky_rename);</v>
       </c>
       <c r="X54" s="37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>String inky_rename;</v>
       </c>
       <c r="Y54" s="92" t="str">
-        <f t="shared" si="8"/>
-        <v>inky_rename = ((GlobalVariables) this.getApplication()).getInky_rename();</v>
+        <f t="shared" si="10"/>
+        <v>inky_rename = globalVariables.getInky_rename();</v>
       </c>
       <c r="Z54" s="90" t="str">
         <f t="shared" si="9"/>
         <v>private String inky_rename = "INKY"; public String getInky_rename(){return inky_rename;} public void setInky_rename(String inky_rename){this.inky_rename = inky_rename;}</v>
+      </c>
+    </row>
+    <row r="55" spans="14:26">
+      <c r="N55" t="s">
+        <v>139</v>
+      </c>
+      <c r="P55" t="str">
+        <f>CONCATENATE(S55," = ",Q55)</f>
+        <v>sa_game_guAtStart = 900100</v>
+      </c>
+      <c r="Q55">
+        <v>900100</v>
+      </c>
+      <c r="S55" t="s">
+        <v>261</v>
+      </c>
+      <c r="T55" t="s">
+        <v>247</v>
+      </c>
+      <c r="W55" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_guAtStart(sa_game_guAtStart);</v>
+      </c>
+      <c r="X55" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_guAtStart;</v>
+      </c>
+      <c r="Y55" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_guAtStart = globalVariables.getSA_game_guAtStart();</v>
+      </c>
+      <c r="Z55" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_guAtStart = 900100; public long getSA_game_guAtStart(){return sa_game_guAtStart;} public void setSA_game_guAtStart(long sa_game_guAtStart){this.sa_game_guAtStart = sa_game_guAtStart;}</v>
+      </c>
+    </row>
+    <row r="56" spans="14:26">
+      <c r="N56" t="s">
+        <v>139</v>
+      </c>
+      <c r="P56" t="str">
+        <f t="shared" ref="P56:P68" si="11">CONCATENATE(S56," = ",Q56)</f>
+        <v>sa_game_guIncome = 900010</v>
+      </c>
+      <c r="Q56">
+        <v>900010</v>
+      </c>
+      <c r="S56" t="s">
+        <v>262</v>
+      </c>
+      <c r="T56" t="s">
+        <v>248</v>
+      </c>
+      <c r="W56" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_guIncome(sa_game_guIncome);</v>
+      </c>
+      <c r="X56" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_guIncome;</v>
+      </c>
+      <c r="Y56" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_guIncome = globalVariables.getSA_game_guIncome();</v>
+      </c>
+      <c r="Z56" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_guIncome = 900010; public long getSA_game_guIncome(){return sa_game_guIncome;} public void setSA_game_guIncome(long sa_game_guIncome){this.sa_game_guIncome = sa_game_guIncome;}</v>
+      </c>
+    </row>
+    <row r="57" spans="14:26">
+      <c r="N57" t="s">
+        <v>139</v>
+      </c>
+      <c r="P57" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_huAtStart = 900100</v>
+      </c>
+      <c r="Q57">
+        <v>900100</v>
+      </c>
+      <c r="S57" t="s">
+        <v>263</v>
+      </c>
+      <c r="T57" t="s">
+        <v>249</v>
+      </c>
+      <c r="W57" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_huAtStart(sa_game_huAtStart);</v>
+      </c>
+      <c r="X57" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_huAtStart;</v>
+      </c>
+      <c r="Y57" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_huAtStart = globalVariables.getSA_game_huAtStart();</v>
+      </c>
+      <c r="Z57" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_huAtStart = 900100; public long getSA_game_huAtStart(){return sa_game_huAtStart;} public void setSA_game_huAtStart(long sa_game_huAtStart){this.sa_game_huAtStart = sa_game_huAtStart;}</v>
+      </c>
+    </row>
+    <row r="58" spans="14:26">
+      <c r="N58" t="s">
+        <v>139</v>
+      </c>
+      <c r="P58" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_huHealing = 900010</v>
+      </c>
+      <c r="Q58">
+        <v>900010</v>
+      </c>
+      <c r="S58" t="s">
+        <v>264</v>
+      </c>
+      <c r="T58" t="s">
+        <v>250</v>
+      </c>
+      <c r="W58" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_huHealing(sa_game_huHealing);</v>
+      </c>
+      <c r="X58" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_huHealing;</v>
+      </c>
+      <c r="Y58" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_huHealing = globalVariables.getSA_game_huHealing();</v>
+      </c>
+      <c r="Z58" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_huHealing = 900010; public long getSA_game_huHealing(){return sa_game_huHealing;} public void setSA_game_huHealing(long sa_game_huHealing){this.sa_game_huHealing = sa_game_huHealing;}</v>
+      </c>
+    </row>
+    <row r="59" spans="14:26">
+      <c r="N59" t="s">
+        <v>139</v>
+      </c>
+      <c r="P59" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_hu4gu = 900001</v>
+      </c>
+      <c r="Q59">
+        <v>900001</v>
+      </c>
+      <c r="S59" t="s">
+        <v>265</v>
+      </c>
+      <c r="T59" t="s">
+        <v>251</v>
+      </c>
+      <c r="W59" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_hu4gu(sa_game_hu4gu);</v>
+      </c>
+      <c r="X59" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_hu4gu;</v>
+      </c>
+      <c r="Y59" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_hu4gu = globalVariables.getSA_game_hu4gu();</v>
+      </c>
+      <c r="Z59" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_hu4gu = 900001; public long getSA_game_hu4gu(){return sa_game_hu4gu;} public void setSA_game_hu4gu(long sa_game_hu4gu){this.sa_game_hu4gu = sa_game_hu4gu;}</v>
+      </c>
+    </row>
+    <row r="60" spans="14:26">
+      <c r="N60" t="s">
+        <v>139</v>
+      </c>
+      <c r="P60" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_ou4gu = 900001</v>
+      </c>
+      <c r="Q60">
+        <v>900001</v>
+      </c>
+      <c r="S60" t="s">
+        <v>266</v>
+      </c>
+      <c r="T60" t="s">
+        <v>252</v>
+      </c>
+      <c r="W60" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_ou4gu(sa_game_ou4gu);</v>
+      </c>
+      <c r="X60" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_ou4gu;</v>
+      </c>
+      <c r="Y60" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_ou4gu = globalVariables.getSA_game_ou4gu();</v>
+      </c>
+      <c r="Z60" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_ou4gu = 900001; public long getSA_game_ou4gu(){return sa_game_ou4gu;} public void setSA_game_ou4gu(long sa_game_ou4gu){this.sa_game_ou4gu = sa_game_ou4gu;}</v>
+      </c>
+    </row>
+    <row r="61" spans="14:26">
+      <c r="N61" t="s">
+        <v>139</v>
+      </c>
+      <c r="P61" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_firstStrikeBonus = 900010</v>
+      </c>
+      <c r="Q61">
+        <v>900010</v>
+      </c>
+      <c r="S61" t="s">
+        <v>267</v>
+      </c>
+      <c r="T61" t="s">
+        <v>254</v>
+      </c>
+      <c r="W61" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_firstStrikeBonus(sa_game_firstStrikeBonus);</v>
+      </c>
+      <c r="X61" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_firstStrikeBonus;</v>
+      </c>
+      <c r="Y61" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_firstStrikeBonus = globalVariables.getSA_game_firstStrikeBonus();</v>
+      </c>
+      <c r="Z61" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_firstStrikeBonus = 900010; public long getSA_game_firstStrikeBonus(){return sa_game_firstStrikeBonus;} public void setSA_game_firstStrikeBonus(long sa_game_firstStrikeBonus){this.sa_game_firstStrikeBonus = sa_game_firstStrikeBonus;}</v>
+      </c>
+    </row>
+    <row r="62" spans="14:26">
+      <c r="N62" t="s">
+        <v>139</v>
+      </c>
+      <c r="P62" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_lastStrikeBonus = 900010</v>
+      </c>
+      <c r="Q62">
+        <v>900010</v>
+      </c>
+      <c r="S62" t="s">
+        <v>268</v>
+      </c>
+      <c r="T62" t="s">
+        <v>253</v>
+      </c>
+      <c r="W62" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_lastStrikeBonus(sa_game_lastStrikeBonus);</v>
+      </c>
+      <c r="X62" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_lastStrikeBonus;</v>
+      </c>
+      <c r="Y62" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_lastStrikeBonus = globalVariables.getSA_game_lastStrikeBonus();</v>
+      </c>
+      <c r="Z62" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_lastStrikeBonus = 900010; public long getSA_game_lastStrikeBonus(){return sa_game_lastStrikeBonus;} public void setSA_game_lastStrikeBonus(long sa_game_lastStrikeBonus){this.sa_game_lastStrikeBonus = sa_game_lastStrikeBonus;}</v>
+      </c>
+    </row>
+    <row r="63" spans="14:26">
+      <c r="N63" t="s">
+        <v>139</v>
+      </c>
+      <c r="P63" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_firstKillBonus = 900010</v>
+      </c>
+      <c r="Q63">
+        <v>900010</v>
+      </c>
+      <c r="S63" t="s">
+        <v>269</v>
+      </c>
+      <c r="T63" t="s">
+        <v>255</v>
+      </c>
+      <c r="W63" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_firstKillBonus(sa_game_firstKillBonus);</v>
+      </c>
+      <c r="X63" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_firstKillBonus;</v>
+      </c>
+      <c r="Y63" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_firstKillBonus = globalVariables.getSA_game_firstKillBonus();</v>
+      </c>
+      <c r="Z63" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_firstKillBonus = 900010; public long getSA_game_firstKillBonus(){return sa_game_firstKillBonus;} public void setSA_game_firstKillBonus(long sa_game_firstKillBonus){this.sa_game_firstKillBonus = sa_game_firstKillBonus;}</v>
+      </c>
+    </row>
+    <row r="64" spans="14:26">
+      <c r="N64" t="s">
+        <v>139</v>
+      </c>
+      <c r="P64" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_firstStrikeMult = 900010</v>
+      </c>
+      <c r="Q64">
+        <v>900010</v>
+      </c>
+      <c r="S64" t="s">
+        <v>270</v>
+      </c>
+      <c r="T64" t="s">
+        <v>256</v>
+      </c>
+      <c r="W64" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_firstStrikeMult(sa_game_firstStrikeMult);</v>
+      </c>
+      <c r="X64" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_firstStrikeMult;</v>
+      </c>
+      <c r="Y64" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_firstStrikeMult = globalVariables.getSA_game_firstStrikeMult();</v>
+      </c>
+      <c r="Z64" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_firstStrikeMult = 900010; public long getSA_game_firstStrikeMult(){return sa_game_firstStrikeMult;} public void setSA_game_firstStrikeMult(long sa_game_firstStrikeMult){this.sa_game_firstStrikeMult = sa_game_firstStrikeMult;}</v>
+      </c>
+    </row>
+    <row r="65" spans="14:26">
+      <c r="N65" t="s">
+        <v>139</v>
+      </c>
+      <c r="P65" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_kastStrikeMult = 900010</v>
+      </c>
+      <c r="Q65">
+        <v>900010</v>
+      </c>
+      <c r="S65" t="s">
+        <v>271</v>
+      </c>
+      <c r="T65" t="s">
+        <v>257</v>
+      </c>
+      <c r="W65" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_kastStrikeMult(sa_game_kastStrikeMult);</v>
+      </c>
+      <c r="X65" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>long sa_game_kastStrikeMult;</v>
+      </c>
+      <c r="Y65" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_kastStrikeMult = globalVariables.getSA_game_kastStrikeMult();</v>
+      </c>
+      <c r="Z65" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private long sa_game_kastStrikeMult = 900010; public long getSA_game_kastStrikeMult(){return sa_game_kastStrikeMult;} public void setSA_game_kastStrikeMult(long sa_game_kastStrikeMult){this.sa_game_kastStrikeMult = sa_game_kastStrikeMult;}</v>
+      </c>
+    </row>
+    <row r="66" spans="14:26">
+      <c r="N66" t="s">
+        <v>188</v>
+      </c>
+      <c r="P66" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_ReportAttackers = 1</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+      <c r="S66" t="s">
+        <v>272</v>
+      </c>
+      <c r="T66" t="s">
+        <v>258</v>
+      </c>
+      <c r="W66" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_ReportAttackers(sa_game_ReportAttackers);</v>
+      </c>
+      <c r="X66" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>Integer sa_game_ReportAttackers;</v>
+      </c>
+      <c r="Y66" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_ReportAttackers = globalVariables.getSA_game_ReportAttackers();</v>
+      </c>
+      <c r="Z66" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private Integer sa_game_ReportAttackers = 1; public Integer getSA_game_ReportAttackers(){return sa_game_ReportAttackers;} public void setSA_game_ReportAttackers(Integer sa_game_ReportAttackers){this.sa_game_ReportAttackers = sa_game_ReportAttackers;}</v>
+      </c>
+    </row>
+    <row r="67" spans="14:26">
+      <c r="N67" t="s">
+        <v>188</v>
+      </c>
+      <c r="P67" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_ReportMirros = 1</v>
+      </c>
+      <c r="Q67">
+        <v>1</v>
+      </c>
+      <c r="S67" t="s">
+        <v>273</v>
+      </c>
+      <c r="T67" t="s">
+        <v>259</v>
+      </c>
+      <c r="W67" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_ReportMirros(sa_game_ReportMirros);</v>
+      </c>
+      <c r="X67" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>Integer sa_game_ReportMirros;</v>
+      </c>
+      <c r="Y67" s="92" t="str">
+        <f t="shared" si="10"/>
+        <v>sa_game_ReportMirros = globalVariables.getSA_game_ReportMirros();</v>
+      </c>
+      <c r="Z67" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private Integer sa_game_ReportMirros = 1; public Integer getSA_game_ReportMirros(){return sa_game_ReportMirros;} public void setSA_game_ReportMirros(Integer sa_game_ReportMirros){this.sa_game_ReportMirros = sa_game_ReportMirros;}</v>
+      </c>
+    </row>
+    <row r="68" spans="14:26">
+      <c r="N68" t="s">
+        <v>188</v>
+      </c>
+      <c r="P68" t="str">
+        <f t="shared" si="11"/>
+        <v>sa_game_ReportBeneficiaries = 1</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+      <c r="S68" t="s">
+        <v>274</v>
+      </c>
+      <c r="T68" t="s">
+        <v>260</v>
+      </c>
+      <c r="W68" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>globalVariables.setSA_game_ReportBeneficiaries(sa_game_ReportBeneficiaries);</v>
+      </c>
+      <c r="X68" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>Integer sa_game_ReportBeneficiaries;</v>
+      </c>
+      <c r="Y68" s="92" t="str">
+        <f>CONCATENATE(S68," = globalVariables.get",T68,"();")</f>
+        <v>sa_game_ReportBeneficiaries = globalVariables.getSA_game_ReportBeneficiaries();</v>
+      </c>
+      <c r="Z68" s="90" t="str">
+        <f t="shared" si="9"/>
+        <v>private Integer sa_game_ReportBeneficiaries = 1; public Integer getSA_game_ReportBeneficiaries(){return sa_game_ReportBeneficiaries;} public void setSA_game_ReportBeneficiaries(Integer sa_game_ReportBeneficiaries){this.sa_game_ReportBeneficiaries = sa_game_ReportBeneficiaries;}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated plan for SA_game variables.
</commit_message>
<xml_diff>
--- a/ZacPacMan_shelf_comm_plan.xlsx
+++ b/ZacPacMan_shelf_comm_plan.xlsx
@@ -943,9 +943,6 @@
     <t>SA_game_firstStrikeMult</t>
   </si>
   <si>
-    <t>SA_game_kastStrikeMult</t>
-  </si>
-  <si>
     <t>SA_game_ReportAttackers</t>
   </si>
   <si>
@@ -985,9 +982,6 @@
     <t>sa_game_firstStrikeMult</t>
   </si>
   <si>
-    <t>sa_game_kastStrikeMult</t>
-  </si>
-  <si>
     <t>sa_game_ReportAttackers</t>
   </si>
   <si>
@@ -995,6 +989,12 @@
   </si>
   <si>
     <t>sa_game_ReportBeneficiaries</t>
+  </si>
+  <si>
+    <t>sa_game_lastStrikeMult</t>
+  </si>
+  <si>
+    <t>SA_game_lastStrikeMult</t>
   </si>
 </sst>
 </file>
@@ -19554,8 +19554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X7" workbookViewId="0">
-      <selection activeCell="Y68" sqref="Y10:Y68"/>
+    <sheetView tabSelected="1" topLeftCell="I40" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19681,7 +19681,7 @@
         <v>Master</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" ref="R11:R68" si="4">CONCATENATE(Q11,RIGHT(P11,LEN(P11)-LEN(Q11)))</f>
+        <f t="shared" ref="R11:R54" si="4">CONCATENATE(Q11,RIGHT(P11,LEN(P11)-LEN(Q11)))</f>
         <v>Master_enable_value = 1</v>
       </c>
       <c r="S11" t="str">
@@ -19689,7 +19689,7 @@
         <v>master_enable_value</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" ref="T11:T68" si="6">LEFT(R11,FIND(" =",R11)-1)</f>
+        <f t="shared" ref="T11:T54" si="6">LEFT(R11,FIND(" =",R11)-1)</f>
         <v>Master_enable_value</v>
       </c>
       <c r="U11">
@@ -21913,7 +21913,7 @@
         <v>900100</v>
       </c>
       <c r="S55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="T55" t="s">
         <v>247</v>
@@ -21947,7 +21947,7 @@
         <v>900010</v>
       </c>
       <c r="S56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="T56" t="s">
         <v>248</v>
@@ -21981,7 +21981,7 @@
         <v>900100</v>
       </c>
       <c r="S57" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="T57" t="s">
         <v>249</v>
@@ -22015,7 +22015,7 @@
         <v>900010</v>
       </c>
       <c r="S58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T58" t="s">
         <v>250</v>
@@ -22049,7 +22049,7 @@
         <v>900001</v>
       </c>
       <c r="S59" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="T59" t="s">
         <v>251</v>
@@ -22083,7 +22083,7 @@
         <v>900001</v>
       </c>
       <c r="S60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="T60" t="s">
         <v>252</v>
@@ -22117,7 +22117,7 @@
         <v>900010</v>
       </c>
       <c r="S61" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T61" t="s">
         <v>254</v>
@@ -22151,7 +22151,7 @@
         <v>900010</v>
       </c>
       <c r="S62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T62" t="s">
         <v>253</v>
@@ -22185,7 +22185,7 @@
         <v>900010</v>
       </c>
       <c r="S63" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T63" t="s">
         <v>255</v>
@@ -22219,7 +22219,7 @@
         <v>900010</v>
       </c>
       <c r="S64" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="T64" t="s">
         <v>256</v>
@@ -22247,32 +22247,32 @@
       </c>
       <c r="P65" t="str">
         <f t="shared" si="11"/>
-        <v>sa_game_kastStrikeMult = 900010</v>
+        <v>sa_game_lastStrikeMult = 900010</v>
       </c>
       <c r="Q65">
         <v>900010</v>
       </c>
       <c r="S65" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="T65" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="W65" s="18" t="str">
         <f t="shared" si="7"/>
-        <v>globalVariables.setSA_game_kastStrikeMult(sa_game_kastStrikeMult);</v>
+        <v>globalVariables.setSA_game_lastStrikeMult(sa_game_lastStrikeMult);</v>
       </c>
       <c r="X65" s="37" t="str">
         <f t="shared" si="8"/>
-        <v>long sa_game_kastStrikeMult;</v>
+        <v>long sa_game_lastStrikeMult;</v>
       </c>
       <c r="Y65" s="92" t="str">
         <f t="shared" si="10"/>
-        <v>sa_game_kastStrikeMult = globalVariables.getSA_game_kastStrikeMult();</v>
+        <v>sa_game_lastStrikeMult = globalVariables.getSA_game_lastStrikeMult();</v>
       </c>
       <c r="Z65" s="90" t="str">
         <f t="shared" si="9"/>
-        <v>private long sa_game_kastStrikeMult = 900010; public long getSA_game_kastStrikeMult(){return sa_game_kastStrikeMult;} public void setSA_game_kastStrikeMult(long sa_game_kastStrikeMult){this.sa_game_kastStrikeMult = sa_game_kastStrikeMult;}</v>
+        <v>private long sa_game_lastStrikeMult = 900010; public long getSA_game_lastStrikeMult(){return sa_game_lastStrikeMult;} public void setSA_game_lastStrikeMult(long sa_game_lastStrikeMult){this.sa_game_lastStrikeMult = sa_game_lastStrikeMult;}</v>
       </c>
     </row>
     <row r="66" spans="14:26">
@@ -22287,10 +22287,10 @@
         <v>1</v>
       </c>
       <c r="S66" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W66" s="18" t="str">
         <f t="shared" si="7"/>
@@ -22321,10 +22321,10 @@
         <v>1</v>
       </c>
       <c r="S67" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="T67" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="W67" s="18" t="str">
         <f t="shared" si="7"/>
@@ -22355,10 +22355,10 @@
         <v>1</v>
       </c>
       <c r="S68" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="T68" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W68" s="18" t="str">
         <f t="shared" si="7"/>

</xml_diff>